<commit_message>
wrote test to check positive environemntal impact link is on mainpage
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/16_positive_environmental_impact/Vorlage_Datenmodel_environmentalImpact_08204.xlsx
+++ b/02_work_doc/01_daten/16_positive_environmental_impact/Vorlage_Datenmodel_environmentalImpact_08204.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -136,10 +136,10 @@
     <t xml:space="preserve">Positive Wirkung</t>
   </si>
   <si>
-    <t xml:space="preserve">Hier steht ein Platzhaltertext: Con rest voles molor se reptur, erum sum autaquiae prae nonsequat quas ex exero dolupti dolupta tempossimi, volestiures es doluptatur santius ulparciis et ad eum aceptiistion cum quianihictem unt rest voles molor se reptur, erum sum autaquiae prae nonsequat quas ex exero dolupti dolupta tempossimi, volestiures es doluptatur santius ulparciis et ad eum aceptiistion cum quianihictem unt ut pel ma dolorpo rruntur, accat. Ent, que nimi, quas si odi optatis ex estisque ommossi tatur, vendit por sum ellecatur repudanda simusae et enis ne nus. Ent, que nimi, quas si odi optatis ex estisque ommossi tatur, vendit por sum ellecatur repudanda simusae et enis ne nus. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name Digitale Anwendung</t>
+    <t xml:space="preserve">Das Projekt RLT-Opt adressiert das Problem ineffizienter raumlufttechnischer Anlagen (RLT-Anlagen) in deutschen Nichtwohngebäuden. Der Projektverbund schätzt, dass die ca. 400.000 Teilklima- und 600.000 mittleren bzw. großen Lüftungsanlagen im Gebäudebestand etwa 40 TWh/a Strom verbrauchen, was ca. 8 % des deutschen Gesamtverbrauchs ausmacht (Stand: 2022).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RLT-Opt</t>
   </si>
   <si>
     <t xml:space="preserve">RLT-Opt – Lüftungs- und Klimaanlagen ganzheitlich optimieren </t>
@@ -175,7 +175,7 @@
     <t xml:space="preserve">Hohe positive Umweltwirkungen (Energieeinsparungen)</t>
   </si>
   <si>
-    <t xml:space="preserve">Bild1_RLT-Opt</t>
+    <t xml:space="preserve">img/componentList/environment-positive.svg</t>
   </si>
   <si>
     <t xml:space="preserve">Das Projekt RLT-Opt adressiert das Problem ineffizienter raumlufttechnischer Anlagen (RLT-Anlagen) in deutschen Nichtwohngebäuden. Der Projektverbund schätzt, dass die ca. 400.000 Teilklima- und 600.000 mittleren bzw. großen Lüftungsanlagen im Gebäudebestand etwa 40 TWh/a Strom verbrauchen, was ca. 8 % des deutschen Gesamtverbrauchs ausmacht (Stand: 2022). Trotzdem ist die Anzahl an Anlagen, bei denen energetische Inspektionen durchgeführt wurden, gering (etwa 25.000 Anlagen). Bei diesen Anlagen werden häufig hohe Energieeinsparpotenziale durch die Optimierung der Wärme-, Kälte-, und Stromverbräuche identifiziert. 
@@ -198,7 +198,10 @@
     <t xml:space="preserve">RLT-Opt– Lüftungs- und Klimaanlagen ganzheitlich optimieren</t>
   </si>
   <si>
-    <t xml:space="preserve">ein Platzhaltertext: Con rest voles molor se reptur, erum sum autaquiae prae nonsequat quas ex exero dolupti dolupta tempossimi, volestiures es doluptatur santius ulparciis et ad eum aceptiistion cum quianihictem unt rest voles molor se reptur, erum sum autaquiae prae nonsequat quas ex exero dolupti dolupta tempossimi, volestiures es doluptatur santius ulparciis et ad eum aceptiistion cum quianihictem unt ut pel ma dolorpo rruntur, accat. Ent, que nimi, quas si odi optatis ex estisque ommossi tatur, vendit por sum ellecatur repudanda simusae et enis ne nus. Ent, que nimi, quas si odi optatis ex estisque ommossi tatur, vendit por sum ellecatur repudanda simusae et enis ne nus. </t>
+    <t xml:space="preserve">Der Fokus des Projekts liegt insbesondere auf der Energieeffizienzsteigerung von Heizungs-, Kühlungs- und Klimasysteme in Bürogebäuden unter Berücksichtigung der Zufriedenheit der Nutzenden. Zum Einsatz kommt dabei eine Modell-prädikative Regelung (engl. Model Predicitve Control (MPC)), die es ermöglicht, nicht-lineares Systemverhalten vorauszusagen und automatisiert zu steuern. Verschiedene Studien beziffern die Energieeinsparungen zwischen 15 % und 50 % (Mork et al. 2023).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLEC</t>
   </si>
   <si>
     <t xml:space="preserve">LLEC – Verwaltungsbau: Klimaneutraler Verwaltungsbau als aktiver Teil des Living Lab Energy Campus;
@@ -231,7 +234,7 @@
     <t xml:space="preserve">Verbrauchsreduktion in komplexe Gebäudestrukturen u.a. durch die Nutzenden</t>
   </si>
   <si>
-    <t xml:space="preserve">llec_logo_large_transparent</t>
+    <t xml:space="preserve">assets/images/llec_logo_large_transparent.png</t>
   </si>
   <si>
     <t xml:space="preserve">Die Heterogenität von Gebäuden, die beispielsweise durch unterschiedliche Anlagenparks und/oder Nutzungsprofile entsteht, sowie das Verhalten der Nutzenden von Gebäuden stellen komplexe Herausforderungen zur Minimierung des Energieverbrauchs dar. Oftmals fehlen verlässliche Daten und entsprechende digitale Anwendungen, um den Energieverbrauch und die Effizienz von Gebäuden angemessen zu bewerten und zu optimieren. Durch ihren erheblichen Anteil am Gesamtenergieverbrauch (30 %) steht die Verbesserung der Energieeffizienz und Reduzierung von CO2-Emissionen von Gebäuden zunehmend im Fokus derzeitiger Forschung (United Nations Environment Programme 2021).
@@ -248,6 +251,78 @@
 Für die Nutzendeneinbindung ist zu erwähnen, dass unterschiedlichen Maßnahmen (Dashboards, JuControl, JuPower) seit 2020 durch mehr als 1300 Mitarbeitende genutzt wurden. Zur Evaluierung der Effektivität der Nutzendeneinbindung wurde basierend auf den historischen Daten vor Implementierung der Maßnahmen ein Regressionsmodell aufgesetzt, was den entstandenen Heizenergiebedarf maßgeblich als Funktion der Außentemperatur beschreibt (Fitgüte: R2 = 0,91). Dieses Modell wurde dann ebenso auf die Periode mit implementierten Maßnahmen zur Nutzendeneinbindung angewandt und mit dem tatsächlichen Energieverbrauch des Gebäudes verglichen. Es konnte gezeigt werden, dass, verglichen mit der Referenzperiode, der Heizbedarf in Abhängigkeit der Außentemperatur weniger stark anstieg und die durchschnittliche Temperatur des Pilotgebäudes durchschnittlich um 1 °C gesenkt werden konnte. Diese Effekte trugen maßgeblich zu der gemessenen Verbrauchsreduktion von 11.1 MWh pro Jahr (- 16,7 %) bei, welche die Verantwortlichen auf Grund der gleichen Systemparameter (Energetischer Zustand des Gebäudes und des Heizsystems) auf die effizientere Nutzung des Heizsystems und ein effizienteres Nutzendenverhalten zurückführen. Bei einem Gaskraftwerk zur Heizwärmebereitstellung (angenommener Emissionsfaktor von 200 g CO2e/kWhprimär; Primärenergiefaktor Erdgas = 1,1) entspricht dies einer Einsparung von ca. 2,44 t CO2e pro Jahr. Für Unterschiede in der Außentemperatur der beiden Perioden wurde dabei korrigiert, andere Einflussgrößen wurden jedoch nicht betrachtet (z.B. Wind, Solare Gewinne). Das Komfortlevel der Menschen wurde dabei nicht negativ beeinflusst. Dabei weisen die Projektverantwortlichen auf das zusätzliche Potential hin, da nur ein Fünftel der Büros in dem Gebäude für die Maßnahmen zur Nutzendeneinbindung aktiviert waren. 
 Die negativen Umweltwirkungen der verbauten Komponenten wurden weder für die MPC noch die Nutzendeneinbindung bilanziert. Bei der am LLEC vorzufindenden (Komponenten-)Infrastruktur besteht die Schwierigkeit zur Bewertung der negativen Wirkungen vor allem in der Allokation der Komponenten, da neben den hier beschriebenen digitalen Anwendungen noch viele weitere Prozesse und Anwendungen die gleichen Komponenten nutzen. Daher ist eine genaue Zuordnung zu einzelnen digitalen Anwendungen schwierig. Jedoch mussten für die Einzelraummessungen eine Vielzahl an batteriebetriebenen Komponenten verbaut werden (&gt; 1800 Komponenten auf dem Campus insgesamt). Da all diese Komponenten fortwährend mit den digitalen Anwendungen Daten austauschen bzw. diese auf diese zurückgreifen, fällt ein entsprechend hoher Datenaufwand an. Alleine für die Maßnahmen zur Nutzendeneinbindung wurden in ca. 3 Jahren 364 Mio. Datensätzen erfasst und aufgearbeitet (ca. 74 GB insgesamt bzw. ca. 25 GB/a). Dabei gehen die Forschenden davon aus, dass sich der Datenaufwand bei einer noch praxisnäheren Implementierung um ca. 25% reduzieren lassen könnte. Zum einen, da die Anzahl an Datenpunkten in etwa um diese Größe reduziert werden könnte. Zum anderen, weil nach erfolgreicher Erprobung im Forschungskontext weniger Redundanzen bei den Messstellen und eine geringerer Datengranularität nötig wären.  Für die MPC werden täglich ca. 300 MB an Daten auf einem OpenStack Server verarbeitet. Nur ein Bruchteil entfällt dabei auf die Erfassung der Messdaten aus den Räumen (ca. 5 MB pro Tag; 15 minütige Daten zu Raum-Temperatur, Zustände von Fenster- und Tür-Kontakten und Anzahl an Personen im Raum). Zusammengenommen fragen die Nutzendeneinbindung und die MPC jährlich virtuelle Ressourcen für ca. 124 GB nach, was überschlägig CO2-Emissionen von ca. 339 kg CO2e bedeuten würde (vergleiche Abschätzung der negativen Wirkungen durch die Datenübertragung und -verarbeitung hier ).  
 Schließlich sieht das Projekt verschiedene Anknüpfungsmöglichkeiten für künftige Forschungsvorhaben. Da MPC-Modelle zwar hohe Einsparpotenziale versprechen, jedoch gleichzeitig einen hohen Aufwand für individuelle Kalibrierung benötigen, besteht ein hoher Bedarf für die Entwicklung von einfach übertragbaren MPC-Ansätzen für kommerzielle Zwecke. Auf die vereinfachte Übertragung auf andere Gebäude zielt auch die angestrebte Verknüpfung beider Anwendungen des Projekts ab (MPC &amp; Nutzendeneinbindung). So sind noch effizienzsteigernde Anpassungsmöglichkeiten innerhalb der Kostenfunktion des MPC möglich. Da beide Aspekte modular entwickelt wurden, ist eine zukünftige Verschränkung denkbar und sinnvoll um bspw. die Effektivität der MPC unter Einfluss von benutzerdefinierte Komforteinstellungen oder angepassten Handlungsempfehlungen an die Nutzenden zu testen. Zudem nennen die Forschenden den Bedarf für umfassendere Versuche in größeren Gebäuden unter Einbeziehung ganzzahliger Entscheidungsvariablen, sowie der Vorlauftemperaturen von Heizwasservolumenströmen (zentrale Heizungssysteme) als weitere Entwicklungsfelder. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Althaus, Philipp, Florian Redder, Eziama Ubachukwu, Maximilian Mork, André Xhonneux und Dirk Müller (2022): Enhancing Building Monitoring and Control for District Energy Systems: Technology Selection and Installation within the Living Lab Energy Campus. Applied Sciences 12, Nr. 7 (Januar): 3305.;;
+Mork, Maximilian, Florian Redder, André Xhonneux und Dirk Müller (2023): Real-world implementation and evaluation of a Model Predictive Control framework in an office space. Journal of Building Engineering 78 (1. November): 107619.;;
+Ubachukwu, Eziama, Jana Pick, Lea Riebesel, Paul Lieberenz, Philipp Althaus, Dirk Müller und André Xhonneux (2023): LLEC Energy Dashboard Suite: User Engagement for Energy-Efficient Behavior Using Dashboards and Gamification. In: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), S. 3241–3252. Veranstaltung: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), Las Palmas De Gran Canaria, Spain. http://www.proceedings.com/069564-0291.html.
+United Nations Environment Programme (2021): 2021 Global Status Report for Buildings and Construction: Towards a Zero-Emission, Efficient and Resilient Buildings and Construction Sector. Nairobi, Kenya: United Nations Environment Programme.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wohnungsunternehmen betreiben meist unterschiedliche Gebäude mit einer Vielfalt von Technologien für die Heiz- und Warmwasserversorgung. Das Potenzial zur Betriebsoptimierung dieser Heizzentralen in Mehrfamilienhäusern ist enorm. Dies sollte möglichst bedienerfreundlich und idealerweise automatisiert erfolgen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FeBOp-MFH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FeBOp-MFH – Feldanalyse zur Betriebsoptimierung von Mehrfamilienhäusern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03ET1573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/2018 – 07/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institut für Solarenergieforschung Hameln, Klimaschutz- und Energieagentur Niedersachsen GmbH, proKlima – der enercity-Fonds, Corona SOLAR GmbH; acht niedersächsische Kooperationspartner aus der Wohnungswirtschaft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.klimaschutz-niedersachsen.de/themen/waerme/FeBop.php </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betriebsoptimierung, Dashboard/Plattform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verbrauchsminimierung, Steigerung der Materialeffizienz, Effizienzsteigerung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informations- und Wissensvermittlung, Nudging, Austausch von Komponenten/Geräten, Umsetzung Messkonzepte/Monitoring, Automatisierung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geringe Umweltlasen bei gleichzeitig hoher Verbreitungschance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assets/images/FeBOp_year_comparison.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wohnungsunternehmen betreiben meist unterschiedliche Gebäude mit einer Vielfalt von Technologien für die Heiz- und Warmwasserversorgung. Das Potenzial zur Betriebsoptimierung dieser Heizzentralen in Mehrfamilienhäusern ist enorm. Dies sollte möglichst bedienerfreundlich und idealerweise automatisiert erfolgen. 
+Das Forschungsprojekt FeBOp-MFH zielt darauf ab, mit minimalem zusätzlichem Messaufwand, Daten der Heizzentralen mithilfe eines intelligenten Mess- und Analysesystems zu erfassen und zu analysieren. Dadurch sollen automatisierte Effizienzanalysen ermöglicht und der Betrieb jeder Heizzentrale optimiert werden. Der primäre Fokus des Projekts liegt auf der Erzielung von Energie- und CO2-Einsparungen sowie auf der Komfortsteigerung aus Sicht des Anlagenbetreibers (vereinfachte Betriebsführung). Sekundäre Ziele sind Kosteneinsparungen sowie die Verlängerung der Lebensdauer der Heiztechnik. Die erwarteten Energieeinsparungen liegen bei mindestens 10 %.
+Der Anwendungsbereich des Projekts erstreckt sich auf die Wärmeoptimierung im Betrieb von Mehrfamilienhäusern, die von Wohnungsunternehmen betrieben werden. Strategisch setzt das Projekt auf Monitoring, Informations- und Wissensvermittlung sowie Handlungsempfehlungen. Diese Maßnahmen richten sich hauptsächlich an die Anlagenbetreiber und nicht an die Mietenden. Es kommen zum einen die Betriebsoptimierung sowie die dafür notwendige Aufbereitung mittels Dashboards bzw. einer digitalen Plattform zum Einsatz. Hierzu werden Kennwerte wie der Nutzungsgrad unter anderem mit „adaptiven“ Benchmarks verglichen. Diese adaptiven Benchmarks nach VDI 3807-1 beziehen sich nicht nur auf das individuelle Gebäude, sondern sind besonders für das gesamte Gebäudeportfolio von Interesse. Hierbei wird der Mittelwert der besten 25 % der Gebäude mit vergleichbarer Technik und Nutzung als Benchmark verwendet. Wohnungsbauunternehmen können so die Gebäude bzw. Anlagen mit dem Benchmark vergleichen und größte Bedarfe und Potenziale für ihr eigenes Portfolio identifizieren. Diese adaptive Herangehensweise mit praktisch erreichten und somit realistischen Kennwerten ermöglicht eine kontinuierliche Anpassung der Benchmarks je nach Zeitraum und durchgeführten Modernisierungsmaßnahmen. Dadurch entsteht nicht nur eine interne Vergleichbarkeit, sondern auch die mit anderen Unternehmen und Objekten, was zu gezielten Handlungen anregen kann.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In dem Projekt FeBOp-MFH wurden gezielt die Potenziale zur Effizienzsteigerung von Heizzentralen angegangen. Die zentrale Stellschraube lag in der Effizienzanalyse des bestehenden Systems, um darauf basierend Verbesserungsmöglichkeiten zu identifizieren. Frühzeitiges Erkennen eines ineffizienten oder fehlerhaften Betriebs ermöglichte die Identifikation von geringinvestiv nutzbaren Einsparpotenzialen und den einfachen Nachweis erzielter Energie- und CO2-Einsparungen. Neben den Echtzeitdaten der Anlagen, können die Betreiber aus Monats- und Jahresberichten Ansatzpunkte für Optimierungsoptionen ableiten. Dazu werden wichtige Kennzahlen wie die Auslastung, Betriebszeiten, Temperaturverläufe, Verluste und der Nutzungsgrad der Heizzentrale dargestellt. Die im Projekt identifizierten Stellschrauben zum Heben der Effizienzpotenziale umfassten die Anpassung von Betriebszeiten und Temperaturen, das Minimieren von Zirkulationszeiten und – für einen möglichen Kessel/Heizungstausch – Hilfestellungen für eine bedarfsgerechte Dimensionierung der Heizung, was den zukünftigen Materialeinsatz minimiert und Überdimensionierungen vermeidet. In den bisherigen Untersuchungen wurde zudem die zentrale Trinkwarmwassererzeugung als häufig ineffizient identifiziert, was den Einsatz dezentraler Systeme zur Warmwasserbereitung (z.B. Wohnungsstationen) zu einer weiteren relevanten Stellschraube macht (ebenfalls im Falle möglicher Modernisierungsmaßnahmen durch die Wohnungsunternehmen). 
+Um diese Stellschrauben zu identifizieren, werden zusätzliche Messwerte benötigt. Dazu müssen jedoch nur sehr wenige Zähler, sowie Temperatur- und Volumenstromsensoren verbaut und mit einem extra Datenlogger kommunikativ über Funk oder Kabel verbunden werden. Die minütlichen Daten werden dann auf dem Datenlogger zwischengespeichert, verschlüsselt und an einen Server versendet. Dort findet wiederum die eigentliche, automatisierte Messwertaufbereitung und -auswertung statt. Die Anlagenbetreiber*innen können die Daten sodann in Echtzeit oder aggregiert vom Server abrufen.  
+Methodisch erfolgte die Messwertaufbereitung anhand einer Vergleichsbildung durch adaptive Benchmarks. Dadurch wird die Performance der Anlage schnell mit vergleichbaren Objekten bewertbar. Die detaillierte Aufarbeitung der eigentlichen Betriebsparameter der Heizzentrale erfolgt dann entweder individuell in Echtzeit oder in automatisierter Form der Monats- oder Jahresberichte. Die Berichte sind dabei unter anderem für den monatlichen/jährlichen Vergleich der Performance der Heizzentrale ausgelegt. Für einige Optimierungsstellschrauben werden auch automatisierte Handlungsempfehlungen gegeben. So werden die Anlagenbetreiber*innen beispielsweise darauf hingewiesen, wenn mögliche Ruhezeiten der Trinkwarmwasserzirkulation nicht ausgeschöpft werden oder die Betriebstemperaturen zu hoch sind.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das Analysesystem des Projekts ermöglicht die Evaluierung der ermittelten Kennwerte anhand von drei Referenzszenarien (Benchmarks). Im ersten Szenario wird ein fester Referenzwert als Benchmark gesetzt, der beispielsweise für den Heizkessel nach VDI 3807-5 bestimmt werden kann. Im zweiten Szenario erfolgt der Vergleich anhand von Kennwerten aus den Vorjahren (historische Daten). Dies ist allerdings erst dann sinnvoll, wenn Betriebsdaten aus mindestens zwei Jahren vorliegen und zeitliche Trends identifiziert werden sollen. Im letzten Szenario werden Kennwerte mit den entsprechenden Kennwerten aller anderen Anlagen verglichen. Diese Werte müssen alle auf der gleichen Basis berechnet worden sein. Die Benchmark ist erst dann aussagekräftig, wenn eine größere Anzahl von Anlagen über mindestens ein Jahr untersucht wurden. 
+Im Projekt werden folgende vier Kennwerte genutzt, um einen Überblick über relevanten Qualitäten der Wärmezentralen zu geben. Die Effizienz des Wärmeerzeugers ist von zentraler Bedeutung, da diese Komponente die zugeführte Endenergie in nutzbare Wärme wandelt. Die Wärmeerzeuger werden nach den verschiedenen Endenergieträgern Gas, Öl Holz und Strom unterschieden, nicht jedoch nach Baujahr oder Bauart. Die Effizienz der Komponente wird durch den Jahresnutzungsgrad (Jahresarbeitszahl bei Wärmepumpen) charakterisiert. Er ist definiert als Verhältnis der im Jahr zur Nutzung erzeugten Wärme zu der dem Wärmeerzeuger zugefügten Endenergie ohne erneuerbare Energien. Der nächste untersuchte Kennwert ist die Effizienz der zentralen Trinkwarmwasserversorgung. Sie gibt Aufschluss über Zirkulationsverluste und Verluste der Speicherung und Beladeleitung und ist häufig der Nutzungspfad mit der geringsten Effizienz. Die Effizienz wird über den Nutzungsgrad dargestellt und berechnet sich aus der Wärmeenergie, die im verbrauchten Trinkwarmwasser enthalten ist, dividiert durch die dem Trinkwarmwasserbereiter zugeführte Wärmemenge. Auch der Anteil lokaler erneuerbarer Energien wird betrachtet. Dieser Kennwert stellt dar, wie weit das Gebäude und die Wärmezentrale durch autarke erneuerbare Energie betrieben wird. Er wird aus dem Verhältnis der am und um das Gebäude lokal bereitgestellten erneuerbaren Energien zur Summe aller zugeführten Energien berechnet. Zuletzt werden die spezifischen CO2-Emissionen untersucht. Dieser Kennwert gibt an, welche Gesamtmenge an CO2-Emissionen durch den Wärmeverbrauch des Gebäudes erzeugt werden. Die Kennwerte „Wärmeerzeuger“ und „Trinkwarmwasserversorgung“ reflektieren die Effizienz der Anlagenteile, während die Kennwerte „lokal erzeugte erneuerbare Energien“ und „CO2-Emissionen“ die Zukunftsfähigkeit der Anlage beurteilen. 
+Im einem Beispielobjekt des Projektes ist ein Optimierungspotential für die Effizienz des Kesselnutzungsgrades von 8 % zu erkennen, für Trinkwarmwasserversorgung wird ein Optimierungspotential von 9 % berechnet, allerdings liegt der Zielwert auf einem geringeren Niveau. Ein Anzeichen dafür, dass eine zentrale Trinkwarmwasserbereitung im Allgemeinen keine gute Effizienz aufweist, da signifikante Verteilverluste nicht vermieden werden können. Der Deutsche Verein des Gas- und Wasserfaches gibt an, dass die höchsten Effizienzen und Endenergieeinsparungen hygienisch sicher nur durch eine dezentrale Trinkwarmwasserversorgung erreicht werden können. Für den Anteil erneuerbarer Energie liegt der Zielwert dreimal so hoch wie der Messwert, was einem Potential von 300 % entspricht. Auch hier liegt der Zielwert auf einem niedrigen Niveau, da die lokale Nutzung regenerativer Energien im MFH-Bereich (Umweltwärme, Solarenergie) noch nicht stark verbreitet ist. Im Gegensatz zum gegrenzten Nutzungsgrad der zentralen Trinkwarmwasserversorgung wird der Zielwert bzw. das Potential beim Anteil der regenerativen Energien durch entsprechende Modernisierungen immer weiter Richtung 100% bewegen. Der Kennwert für die CO2-Emissionen liegt am Objekt recht nah am Zielwert, was unter Berücksichtigung des geringen Anteils lokal erzeugter regenerativer Energien auf eine Ausführung der Gebäudedämmung nach mindestens aktuellem Stand der Technik hinweist. 
+Für die Gaskessel im Gesamtbestand mit einem Mittelwert aller Anlagen von 80 % Jahresnutzungsgrad und von den besten Anlagen mit 90 % Jahresnutzungsgrad ergibt sich eine Abweichung von 10 %. Dies stellt auch das mittlere Optimierungspotential dar. Für die zentrale Trinkwarmwasserversorgung werden ebenso Einsparpotentiale berechnet. So zeigte sich an einem Beispielgebäude, dass höhere Trinkwarmwassertemperaturen und eine deutlich geringere Auslastung im Sommer zur Senkung des Nutzungsgrades der Heizzentrale um 10 %-Punkte führen können. Damit einher geht ein gesteigerter Endenergiebedarf von mindestens 10 %.
+Diesen, mit wenigen Mitteln erreichten, Einsparungen bzw. den ggf. durch die Erschließung der aufgezeigten Potenziale noch darüber hinaus möglichen Verbesserungen, stehen nur geringe ökologische Wirkungen gegenüber. Den CO2-Fußabdruck für die Komponenten eines Wärmepumpensystems (1 Wassserzähler, 2 Wärmezähler, 8 kabellose Temperatursensoren, 1 Datenlogger, 1 Smart-Meter) schätzt das Projekt mittels der Hilfestellung  zu den Umweltwirkungen häufig verwendeter Komponenten auf ca. 103,3 kg CO2eq/Jahr. Auch der Datenaufwand ist mit ca. 0,3 GB/Jahr gering. Über die Kennwerte  zu den Umweltlasten der Datenübertragung- und verarbeitung können die CO2-Emissionen auf ca. 0,8 kg CO2eq/Jahr geschätzt werden (Datenübertragung mit VDSL; Serverstandort Deutschland; Use-Case virtuelle Maschine). Bei einem Emissionsfaktor von ca. 0,5 kg CO2eq/kWh  müssten also nur ca. 208 kWh/a Strom eingespart werden, um die Umweltlasten ausgleichen zu können.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive impact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name Digitale Anwendung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bild1_RLT-Opt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">llec_logo_large_transparent</t>
   </si>
   <si>
     <t xml:space="preserve">Althaus, Philipp, Florian Redder, Eziama Ubachukwu, Maximilian Mork, André Xhonneux und Dirk Müller (2022): Enhancing Building Monitoring and Control for District Energy Systems: Technology Selection and Installation within the Living Lab Energy Campus. Applied Sciences 12, Nr. 7 (Januar): 3305.
@@ -257,57 +332,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Platzhaltertext: Con rest voles molor se reptur, erum sum autaquiae prae nonsequat quas ex exero dolupti dolupta tempossimi, volestiures es doluptatur santius ulparciis et ad eum aceptiistion cum quianihictem unt rest voles molor se reptur, erum sum autaquiae prae nonsequat quas ex exero dolupti dolupta tempossimi, volestiures es doluptatur santius ulparciis et ad eum aceptiistion cum quianihictem unt ut pel ma dolorpo rruntur, accat. Ent, que nimi, quas si odi optatis ex estisque ommossi tatur, vendit por sum ellecatur repudanda simusae et enis ne nus. Ent, que nimi, quas si odi optatis ex estisque ommossi tatur, vendit por sum ellecatur repudanda simusae et enis ne nus. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FeBOp-MFH – Feldanalyse zur Betriebsoptimierung von Mehrfamilienhäusern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03ET1573</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/2018 – 07/2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Institut für Solarenergieforschung Hameln, Klimaschutz- und Energieagentur Niedersachsen GmbH, proKlima – der enercity-Fonds, Corona SOLAR GmbH; acht niedersächsische Kooperationspartner aus der Wohnungswirtschaft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.klimaschutz-niedersachsen.de/themen/waerme/FeBop.php </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Betriebsoptimierung, Dashboard/Plattform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verbrauchsminimierung, Steigerung der Materialeffizienz, Effizienzsteigerung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Informations- und Wissensvermittlung, Nudging, Austausch von Komponenten/Geräten, Umsetzung Messkonzepte/Monitoring, Automatisierung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geringe Umweltlasen bei gleichzeitig hoher Verbreitungschance</t>
-  </si>
-  <si>
     <t xml:space="preserve">FeBOp_Jahresvgl_groß</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wohnungsunternehmen betreiben meist unterschiedliche Gebäude mit einer Vielfalt von Technologien für die Heiz- und Warmwasserversorgung. Das Potenzial zur Betriebsoptimierung dieser Heizzentralen in Mehrfamilienhäusern ist enorm. Dies sollte möglichst bedienerfreundlich und idealerweise automatisiert erfolgen. 
-Das Forschungsprojekt FeBOp-MFH zielt darauf ab, mit minimalem zusätzlichem Messaufwand, Daten der Heizzentralen mithilfe eines intelligenten Mess- und Analysesystems zu erfassen und zu analysieren. Dadurch sollen automatisierte Effizienzanalysen ermöglicht und der Betrieb jeder Heizzentrale optimiert werden. Der primäre Fokus des Projekts liegt auf der Erzielung von Energie- und CO2-Einsparungen sowie auf der Komfortsteigerung aus Sicht des Anlagenbetreibers (vereinfachte Betriebsführung). Sekundäre Ziele sind Kosteneinsparungen sowie die Verlängerung der Lebensdauer der Heiztechnik. Die erwarteten Energieeinsparungen liegen bei mindestens 10 %.
-Der Anwendungsbereich des Projekts erstreckt sich auf die Wärmeoptimierung im Betrieb von Mehrfamilienhäusern, die von Wohnungsunternehmen betrieben werden. Strategisch setzt das Projekt auf Monitoring, Informations- und Wissensvermittlung sowie Handlungsempfehlungen. Diese Maßnahmen richten sich hauptsächlich an die Anlagenbetreiber und nicht an die Mietenden. Es kommen zum einen die Betriebsoptimierung sowie die dafür notwendige Aufbereitung mittels Dashboards bzw. einer digitalen Plattform zum Einsatz. Hierzu werden Kennwerte wie der Nutzungsgrad unter anderem mit „adaptiven“ Benchmarks verglichen. Diese adaptiven Benchmarks nach VDI 3807-1 beziehen sich nicht nur auf das individuelle Gebäude, sondern sind besonders für das gesamte Gebäudeportfolio von Interesse. Hierbei wird der Mittelwert der besten 25 % der Gebäude mit vergleichbarer Technik und Nutzung als Benchmark verwendet. Wohnungsbauunternehmen können so die Gebäude bzw. Anlagen mit dem Benchmark vergleichen und größte Bedarfe und Potenziale für ihr eigenes Portfolio identifizieren. Diese adaptive Herangehensweise mit praktisch erreichten und somit realistischen Kennwerten ermöglicht eine kontinuierliche Anpassung der Benchmarks je nach Zeitraum und durchgeführten Modernisierungsmaßnahmen. Dadurch entsteht nicht nur eine interne Vergleichbarkeit, sondern auch die mit anderen Unternehmen und Objekten, was zu gezielten Handlungen anregen kann.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In dem Projekt FeBOp-MFH wurden gezielt die Potenziale zur Effizienzsteigerung von Heizzentralen angegangen. Die zentrale Stellschraube lag in der Effizienzanalyse des bestehenden Systems, um darauf basierend Verbesserungsmöglichkeiten zu identifizieren. Frühzeitiges Erkennen eines ineffizienten oder fehlerhaften Betriebs ermöglichte die Identifikation von geringinvestiv nutzbaren Einsparpotenzialen und den einfachen Nachweis erzielter Energie- und CO2-Einsparungen. Neben den Echtzeitdaten der Anlagen, können die Betreiber aus Monats- und Jahresberichten Ansatzpunkte für Optimierungsoptionen ableiten. Dazu werden wichtige Kennzahlen wie die Auslastung, Betriebszeiten, Temperaturverläufe, Verluste und der Nutzungsgrad der Heizzentrale dargestellt. Die im Projekt identifizierten Stellschrauben zum Heben der Effizienzpotenziale umfassten die Anpassung von Betriebszeiten und Temperaturen, das Minimieren von Zirkulationszeiten und – für einen möglichen Kessel/Heizungstausch – Hilfestellungen für eine bedarfsgerechte Dimensionierung der Heizung, was den zukünftigen Materialeinsatz minimiert und Überdimensionierungen vermeidet. In den bisherigen Untersuchungen wurde zudem die zentrale Trinkwarmwassererzeugung als häufig ineffizient identifiziert, was den Einsatz dezentraler Systeme zur Warmwasserbereitung (z.B. Wohnungsstationen) zu einer weiteren relevanten Stellschraube macht (ebenfalls im Falle möglicher Modernisierungsmaßnahmen durch die Wohnungsunternehmen). 
-Um diese Stellschrauben zu identifizieren, werden zusätzliche Messwerte benötigt. Dazu müssen jedoch nur sehr wenige Zähler, sowie Temperatur- und Volumenstromsensoren verbaut und mit einem extra Datenlogger kommunikativ über Funk oder Kabel verbunden werden. Die minütlichen Daten werden dann auf dem Datenlogger zwischengespeichert, verschlüsselt und an einen Server versendet. Dort findet wiederum die eigentliche, automatisierte Messwertaufbereitung und -auswertung statt. Die Anlagenbetreiber*innen können die Daten sodann in Echtzeit oder aggregiert vom Server abrufen.  
-Methodisch erfolgte die Messwertaufbereitung anhand einer Vergleichsbildung durch adaptive Benchmarks. Dadurch wird die Performance der Anlage schnell mit vergleichbaren Objekten bewertbar. Die detaillierte Aufarbeitung der eigentlichen Betriebsparameter der Heizzentrale erfolgt dann entweder individuell in Echtzeit oder in automatisierter Form der Monats- oder Jahresberichte. Die Berichte sind dabei unter anderem für den monatlichen/jährlichen Vergleich der Performance der Heizzentrale ausgelegt. Für einige Optimierungsstellschrauben werden auch automatisierte Handlungsempfehlungen gegeben. So werden die Anlagenbetreiber*innen beispielsweise darauf hingewiesen, wenn mögliche Ruhezeiten der Trinkwarmwasserzirkulation nicht ausgeschöpft werden oder die Betriebstemperaturen zu hoch sind.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Das Analysesystem des Projekts ermöglicht die Evaluierung der ermittelten Kennwerte anhand von drei Referenzszenarien (Benchmarks). Im ersten Szenario wird ein fester Referenzwert als Benchmark gesetzt, der beispielsweise für den Heizkessel nach VDI 3807-5 bestimmt werden kann. Im zweiten Szenario erfolgt der Vergleich anhand von Kennwerten aus den Vorjahren (historische Daten). Dies ist allerdings erst dann sinnvoll, wenn Betriebsdaten aus mindestens zwei Jahren vorliegen und zeitliche Trends identifiziert werden sollen. Im letzten Szenario werden Kennwerte mit den entsprechenden Kennwerten aller anderen Anlagen verglichen. Diese Werte müssen alle auf der gleichen Basis berechnet worden sein. Die Benchmark ist erst dann aussagekräftig, wenn eine größere Anzahl von Anlagen über mindestens ein Jahr untersucht wurden. 
-Im Projekt werden folgende vier Kennwerte genutzt, um einen Überblick über relevanten Qualitäten der Wärmezentralen zu geben. Die Effizienz des Wärmeerzeugers ist von zentraler Bedeutung, da diese Komponente die zugeführte Endenergie in nutzbare Wärme wandelt. Die Wärmeerzeuger werden nach den verschiedenen Endenergieträgern Gas, Öl Holz und Strom unterschieden, nicht jedoch nach Baujahr oder Bauart. Die Effizienz der Komponente wird durch den Jahresnutzungsgrad (Jahresarbeitszahl bei Wärmepumpen) charakterisiert. Er ist definiert als Verhältnis der im Jahr zur Nutzung erzeugten Wärme zu der dem Wärmeerzeuger zugefügten Endenergie ohne erneuerbare Energien. Der nächste untersuchte Kennwert ist die Effizienz der zentralen Trinkwarmwasserversorgung. Sie gibt Aufschluss über Zirkulationsverluste und Verluste der Speicherung und Beladeleitung und ist häufig der Nutzungspfad mit der geringsten Effizienz. Die Effizienz wird über den Nutzungsgrad dargestellt und berechnet sich aus der Wärmeenergie, die im verbrauchten Trinkwarmwasser enthalten ist, dividiert durch die dem Trinkwarmwasserbereiter zugeführte Wärmemenge. Auch der Anteil lokaler erneuerbarer Energien wird betrachtet. Dieser Kennwert stellt dar, wie weit das Gebäude und die Wärmezentrale durch autarke erneuerbare Energie betrieben wird. Er wird aus dem Verhältnis der am und um das Gebäude lokal bereitgestellten erneuerbaren Energien zur Summe aller zugeführten Energien berechnet. Zuletzt werden die spezifischen CO2-Emissionen untersucht. Dieser Kennwert gibt an, welche Gesamtmenge an CO2-Emissionen durch den Wärmeverbrauch des Gebäudes erzeugt werden. Die Kennwerte „Wärmeerzeuger“ und „Trinkwarmwasserversorgung“ reflektieren die Effizienz der Anlagenteile, während die Kennwerte „lokal erzeugte erneuerbare Energien“ und „CO2-Emissionen“ die Zukunftsfähigkeit der Anlage beurteilen. 
-Im einem Beispielobjekt des Projektes ist ein Optimierungspotential für die Effizienz des Kesselnutzungsgrades von 8 % zu erkennen, für Trinkwarmwasserversorgung wird ein Optimierungspotential von 9 % berechnet, allerdings liegt der Zielwert auf einem geringeren Niveau. Ein Anzeichen dafür, dass eine zentrale Trinkwarmwasserbereitung im Allgemeinen keine gute Effizienz aufweist, da signifikante Verteilverluste nicht vermieden werden können. Der Deutsche Verein des Gas- und Wasserfaches gibt an, dass die höchsten Effizienzen und Endenergieeinsparungen hygienisch sicher nur durch eine dezentrale Trinkwarmwasserversorgung erreicht werden können. Für den Anteil erneuerbarer Energie liegt der Zielwert dreimal so hoch wie der Messwert, was einem Potential von 300 % entspricht. Auch hier liegt der Zielwert auf einem niedrigen Niveau, da die lokale Nutzung regenerativer Energien im MFH-Bereich (Umweltwärme, Solarenergie) noch nicht stark verbreitet ist. Im Gegensatz zum gegrenzten Nutzungsgrad der zentralen Trinkwarmwasserversorgung wird der Zielwert bzw. das Potential beim Anteil der regenerativen Energien durch entsprechende Modernisierungen immer weiter Richtung 100% bewegen. Der Kennwert für die CO2-Emissionen liegt am Objekt recht nah am Zielwert, was unter Berücksichtigung des geringen Anteils lokal erzeugter regenerativer Energien auf eine Ausführung der Gebäudedämmung nach mindestens aktuellem Stand der Technik hinweist. 
-Für die Gaskessel im Gesamtbestand mit einem Mittelwert aller Anlagen von 80 % Jahresnutzungsgrad und von den besten Anlagen mit 90 % Jahresnutzungsgrad ergibt sich eine Abweichung von 10 %. Dies stellt auch das mittlere Optimierungspotential dar. Für die zentrale Trinkwarmwasserversorgung werden ebenso Einsparpotentiale berechnet. So zeigte sich an einem Beispielgebäude, dass höhere Trinkwarmwassertemperaturen und eine deutlich geringere Auslastung im Sommer zur Senkung des Nutzungsgrades der Heizzentrale um 10 %-Punkte führen können. Damit einher geht ein gesteigerter Endenergiebedarf von mindestens 10 %.
-Diesen, mit wenigen Mitteln erreichten, Einsparungen bzw. den ggf. durch die Erschließung der aufgezeigten Potenziale noch darüber hinaus möglichen Verbesserungen, stehen nur geringe ökologische Wirkungen gegenüber. Den CO2-Fußabdruck für die Komponenten eines Wärmepumpensystems (1 Wassserzähler, 2 Wärmezähler, 8 kabellose Temperatursensoren, 1 Datenlogger, 1 Smart-Meter) schätzt das Projekt mittels der Hilfestellung  zu den Umweltwirkungen häufig verwendeter Komponenten auf ca. 103,3 kg CO2eq/Jahr. Auch der Datenaufwand ist mit ca. 0,3 GB/Jahr gering. Über die Kennwerte  zu den Umweltlasten der Datenübertragung- und verarbeitung können die CO2-Emissionen auf ca. 0,8 kg CO2eq/Jahr geschätzt werden (Datenübertragung mit VDSL; Serverstandort Deutschland; Use-Case virtuelle Maschine). Bei einem Emissionsfaktor von ca. 0,5 kg CO2eq/kWh  müssten also nur ca. 208 kWh/a Strom eingespart werden, um die Umweltlasten ausgleichen zu können.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Positive impact</t>
   </si>
 </sst>
 </file>
@@ -701,15 +726,16 @@
   </sheetPr>
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="26.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="8.72"/>
   </cols>
   <sheetData>
@@ -842,54 +868,54 @@
         <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="X3" s="8"/>
     </row>
@@ -898,54 +924,54 @@
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -981,7 +1007,7 @@
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1056,10 +1082,10 @@
     </row>
     <row r="2" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>23</v>
@@ -1095,7 +1121,7 @@
         <v>33</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>35</v>
@@ -1112,110 +1138,110 @@
     </row>
     <row r="3" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="X3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
working on positive environmental impacts
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/16_positive_environmental_impact/Vorlage_Datenmodel_environmentalImpact_08204.xlsx
+++ b/02_work_doc/01_daten/16_positive_environmental_impact/Vorlage_Datenmodel_environmentalImpact_08204.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="77">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -212,7 +212,7 @@
 03ET1551A</t>
   </si>
   <si>
-    <t xml:space="preserve">01/2018 – 06/2025
+    <t xml:space="preserve">01/2018 – 06/2025,
 01/2018 – 03/2025 </t>
   </si>
   <si>
@@ -320,6 +320,10 @@
   </si>
   <si>
     <t xml:space="preserve">Bild1_RLT-Opt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/2018 – 06/2025
+01/2018 – 03/2025 </t>
   </si>
   <si>
     <t xml:space="preserve">llec_logo_large_transparent</t>
@@ -727,7 +731,7 @@
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -735,7 +739,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="26.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="8.72"/>
   </cols>
   <sheetData>
@@ -1150,7 +1154,7 @@
         <v>42</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>44</v>
@@ -1173,7 +1177,7 @@
         <v>49</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P3" s="7" t="s">
         <v>51</v>
@@ -1188,7 +1192,7 @@
         <v>41</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="X3" s="8"/>
     </row>
@@ -1229,7 +1233,7 @@
         <v>65</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="P4" s="7" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
inserted links onto postivei_environemntal_impact sites
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/16_positive_environmental_impact/Vorlage_Datenmodel_environmentalImpact_08204.xlsx
+++ b/02_work_doc/01_daten/16_positive_environmental_impact/Vorlage_Datenmodel_environmentalImpact_08204.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="82">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -186,16 +186,133 @@
   </si>
   <si>
     <t xml:space="preserve">Im Rahmen des Projekts wurden verschiedene Ansätze verfolgt, um Potenziale zu heben und die Effizienz der raumlufttechnischen Anlagen zu steigern. Eine zentrale Stellschraube war die einfache Regelungsoptimierung nach den Normen DIN EN 15232 und ISO 52120. Hierbei erfolgte eine Gesamtsystembetrachtung, um den Volumenstrom des Ventilators aus Basis eines Soll-Ist-Vergleichs zu minimieren. Bedarfsgerechte Anpassungen der Betriebszeiten und Volumenströme im fortlaufenden Betrieb wurden ebenfalls umgesetzt. Zusätzlich wurden umfangreichere Optimierungsmaßnahmen auf Grundlage von Monitoring-Daten durchgeführt, um beispielsweise gleichzeitiges Heizen und Kühlen zu verhindern.
+&lt;br&gt;&lt;br&gt;
 Für die technische Umsetzung kamen zwei Varianten des Monitorings zum Einsatz. Ein mobiles Monitoring wurde zur Erfassung und Bewertung des Status-Quo genutzt, während ein stationäres Monitoring mit festverbauten Komponenten zusätzliche Einblicke in den Betrieb und eine kontinuierliche Betriebsoptimierung ermöglichte. Das mobile Monitoring erfordert weniger Komponenten. Der Ressourcen-Energiebedarf der Technik für das mobile Monitoring wird im Projekt als sehr gering eingeschätzt. Er beläuft sich auf wenige zusätzliche Sensoren und Zähler. Nichtsdestotrotz lassen sich bereits mit dem mobilen Monitoring enorme Einspareffekte erzielen, insbesondere in Bezug auf die Funktionalität und Dimensionierung der Anlagen bzw. deren Betriebsparameter. 
+&lt;br&gt;&lt;br&gt;
 Die Implementierung des stationären Monitorings erforderte wiederum zusätzliche Hardware und einen höheren Datenaufwand. Dabei gilt grundsätzlich, dass Art und Anzahl der zusätzlich notwendigen Komponenten stark von der Größe und Grundausstattung der Liegenschaft sowie von den dortigen Anlagen abhängt. Mit der Aufnahme detaillierter Betriebszustände sind dann jedoch tiefergehende Analysen möglich, mit denen weitere Einsparpotenziale erst erschlossen werden können. </t>
   </si>
   <si>
-    <t xml:space="preserve">Als positive Umweltwirkungen wurden im Projekt vor allem Energie- und CO2-Einsparungen angestrebt. Die Quantifizierung dieser Wirkungen wurde mittels eines Vorher-Nachher-Vergleichs tatsächlicher Energiemengen versucht, der sich auf unterschiedliche Zeiträume erstrecken kann (in Abh. des jeweiligen Monitoringkonzepts – mobil und/oder stationär). Im Allgemeinen wurden Kennwerte zur Anlagenbewertung in Anlehnung an DIN SPEC 15240 und DIN 18599 gebildet. Einsparungen wurden teilweise messtechnisch nachgewiesen und teilweise über Hochrechnungen nach allgemeinen physikalischen Regeln bewertet, wobei um Wettereinflüsse gewichtete Bereinigungen vorgenommen wurden. Darauf aufbauend wurden die CO2-Einsparungen ausgehend von den, vom Bundesamt für Wirtschaft und Ausfuhrkontrolle veröffentlichten, Emissionsfaktoren für Energieaudits berechnet.     
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Als positive Umweltwirkungen wurden im Projekt vor allem Energie- und CO2-Einsparungen angestrebt. Die Quantifizierung dieser Wirkungen wurde mittels eines Vorher-Nachher-Vergleichs tatsächlicher Energiemengen versucht, der sich auf unterschiedliche Zeiträume erstrecken kann (in Abh. des jeweiligen Monitoringkonzepts – mobil und/oder stationär). Im Allgemeinen wurden Kennwerte zur Anlagenbewertung in Anlehnung an DIN SPEC 15240 und DIN 18599 gebildet. Einsparungen wurden teilweise messtechnisch nachgewiesen und teilweise über Hochrechnungen nach allgemeinen physikalischen Regeln bewertet, wobei um Wettereinflüsse gewichtete Bereinigungen vorgenommen wurden. Darauf aufbauend wurden die CO2-Einsparungen ausgehend von den, vom Bundesamt für Wirtschaft und Ausfuhrkontrolle veröffentlichten, Emissionsfaktoren für Energieaudits berechnet.&lt;sup id=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"ref1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&gt;&lt;a href="#footnote1"&gt;1&lt;/a&gt;&lt;/sup&gt;    &lt;br&gt;&lt;br&gt;
 Die erzielten Ergebnisse der Optimierung nach den Normen DIN EN 15232 und ISO 52120 waren bemerkenswert mit durchschnittlichen Stromeinsparungen von durchgängig &gt; 30 %. Gerade das grundsätzliche Einstellen des Volumenstroms (Soll-Ist Abgleich, Anpassen der Betriebszeiten etc.) stellt dabei eine einfach umzusetzende Maßnahme dar, welche sich bereits unter Einsatz des mobilen Monitorings – also unter minimalen Einsatz von Messtechnik und Ressourcen – durchführen lässt. Bei einigen Anlagen können die somit erzielten Einsparungen auch noch deutlich höher als die mittleren 30 % ausfallen. Denn bereits bei einer Verringerung des Volumenstroms um 20 % halbiert sich die Leistungsaufnahme. So konnte der Volumenstrom für die Belüftung des Kellerbereichs einer Beispielliegenschaft um 39 % gesenkt werden, was eine Reduktion des Strombedarfs um 78 % bewirkte. Jährlich können somit ca. 270 MWh bzw. 198 tCO2eqeingespart werden. Mit der Feinjustierung der Anlagen in Abhängigkeit der Raumbelegung/Raumnutzung lassen sich dann weitere Effizienzpotenziale erschließen. Dafür wird jedoch das stationäre Monitoring notwendig, da längere Zeiträume betrachtet werden müssen. Eine weitere positive Umweltwirkung die mit der Optimierung des Betriebs einhergeht: durch die geringe Nutzung, verschleißen die Anlagen auch weniger. Dadurch kann die Lebensdauer deutlich gesteigert werden. Der Projektverbund geht hier von möglichen Lebensdauersteigerungen von bis zu 10 Jahren aus. Ressourcen werden somit länger genutzt und Emissionen vermieden. Ebenso wird die Fehlererkennung vereinfacht bzw. verfrüht, was dazu führen kann, die Anlagen schneller und effektiver zu warten bzw. instand zu halten.  
 Negative Umweltauswirkungen der digitalen Anwendungen wurden nicht mit in die Bilanz einbezogen. Je nach vorhandener Anlagentechnik und Gebäudeleittechnik fallen die Emissionen, hervorgerufen durch das Monitoring sowie die Datenverarbeitung, in den einzelnen Liegenschaften unterschiedlich hoch aus. Am Beispiel des großen Bürogebäudekomplexes (größte untersuchte Liegenschaft): hier wurden über hundert zusätzliche Sensoren (Lufttemperatur, Bestrahlungsstärke, Luftfeuchte, Präsenzmelder, CO2, Druck) ca. 50 Zähler (Strom, Volumenstrom, Wärmemengen), mehrere Kommunikationssysteme (BUS-Systeme, Router, Repeater, Laptops) und mehrere hundert Meter Kabel (Strom, Luft, LAN) für das stationäre Monitoring zusätzlich installiert. Insgesamt entsteht bei dieser Liegenschaft ein Datenaufwand von 10 GB/Jahr. Bei solchen, vergleichsweise komplexen, Liegenschaften kann es zudem zu weiteren Hürden kommen, die die Effektivität der Maßnahmen verringern können. Hier ist vor allem die Gebäudeleittechnik bzw. deren Zugänglichkeit (geschlossene Schnittstellen, Fehlen der Expert*innenebene) zu nennen, welche die Umsetzbarkeit der Handlungsempfehlungen zur Betriebsoptimierung erschweren kann. Prädiktive Regelstrategien, die ggf. noch höhere Einsparpotenziale mit sich bringen würden, sind somit oftmals nur kostspielig umsetzbar. Gleichzeitig ist es sinnvoll, die Anlagenbetreiber*innen bei der Umsetzung der möglichen Betriebsoptimierungsstrategien (z.B. manuelles Einstellen des Volumenstroms oder der Betriebszeiten) zu unterstützen, da sich im Projekt zeigte, dass diesbezüglich z.T. wenig Expertise und vorherige Berührungspunkte existieren. Trotz der materiellen Aufwände und technisch-organisatorischen Hürden, konnten auch bei großen Liegenschaften Stromeinsparungen von durchgängig &gt; 30 % realisiert werden. </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">RLT-Opt– Lüftungs- und Klimaanlagen ganzheitlich optimieren</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup id=”sup1”&gt;&lt;a href="#ref1"&gt;1&lt;/a&gt;&lt;/sup&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Basis für Berechnung: Emissionsfaktor Strom (Effizienzmaßnahmen) = 0,732 tCO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/MWh, aus </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Informationsblatt CO</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-Faktoren</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; Bundesamt für Wirtschaft und Ausfuhrkontrolle, 2021.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Der Fokus des Projekts liegt insbesondere auf der Energieeffizienzsteigerung von Heizungs-, Kühlungs- und Klimasysteme in Bürogebäuden unter Berücksichtigung der Zufriedenheit der Nutzenden. Zum Einsatz kommt dabei eine Modell-prädikative Regelung (engl. Model Predicitve Control (MPC)), die es ermöglicht, nicht-lineares Systemverhalten vorauszusagen und automatisiert zu steuern. Verschiedene Studien beziffern die Energieeinsparungen zwischen 15 % und 50 % (Mork et al. 2023).</t>
@@ -237,27 +354,124 @@
     <t xml:space="preserve">assets/images/llec_logo_large_transparent.png</t>
   </si>
   <si>
-    <t xml:space="preserve">Die Heterogenität von Gebäuden, die beispielsweise durch unterschiedliche Anlagenparks und/oder Nutzungsprofile entsteht, sowie das Verhalten der Nutzenden von Gebäuden stellen komplexe Herausforderungen zur Minimierung des Energieverbrauchs dar. Oftmals fehlen verlässliche Daten und entsprechende digitale Anwendungen, um den Energieverbrauch und die Effizienz von Gebäuden angemessen zu bewerten und zu optimieren. Durch ihren erheblichen Anteil am Gesamtenergieverbrauch (30 %) steht die Verbesserung der Energieeffizienz und Reduzierung von CO2-Emissionen von Gebäuden zunehmend im Fokus derzeitiger Forschung (United Nations Environment Programme 2021).
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Die Heterogenität von Gebäuden, die beispielsweise durch unterschiedliche Anlagenparks und/oder Nutzungsprofile entsteht, sowie das Verhalten der Nutzenden von Gebäuden stellen komplexe Herausforderungen zur Minimierung des Energieverbrauchs dar. Oftmals fehlen verlässliche Daten und entsprechende digitale Anwendungen, um den Energieverbrauch und die Effizienz von Gebäuden angemessen zu bewerten und zu optimieren. Durch ihren erheblichen Anteil am Gesamtenergieverbrauch (30 %) steht die Verbesserung der Energieeffizienz und Reduzierung von CO2-Emissionen von Gebäuden zunehmend im Fokus derzeitiger Forschung &lt;a href="#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">United_Nations_Environment_2021"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(United Nations Environment Programme 2021)&lt;/a&gt;.
+&lt;br&gt;&lt;br&gt;
 Das Living Lab Energy Campus (LLEC) am Forschungszentrum Jülich verfolgt das Ziel, Lösungen für die Energieeffizienz in Gebäuden zu erforschen und der Öffentlichkeit  vorzustellen. Hochgradig vernetzte Demonstratoren zeigen verschiedene Forschungsarbeiten, beispielsweise zu Photovoltaik oder der Energiespeicherung. Außerdem wird in zwei Projekten versucht, durch die Integration innovativer Technologien und Ansätze den Energieverbrauch zu minimieren. Zentraler Schlüssel ist dabei die Erfassung und Analyse von Gebäudedaten. Darauf aufbauend werden modulare Lösungen entworfen, die nach erfolgreicher Testung auch auf andere Gebäude übertragen werden können. Ein Schwerpunkt der Optimierung ist diesbezüglich die Entwicklung intelligenter Regelung zur Steuerung von Energieverbrauchsanlagen in einigen Gebäuden und der Energiedemonstratoren des Campus. Um der hohen Heterogenität der Gebäude bzw. Gebäudeteile zu begegnen, muss dabei eine Vielzahl an Einflussgrößen betrachtet werden. Parallel dazu wird in einem anderen Gebäude das Nutzerverhalten als aktives Mittel zur Verbrauchsminimierung erforscht und genutzt. Das LLEC ermöglicht die Entwicklung und Anwendung solcher Lösungen in einem repräsentativen und realistischen Umfeld, das Validierung von Forschungsergebnissen ermöglicht. Insbesondere im Verwaltungsbau kann die Einwirkung auf die intrinsische Motivation von Personen essentiell sein, da sie sich nachgewiesenermaßen nicht für ihren Einfluss auf Energieverbrauch verantwortlich fühlen, solange sie die Kosten nicht tragen. 
 Ein weiteres Ziel des Projekts ist die Förderung des Wissenstransfers und die Sensibilisierung für das Thema Energieeffizienz in Gebäuden. Das LLEC bietet dazu Schulungen, Workshops und Informationsveranstaltungen für Fachleute, Studierende und die interessierte Öffentlichkeit an, um das Bewusstsein für energieeffizientes Bauen zu stärken und Fachwissen zu verbreiten.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Der Fokus des Projekts liegt insbesondere auf der Energieeffizienzsteigerung von Heizungs-, Kühlungs- und Klimasysteme in Bürogebäuden unter Berücksichtigung der Zufriedenheit der Nutzenden. Zum Einsatz kommt dabei eine Modell-prädikative Regelung (engl. Model Predicitve Control (MPC)), die es ermöglicht, nicht-lineares Systemverhalten vorauszusagen und automatisiert zu steuern. Verschiedene Studien beziffern die Energieeinsparungen zwischen 15 % und 50 % (Mork et al. 2023). Im Projekt berücksichtigt die praktisch umgesetzte MPC den Energieverbrauch für Heizung und Beleuchtung, thermisches Unbehagen, sowie potenzielle Nutzer-Störungen durch hochfrequentes Fahren der Verschattung. Die Steuerung erfolgt unter Rücksichtnahme auf Abstimmungsparameter und Komfortgrenzen. Es ist zu erwähnen, dass für die Nutzung der MPC derzeit eine maßgeschneiderte Modellierung für jedes individuelle Gebäude notwendig ist, aber auch in diesem Projekt an Vereinfachungen gearbeitet wird (z.B. einfach zu erstellende und übertragbare Modelica-Module).  Bezüglich des Einflusses des Wetters wurden unterschiedliche Effekte wie Außentemperaturen / Heizbedarfe, Windstärken und solare Gewinne mit in die Steueralgorithmen einbezogen. 
-Unabhängig von den Ansätzen zur MPC, beschäftigen sich die Forschenden mit der Integration von Softwareanwendungen, die es ermöglichen, Energieverbrauchsdaten einzusehen und den Nutzenden Echtzeitempfehlungen für Verhaltensänderungen zu geben (Ubachukwu et al. 2023). Das „Energy Dashboard“ bietet Mitarbeitenden und Besucher*innen des LLEC u.a. auf Raumlevel einen Überblick über Heiz- und Stromverbrauch in Echtzeit. „JuControl“ geht eine Ebene weiter und ermöglicht es den Nutzenden, ihre persönlichen Präferenzen für das Raumklima abzubilden und in die Steuerung einzugreifen. In die Anwendung ist dabei ein Gamification Ansatz eingebettet, der den Vergleich mit anderen Personen/Teams ermöglicht. Das Feedback an die Nutzenden erfolgt über ein Ampelsystem, das den Energieverbrauch angibt. Die Bewertung der Ampel erfolgt anhand festgelegter Grenzen, gemessen in Kilowattstunden. Außerdem spiegelte die Anwendung einen “Energiestrafwert” wider, der simuliert wie hoch der Energieverbrauch des gesamten LLEC Campus gewesen wäre, wenn alle Personen ein entsprechendes Nutzungsprofil gehabt hätten (Idealwert). In diesem Sinne grenzt sich das Projekt von herkömmlichen Ansätzen zur Bewertung der positiven Umweltwirkungen ab. Während normalerweise die Einsparung in Referenz zum Status-Quo-Verbrauch gesetzt wird, fragt die Referenz am LLEC nach dem Idealzustand, der erreicht werden könnte. Denn je nach Lage, Nutzungsart und persönlichen Erfahrungen der Nutzenden, können die Möglichkeiten zu Energieeinsparungen in Einzelräumen stark variieren. Durch die Definition eines Ideals wird diesen Einflüssen Rechnung getragen. Ergänzt wird das System zur Nutzendeneinbindung durch ein Leaderboard (in der Anwendung „JuPower“), das Teams mit dem niedrigsten Energieverbrauch auszeichnet. Anreize für energieeffizientes Verhalten der Nutzenden wird zudem durch soziale Interaktion und „game rewards“ geschaffen.
-Um die korrekte Messung der Daten zu gewährleisten wurden in allen teilnehmenden Gebäuden Sensoren des Typs EnOcean zur Messung der Luftqualität, der CO2 Konzentration, Temperatur und Feuchtigkeit verbaut. Die Verarbeitung der Daten erfolgte mit M-Bus. Zur automatischen Steuerung von Beleuchtung, Heizung und Sonnenschutz kamen KNX Steuerelemente und BACnet-Systeme zum Einsatz. Über den gesamten Campus des LLEC wurden Untersuchungen zur Integration von über 1800 Geräten in 18 Gebäuden mittels einer Informations- und Kommunikationsplattform durchgeführt (EnOcean: 1676 Sensoren und 108 Aktuatoren, KNX: 48 Sensoren und 36 Aktuatoren) (Althaus et al. 2022). </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Der Fokus des Projekts liegt insbesondere auf der Energieeffizienzsteigerung von Heizungs-, Kühlungs- und Klimasysteme in Bürogebäuden unter Berücksichtigung der Zufriedenheit der Nutzenden. Zum Einsatz kommt dabei eine Modell-prädikative Regelung (engl. Model Predicitve Control (MPC)), die es ermöglicht, nicht-lineares Systemverhalten vorauszusagen und automatisiert zu steuern. Verschiedene Studien beziffern die Energieeinsparungen zwischen 15 % und 50 % &lt;a href=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"#Mork,_Maximilian,_Florian_2023"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(Mork et al. 2023)&lt;/a&gt;. Im Projekt berücksichtigt die praktisch umgesetzte MPC den Energieverbrauch für Heizung und Beleuchtung, thermisches Unbehagen, sowie potenzielle Nutzer-Störungen durch hochfrequentes Fahren der Verschattung. Die Steuerung erfolgt unter Rücksichtnahme auf Abstimmungsparameter und Komfortgrenzen. Es ist zu erwähnen, dass für die Nutzung der MPC derzeit eine maßgeschneiderte Modellierung für jedes individuelle Gebäude notwendig ist, aber auch in diesem Projekt an Vereinfachungen gearbeitet wird (z.B. einfach zu erstellende und übertragbare Modelica-Module).  Bezüglich des Einflusses des Wetters wurden unterschiedliche Effekte wie Außentemperaturen / Heizbedarfe, Windstärken und solare Gewinne mit in die Steueralgorithmen einbezogen. &lt;br&gt;&lt;br&gt; 
+Unabhängig von den Ansätzen zur MPC, beschäftigen sich die Forschenden mit der Integration von Softwareanwendungen, die es ermöglichen, Energieverbrauchsdaten einzusehen und den Nutzenden Echtzeitempfehlungen für Verhaltensänderungen zu geben &lt;a href=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"#Ubachukwu,_Eziama,_Jana_2023"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(Ubachukwu et al. 2023)&lt;/a&gt;. Das „Energy Dashboard“ bietet Mitarbeitenden und Besucher*innen des LLEC u.a. auf Raumlevel einen Überblick über Heiz- und Stromverbrauch in Echtzeit. „JuControl“ geht eine Ebene weiter und ermöglicht es den Nutzenden, ihre persönlichen Präferenzen für das Raumklima abzubilden und in die Steuerung einzugreifen. In die Anwendung ist dabei ein Gamification Ansatz eingebettet, der den Vergleich mit anderen Personen/Teams ermöglicht. Das Feedback an die Nutzenden erfolgt über ein Ampelsystem, das den Energieverbrauch angibt. Die Bewertung der Ampel erfolgt anhand festgelegter Grenzen, gemessen in Kilowattstunden. Außerdem spiegelte die Anwendung einen “Energiestrafwert” wider, der simuliert wie hoch der Energieverbrauch des gesamten LLEC Campus gewesen wäre, wenn alle Personen ein entsprechendes Nutzungsprofil gehabt hätten (Idealwert). In diesem Sinne grenzt sich das Projekt von herkömmlichen Ansätzen zur Bewertung der positiven Umweltwirkungen ab. Während normalerweise die Einsparung in Referenz zum Status-Quo-Verbrauch gesetzt wird, fragt die Referenz am LLEC nach dem Idealzustand, der erreicht werden könnte. Denn je nach Lage, Nutzungsart und persönlichen Erfahrungen der Nutzenden, können die Möglichkeiten zu Energieeinsparungen in Einzelräumen stark variieren. Durch die Definition eines Ideals wird diesen Einflüssen Rechnung getragen. Ergänzt wird das System zur Nutzendeneinbindung durch ein Leaderboard (in der Anwendung „JuPower“), das Teams mit dem niedrigsten Energieverbrauch auszeichnet. Anreize für energieeffizientes Verhalten der Nutzenden wird zudem durch soziale Interaktion und „game rewards“ geschaffen.
+&lt;br&gt;&lt;br&gt;Um die korrekte Messung der Daten zu gewährleisten wurden in allen teilnehmenden Gebäuden Sensoren des Typs EnOcean zur Messung der Luftqualität, der CO2 Konzentration, Temperatur und Feuchtigkeit verbaut. Die Verarbeitung der Daten erfolgte mit M-Bus. Zur automatischen Steuerung von Beleuchtung, Heizung und Sonnenschutz kamen KNX Steuerelemente und BACnet-Systeme zum Einsatz. Über den gesamten Campus des LLEC wurden Untersuchungen zur Integration von über 1800 Geräten in 18 Gebäuden mittels einer Informations- und Kommunikationsplattform durchgeführt (EnOcean: 1676 Sensoren und 108 Aktuatoren, KNX: 48 Sensoren und 36 Aktuatoren) &lt;a href="#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Althaus,_Philipp,_Florian</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_2022"&gt;(Althaus et al. 2022)&lt;/a&gt;. </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Die Forschenden schätzen die Energieeinsparungen, die mittels MPC erreicht werden können, über sämtliche getestete Gebäude auf ca. 10 – 15 %. Dazu wurde ein digitaler Zwilling der Gebäude mittels unterschiedlicher Regelstrategien vergleichend betrieben. Den größten Einfluss auf die Energieeinsparungen haben dabei das intelligente Steuern der Raumtemperatur, der automatisierten Fensteröffnung sowie das Anpassen des Sonnenschutzes (Fokus Wärme/Klimatisierung; Auswirkungen auf Strombedarf für Beleuchtung nicht inkludiert).  Der Sonnenschutz ist so ausgelegt, dass ein Maximum an solaren Wärmegewinnen und Tageslicht nutzbar gemacht werden kann, um den Energieverbrauch für Heizung und Beleuchtung zu minimieren. Die messtechnische Überprüfung konnte die Simulationen qualitativ bestätigen. So wurden energieeffizientere Raumtemperaturprofile gemessen. Ein genauer Vergleich des Energieverbrauchs konnte jedoch auf Grund mangelnder Zähler in den einzelnen Räumen / Gebäudeteilen nicht zielführend durchgeführt werden. Quantitativ kann das LLEC die hohe Genauigkeit des white-box MPC-Modells bestätigen. Der Root Mean Square Error (RSME) zwischen gemessener und geschätzter Raumtemperatur lag bei 0,49 °C. Zudem konnte die effiziente Arbeitsweise der Regelung belegt werden. Im Vergleich mit einem konventionellen Regelungsansatz (0,47 kh/d) blieb die thermische Unbehaglichkeit mit einem Wert von 0,53 kh/d weitestgehend stabil. 
+&lt;br&gt;&lt;br&gt;
 Für die Nutzendeneinbindung ist zu erwähnen, dass unterschiedlichen Maßnahmen (Dashboards, JuControl, JuPower) seit 2020 durch mehr als 1300 Mitarbeitende genutzt wurden. Zur Evaluierung der Effektivität der Nutzendeneinbindung wurde basierend auf den historischen Daten vor Implementierung der Maßnahmen ein Regressionsmodell aufgesetzt, was den entstandenen Heizenergiebedarf maßgeblich als Funktion der Außentemperatur beschreibt (Fitgüte: R2 = 0,91). Dieses Modell wurde dann ebenso auf die Periode mit implementierten Maßnahmen zur Nutzendeneinbindung angewandt und mit dem tatsächlichen Energieverbrauch des Gebäudes verglichen. Es konnte gezeigt werden, dass, verglichen mit der Referenzperiode, der Heizbedarf in Abhängigkeit der Außentemperatur weniger stark anstieg und die durchschnittliche Temperatur des Pilotgebäudes durchschnittlich um 1 °C gesenkt werden konnte. Diese Effekte trugen maßgeblich zu der gemessenen Verbrauchsreduktion von 11.1 MWh pro Jahr (- 16,7 %) bei, welche die Verantwortlichen auf Grund der gleichen Systemparameter (Energetischer Zustand des Gebäudes und des Heizsystems) auf die effizientere Nutzung des Heizsystems und ein effizienteres Nutzendenverhalten zurückführen. Bei einem Gaskraftwerk zur Heizwärmebereitstellung (angenommener Emissionsfaktor von 200 g CO2e/kWhprimär; Primärenergiefaktor Erdgas = 1,1) entspricht dies einer Einsparung von ca. 2,44 t CO2e pro Jahr. Für Unterschiede in der Außentemperatur der beiden Perioden wurde dabei korrigiert, andere Einflussgrößen wurden jedoch nicht betrachtet (z.B. Wind, Solare Gewinne). Das Komfortlevel der Menschen wurde dabei nicht negativ beeinflusst. Dabei weisen die Projektverantwortlichen auf das zusätzliche Potential hin, da nur ein Fünftel der Büros in dem Gebäude für die Maßnahmen zur Nutzendeneinbindung aktiviert waren. 
-Die negativen Umweltwirkungen der verbauten Komponenten wurden weder für die MPC noch die Nutzendeneinbindung bilanziert. Bei der am LLEC vorzufindenden (Komponenten-)Infrastruktur besteht die Schwierigkeit zur Bewertung der negativen Wirkungen vor allem in der Allokation der Komponenten, da neben den hier beschriebenen digitalen Anwendungen noch viele weitere Prozesse und Anwendungen die gleichen Komponenten nutzen. Daher ist eine genaue Zuordnung zu einzelnen digitalen Anwendungen schwierig. Jedoch mussten für die Einzelraummessungen eine Vielzahl an batteriebetriebenen Komponenten verbaut werden (&gt; 1800 Komponenten auf dem Campus insgesamt). Da all diese Komponenten fortwährend mit den digitalen Anwendungen Daten austauschen bzw. diese auf diese zurückgreifen, fällt ein entsprechend hoher Datenaufwand an. Alleine für die Maßnahmen zur Nutzendeneinbindung wurden in ca. 3 Jahren 364 Mio. Datensätzen erfasst und aufgearbeitet (ca. 74 GB insgesamt bzw. ca. 25 GB/a). Dabei gehen die Forschenden davon aus, dass sich der Datenaufwand bei einer noch praxisnäheren Implementierung um ca. 25% reduzieren lassen könnte. Zum einen, da die Anzahl an Datenpunkten in etwa um diese Größe reduziert werden könnte. Zum anderen, weil nach erfolgreicher Erprobung im Forschungskontext weniger Redundanzen bei den Messstellen und eine geringerer Datengranularität nötig wären.  Für die MPC werden täglich ca. 300 MB an Daten auf einem OpenStack Server verarbeitet. Nur ein Bruchteil entfällt dabei auf die Erfassung der Messdaten aus den Räumen (ca. 5 MB pro Tag; 15 minütige Daten zu Raum-Temperatur, Zustände von Fenster- und Tür-Kontakten und Anzahl an Personen im Raum). Zusammengenommen fragen die Nutzendeneinbindung und die MPC jährlich virtuelle Ressourcen für ca. 124 GB nach, was überschlägig CO2-Emissionen von ca. 339 kg CO2e bedeuten würde (vergleiche Abschätzung der negativen Wirkungen durch die Datenübertragung und -verarbeitung hier ).  
+&lt;br&gt;&lt;br&gt;
+Die negativen Umweltwirkungen der verbauten Komponenten wurden weder für die MPC noch die Nutzendeneinbindung bilanziert. Bei der am LLEC vorzufindenden (Komponenten-)Infrastruktur besteht die Schwierigkeit zur Bewertung der negativen Wirkungen vor allem in der Allokation der Komponenten, da neben den hier beschriebenen digitalen Anwendungen noch viele weitere Prozesse und Anwendungen die gleichen Komponenten nutzen. Daher ist eine genaue Zuordnung zu einzelnen digitalen Anwendungen schwierig. Jedoch mussten für die Einzelraummessungen eine Vielzahl an batteriebetriebenen Komponenten verbaut werden (&gt; 1800 Komponenten auf dem Campus insgesamt). Da all diese Komponenten fortwährend mit den digitalen Anwendungen Daten austauschen bzw. diese auf diese zurückgreifen, fällt ein entsprechend hoher Datenaufwand an. Alleine für die Maßnahmen zur Nutzendeneinbindung wurden in ca. 3 Jahren 364 Mio. Datensätzen erfasst und aufgearbeitet (ca. 74 GB insgesamt bzw. ca. 25 GB/a). Dabei gehen die Forschenden davon aus, dass sich der Datenaufwand bei einer noch praxisnäheren Implementierung um ca. 25% reduzieren lassen könnte. Zum einen, da die Anzahl an Datenpunkten in etwa um diese Größe reduziert werden könnte. Zum anderen, weil nach erfolgreicher Erprobung im Forschungskontext weniger Redundanzen bei den Messstellen und eine geringerer Datengranularität nötig wären.  Für die MPC werden täglich ca. 300 MB an Daten auf einem OpenStack Server verarbeitet. Nur ein Bruchteil entfällt dabei auf die Erfassung der Messdaten aus den Räumen (ca. 5 MB pro Tag; 15 minütige Daten zu Raum-Temperatur, Zustände von Fenster- und Tür-Kontakten und Anzahl an Personen im Raum). Zusammengenommen fragen die Nutzendeneinbindung und die MPC jährlich virtuelle Ressourcen für ca. 124 GB nach, was überschlägig CO2-Emissionen von ca. 339 kg CO2e bedeuten würde (vergleiche Abschätzung der negativen Wirkungen durch die Datenübertragung und -verarbeitung &lt;a href=“{% url  'dataProcessing' %}“&gt;hier&lt;/a&gt; ).  
+&lt;br&gt;&lt;br&gt;
 Schließlich sieht das Projekt verschiedene Anknüpfungsmöglichkeiten für künftige Forschungsvorhaben. Da MPC-Modelle zwar hohe Einsparpotenziale versprechen, jedoch gleichzeitig einen hohen Aufwand für individuelle Kalibrierung benötigen, besteht ein hoher Bedarf für die Entwicklung von einfach übertragbaren MPC-Ansätzen für kommerzielle Zwecke. Auf die vereinfachte Übertragung auf andere Gebäude zielt auch die angestrebte Verknüpfung beider Anwendungen des Projekts ab (MPC &amp; Nutzendeneinbindung). So sind noch effizienzsteigernde Anpassungsmöglichkeiten innerhalb der Kostenfunktion des MPC möglich. Da beide Aspekte modular entwickelt wurden, ist eine zukünftige Verschränkung denkbar und sinnvoll um bspw. die Effektivität der MPC unter Einfluss von benutzerdefinierte Komforteinstellungen oder angepassten Handlungsempfehlungen an die Nutzenden zu testen. Zudem nennen die Forschenden den Bedarf für umfassendere Versuche in größeren Gebäuden unter Einbeziehung ganzzahliger Entscheidungsvariablen, sowie der Vorlauftemperaturen von Heizwasservolumenströmen (zentrale Heizungssysteme) als weitere Entwicklungsfelder. </t>
   </si>
   <si>
     <t xml:space="preserve">Althaus, Philipp, Florian Redder, Eziama Ubachukwu, Maximilian Mork, André Xhonneux und Dirk Müller (2022): Enhancing Building Monitoring and Control for District Energy Systems: Technology Selection and Installation within the Living Lab Energy Campus. Applied Sciences 12, Nr. 7 (Januar): 3305.;;
 Mork, Maximilian, Florian Redder, André Xhonneux und Dirk Müller (2023): Real-world implementation and evaluation of a Model Predictive Control framework in an office space. Journal of Building Engineering 78 (1. November): 107619.;;
-Ubachukwu, Eziama, Jana Pick, Lea Riebesel, Paul Lieberenz, Philipp Althaus, Dirk Müller und André Xhonneux (2023): LLEC Energy Dashboard Suite: User Engagement for Energy-Efficient Behavior Using Dashboards and Gamification. In: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), S. 3241–3252. Veranstaltung: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), Las Palmas De Gran Canaria, Spain. http://www.proceedings.com/069564-0291.html.
-United Nations Environment Programme (2021): 2021 Global Status Report for Buildings and Construction: Towards a Zero-Emission, Efficient and Resilient Buildings and Construction Sector. Nairobi, Kenya: United Nations Environment Programme.
-</t>
+Ubachukwu, Eziama, Jana Pick, Lea Riebesel, Paul Lieberenz, Philipp Althaus, Dirk Müller und André Xhonneux (2023): LLEC Energy Dashboard Suite: User Engagement for Energy-Efficient Behavior Using Dashboards and Gamification. In: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), S. 3241–3252. Veranstaltung: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), Las Palmas De Gran Canaria, Spain. &lt;a href="http://www.proceedings.com/069564-0291.html"&gt;http://www.proceedings.com/069564-0291.html&lt;/a&gt;.;;
+United Nations Environment Programme (2021): 2021 Global Status Report for Buildings and Construction: Towards a Zero-Emission, Efficient and Resilient Buildings and Construction Sector. Nairobi, Kenya: United Nations Environment Programme.</t>
   </si>
   <si>
     <t xml:space="preserve">Wohnungsunternehmen betreiben meist unterschiedliche Gebäude mit einer Vielfalt von Technologien für die Heiz- und Warmwasserversorgung. Das Potenzial zur Betriebsoptimierung dieser Heizzentralen in Mehrfamilienhäusern ist enorm. Dies sollte möglichst bedienerfreundlich und idealerweise automatisiert erfolgen. </t>
@@ -310,7 +524,37 @@
 Im Projekt werden folgende vier Kennwerte genutzt, um einen Überblick über relevanten Qualitäten der Wärmezentralen zu geben. Die Effizienz des Wärmeerzeugers ist von zentraler Bedeutung, da diese Komponente die zugeführte Endenergie in nutzbare Wärme wandelt. Die Wärmeerzeuger werden nach den verschiedenen Endenergieträgern Gas, Öl Holz und Strom unterschieden, nicht jedoch nach Baujahr oder Bauart. Die Effizienz der Komponente wird durch den Jahresnutzungsgrad (Jahresarbeitszahl bei Wärmepumpen) charakterisiert. Er ist definiert als Verhältnis der im Jahr zur Nutzung erzeugten Wärme zu der dem Wärmeerzeuger zugefügten Endenergie ohne erneuerbare Energien. Der nächste untersuchte Kennwert ist die Effizienz der zentralen Trinkwarmwasserversorgung. Sie gibt Aufschluss über Zirkulationsverluste und Verluste der Speicherung und Beladeleitung und ist häufig der Nutzungspfad mit der geringsten Effizienz. Die Effizienz wird über den Nutzungsgrad dargestellt und berechnet sich aus der Wärmeenergie, die im verbrauchten Trinkwarmwasser enthalten ist, dividiert durch die dem Trinkwarmwasserbereiter zugeführte Wärmemenge. Auch der Anteil lokaler erneuerbarer Energien wird betrachtet. Dieser Kennwert stellt dar, wie weit das Gebäude und die Wärmezentrale durch autarke erneuerbare Energie betrieben wird. Er wird aus dem Verhältnis der am und um das Gebäude lokal bereitgestellten erneuerbaren Energien zur Summe aller zugeführten Energien berechnet. Zuletzt werden die spezifischen CO2-Emissionen untersucht. Dieser Kennwert gibt an, welche Gesamtmenge an CO2-Emissionen durch den Wärmeverbrauch des Gebäudes erzeugt werden. Die Kennwerte „Wärmeerzeuger“ und „Trinkwarmwasserversorgung“ reflektieren die Effizienz der Anlagenteile, während die Kennwerte „lokal erzeugte erneuerbare Energien“ und „CO2-Emissionen“ die Zukunftsfähigkeit der Anlage beurteilen. 
 Im einem Beispielobjekt des Projektes ist ein Optimierungspotential für die Effizienz des Kesselnutzungsgrades von 8 % zu erkennen, für Trinkwarmwasserversorgung wird ein Optimierungspotential von 9 % berechnet, allerdings liegt der Zielwert auf einem geringeren Niveau. Ein Anzeichen dafür, dass eine zentrale Trinkwarmwasserbereitung im Allgemeinen keine gute Effizienz aufweist, da signifikante Verteilverluste nicht vermieden werden können. Der Deutsche Verein des Gas- und Wasserfaches gibt an, dass die höchsten Effizienzen und Endenergieeinsparungen hygienisch sicher nur durch eine dezentrale Trinkwarmwasserversorgung erreicht werden können. Für den Anteil erneuerbarer Energie liegt der Zielwert dreimal so hoch wie der Messwert, was einem Potential von 300 % entspricht. Auch hier liegt der Zielwert auf einem niedrigen Niveau, da die lokale Nutzung regenerativer Energien im MFH-Bereich (Umweltwärme, Solarenergie) noch nicht stark verbreitet ist. Im Gegensatz zum gegrenzten Nutzungsgrad der zentralen Trinkwarmwasserversorgung wird der Zielwert bzw. das Potential beim Anteil der regenerativen Energien durch entsprechende Modernisierungen immer weiter Richtung 100% bewegen. Der Kennwert für die CO2-Emissionen liegt am Objekt recht nah am Zielwert, was unter Berücksichtigung des geringen Anteils lokal erzeugter regenerativer Energien auf eine Ausführung der Gebäudedämmung nach mindestens aktuellem Stand der Technik hinweist. 
 Für die Gaskessel im Gesamtbestand mit einem Mittelwert aller Anlagen von 80 % Jahresnutzungsgrad und von den besten Anlagen mit 90 % Jahresnutzungsgrad ergibt sich eine Abweichung von 10 %. Dies stellt auch das mittlere Optimierungspotential dar. Für die zentrale Trinkwarmwasserversorgung werden ebenso Einsparpotentiale berechnet. So zeigte sich an einem Beispielgebäude, dass höhere Trinkwarmwassertemperaturen und eine deutlich geringere Auslastung im Sommer zur Senkung des Nutzungsgrades der Heizzentrale um 10 %-Punkte führen können. Damit einher geht ein gesteigerter Endenergiebedarf von mindestens 10 %.
-Diesen, mit wenigen Mitteln erreichten, Einsparungen bzw. den ggf. durch die Erschließung der aufgezeigten Potenziale noch darüber hinaus möglichen Verbesserungen, stehen nur geringe ökologische Wirkungen gegenüber. Den CO2-Fußabdruck für die Komponenten eines Wärmepumpensystems (1 Wassserzähler, 2 Wärmezähler, 8 kabellose Temperatursensoren, 1 Datenlogger, 1 Smart-Meter) schätzt das Projekt mittels der Hilfestellung  zu den Umweltwirkungen häufig verwendeter Komponenten auf ca. 103,3 kg CO2eq/Jahr. Auch der Datenaufwand ist mit ca. 0,3 GB/Jahr gering. Über die Kennwerte  zu den Umweltlasten der Datenübertragung- und verarbeitung können die CO2-Emissionen auf ca. 0,8 kg CO2eq/Jahr geschätzt werden (Datenübertragung mit VDSL; Serverstandort Deutschland; Use-Case virtuelle Maschine). Bei einem Emissionsfaktor von ca. 0,5 kg CO2eq/kWh  müssten also nur ca. 208 kWh/a Strom eingespart werden, um die Umweltlasten ausgleichen zu können.</t>
+Diesen, mit wenigen Mitteln erreichten, Einsparungen bzw. den ggf. durch die Erschließung der aufgezeigten Potenziale noch darüber hinaus möglichen Verbesserungen, stehen nur geringe ökologische Wirkungen gegenüber. Den CO2-Fußabdruck für die Komponenten eines Wärmepumpensystems (1 Wassserzähler, 2 Wärmezähler, 8 kabellose Temperatursensoren, 1 Datenlogger, 1 Smart-Meter) schätzt das Projekt mittels der &lt;a href="{% url 'components' %}"&gt;Hilfestellung&lt;/a&gt;  zu den Umweltwirkungen häufig verwendeter Komponenten auf ca. 103,3 kg CO2eq/Jahr. Auch der Datenaufwand ist mit ca. 0,3 GB/Jahr gering. Über die &lt;a href="{% url 'dataProcessing' %}"&gt;Kennwerte&lt;/a&gt;  zu den Umweltlasten der Datenübertragung- und verarbeitung können die CO2-Emissionen auf ca. 0,8 kg CO2eq/Jahr geschätzt werden (Datenübertragung mit VDSL; Serverstandort Deutschland; Use-Case virtuelle Maschine). Bei einem Emissionsfaktor von ca. 0,5 kg CO2eq/kWh&lt;sup&gt;&lt;a href="#sup1"&gt;1&lt;/a&gt;&lt;/sup&gt;  müssten also nur ca. 208 kWh/a Strom eingespart werden, um die Umweltlasten ausgleichen zu können.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;sup id=”sup1”&gt;&lt;a href="#ref1"&gt;1&lt;/a&gt;&lt;/sup&gt; Vergleiche: &lt;a href='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'&gt;https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf&lt;/a&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Positive impact</t>
@@ -320,6 +564,16 @@
   </si>
   <si>
     <t xml:space="preserve">Bild1_RLT-Opt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Im Rahmen des Projekts wurden verschiedene Ansätze verfolgt, um Potenziale zu heben und die Effizienz der raumlufttechnischen Anlagen zu steigern. Eine zentrale Stellschraube war die einfache Regelungsoptimierung nach den Normen DIN EN 15232 und ISO 52120. Hierbei erfolgte eine Gesamtsystembetrachtung, um den Volumenstrom des Ventilators aus Basis eines Soll-Ist-Vergleichs zu minimieren. Bedarfsgerechte Anpassungen der Betriebszeiten und Volumenströme im fortlaufenden Betrieb wurden ebenfalls umgesetzt. Zusätzlich wurden umfangreichere Optimierungsmaßnahmen auf Grundlage von Monitoring-Daten durchgeführt, um beispielsweise gleichzeitiges Heizen und Kühlen zu verhindern.
+Für die technische Umsetzung kamen zwei Varianten des Monitorings zum Einsatz. Ein mobiles Monitoring wurde zur Erfassung und Bewertung des Status-Quo genutzt, während ein stationäres Monitoring mit festverbauten Komponenten zusätzliche Einblicke in den Betrieb und eine kontinuierliche Betriebsoptimierung ermöglichte. Das mobile Monitoring erfordert weniger Komponenten. Der Ressourcen-Energiebedarf der Technik für das mobile Monitoring wird im Projekt als sehr gering eingeschätzt. Er beläuft sich auf wenige zusätzliche Sensoren und Zähler. Nichtsdestotrotz lassen sich bereits mit dem mobilen Monitoring enorme Einspareffekte erzielen, insbesondere in Bezug auf die Funktionalität und Dimensionierung der Anlagen bzw. deren Betriebsparameter. 
+Die Implementierung des stationären Monitorings erforderte wiederum zusätzliche Hardware und einen höheren Datenaufwand. Dabei gilt grundsätzlich, dass Art und Anzahl der zusätzlich notwendigen Komponenten stark von der Größe und Grundausstattung der Liegenschaft sowie von den dortigen Anlagen abhängt. Mit der Aufnahme detaillierter Betriebszustände sind dann jedoch tiefergehende Analysen möglich, mit denen weitere Einsparpotenziale erst erschlossen werden können. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als positive Umweltwirkungen wurden im Projekt vor allem Energie- und CO2-Einsparungen angestrebt. Die Quantifizierung dieser Wirkungen wurde mittels eines Vorher-Nachher-Vergleichs tatsächlicher Energiemengen versucht, der sich auf unterschiedliche Zeiträume erstrecken kann (in Abh. des jeweiligen Monitoringkonzepts – mobil und/oder stationär). Im Allgemeinen wurden Kennwerte zur Anlagenbewertung in Anlehnung an DIN SPEC 15240 und DIN 18599 gebildet. Einsparungen wurden teilweise messtechnisch nachgewiesen und teilweise über Hochrechnungen nach allgemeinen physikalischen Regeln bewertet, wobei um Wettereinflüsse gewichtete Bereinigungen vorgenommen wurden. Darauf aufbauend wurden die CO2-Einsparungen ausgehend von den, vom Bundesamt für Wirtschaft und Ausfuhrkontrolle veröffentlichten, Emissionsfaktoren für Energieaudits berechnet.&lt;sup id="ref1"&gt;&lt;a href="#footnote1"&gt;1&lt;/a&gt;&lt;/sup&gt;    &lt;br&gt;&lt;br&gt;
+Die erzielten Ergebnisse der Optimierung nach den Normen DIN EN 15232 und ISO 52120 waren bemerkenswert mit durchschnittlichen Stromeinsparungen von durchgängig &gt; 30 %. Gerade das grundsätzliche Einstellen des Volumenstroms (Soll-Ist Abgleich, Anpassen der Betriebszeiten etc.) stellt dabei eine einfach umzusetzende Maßnahme dar, welche sich bereits unter Einsatz des mobilen Monitorings – also unter minimalen Einsatz von Messtechnik und Ressourcen – durchführen lässt. Bei einigen Anlagen können die somit erzielten Einsparungen auch noch deutlich höher als die mittleren 30 % ausfallen. Denn bereits bei einer Verringerung des Volumenstroms um 20 % halbiert sich die Leistungsaufnahme. So konnte der Volumenstrom für die Belüftung des Kellerbereichs einer Beispielliegenschaft um 39 % gesenkt werden, was eine Reduktion des Strombedarfs um 78 % bewirkte. Jährlich können somit ca. 270 MWh bzw. 198 tCO2eqeingespart werden. Mit der Feinjustierung der Anlagen in Abhängigkeit der Raumbelegung/Raumnutzung lassen sich dann weitere Effizienzpotenziale erschließen. Dafür wird jedoch das stationäre Monitoring notwendig, da längere Zeiträume betrachtet werden müssen. Eine weitere positive Umweltwirkung die mit der Optimierung des Betriebs einhergeht: durch die geringe Nutzung, verschleißen die Anlagen auch weniger. Dadurch kann die Lebensdauer deutlich gesteigert werden. Der Projektverbund geht hier von möglichen Lebensdauersteigerungen von bis zu 10 Jahren aus. Ressourcen werden somit länger genutzt und Emissionen vermieden. Ebenso wird die Fehlererkennung vereinfacht bzw. verfrüht, was dazu führen kann, die Anlagen schneller und effektiver zu warten bzw. instand zu halten.  
+Negative Umweltauswirkungen der digitalen Anwendungen wurden nicht mit in die Bilanz einbezogen. Je nach vorhandener Anlagentechnik und Gebäudeleittechnik fallen die Emissionen, hervorgerufen durch das Monitoring sowie die Datenverarbeitung, in den einzelnen Liegenschaften unterschiedlich hoch aus. Am Beispiel des großen Bürogebäudekomplexes (größte untersuchte Liegenschaft): hier wurden über hundert zusätzliche Sensoren (Lufttemperatur, Bestrahlungsstärke, Luftfeuchte, Präsenzmelder, CO2, Druck) ca. 50 Zähler (Strom, Volumenstrom, Wärmemengen), mehrere Kommunikationssysteme (BUS-Systeme, Router, Repeater, Laptops) und mehrere hundert Meter Kabel (Strom, Luft, LAN) für das stationäre Monitoring zusätzlich installiert. Insgesamt entsteht bei dieser Liegenschaft ein Datenaufwand von 10 GB/Jahr. Bei solchen, vergleichsweise komplexen, Liegenschaften kann es zudem zu weiteren Hürden kommen, die die Effektivität der Maßnahmen verringern können. Hier ist vor allem die Gebäudeleittechnik bzw. deren Zugänglichkeit (geschlossene Schnittstellen, Fehlen der Expert*innenebene) zu nennen, welche die Umsetzbarkeit der Handlungsempfehlungen zur Betriebsoptimierung erschweren kann. Prädiktive Regelstrategien, die ggf. noch höhere Einsparpotenziale mit sich bringen würden, sind somit oftmals nur kostspielig umsetzbar. Gleichzeitig ist es sinnvoll, die Anlagenbetreiber*innen bei der Umsetzung der möglichen Betriebsoptimierungsstrategien (z.B. manuelles Einstellen des Volumenstroms oder der Betriebszeiten) zu unterstützen, da sich im Projekt zeigte, dass diesbezüglich z.T. wenig Expertise und vorherige Berührungspunkte existieren. Trotz der materiellen Aufwände und technisch-organisatorischen Hürden, konnten auch bei großen Liegenschaften Stromeinsparungen von durchgängig &gt; 30 % realisiert werden. </t>
   </si>
   <si>
     <t xml:space="preserve">01/2018 – 06/2025
@@ -329,11 +583,14 @@
     <t xml:space="preserve">llec_logo_large_transparent</t>
   </si>
   <si>
-    <t xml:space="preserve">Althaus, Philipp, Florian Redder, Eziama Ubachukwu, Maximilian Mork, André Xhonneux und Dirk Müller (2022): Enhancing Building Monitoring and Control for District Energy Systems: Technology Selection and Installation within the Living Lab Energy Campus. Applied Sciences 12, Nr. 7 (Januar): 3305.
-Mork, Maximilian, Florian Redder, André Xhonneux und Dirk Müller (2023): Real-world implementation and evaluation of a Model Predictive Control framework in an office space. Journal of Building Engineering 78 (1. November): 107619.
-Ubachukwu, Eziama, Jana Pick, Lea Riebesel, Paul Lieberenz, Philipp Althaus, Dirk Müller und André Xhonneux (2023): LLEC Energy Dashboard Suite: User Engagement for Energy-Efficient Behavior Using Dashboards and Gamification. In: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), S. 3241–3252. Veranstaltung: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), Las Palmas De Gran Canaria, Spain. http://www.proceedings.com/069564-0291.html.
-United Nations Environment Programme (2021): 2021 Global Status Report for Buildings and Construction: Towards a Zero-Emission, Efficient and Resilient Buildings and Construction Sector. Nairobi, Kenya: United Nations Environment Programme.
-</t>
+    <t xml:space="preserve">Die Heterogenität von Gebäuden, die beispielsweise durch unterschiedliche Anlagenparks und/oder Nutzungsprofile entsteht, sowie das Verhalten der Nutzenden von Gebäuden stellen komplexe Herausforderungen zur Minimierung des Energieverbrauchs dar. Oftmals fehlen verlässliche Daten und entsprechende digitale Anwendungen, um den Energieverbrauch und die Effizienz von Gebäuden angemessen zu bewerten und zu optimieren. Durch ihren erheblichen Anteil am Gesamtenergieverbrauch (30 %) steht die Verbesserung der Energieeffizienz und Reduzierung von CO2-Emissionen von Gebäuden zunehmend im Fokus derzeitiger Forschung (United Nations Environment Programme 2021).
+Das Living Lab Energy Campus (LLEC) am Forschungszentrum Jülich verfolgt das Ziel, Lösungen für die Energieeffizienz in Gebäuden zu erforschen und der Öffentlichkeit  vorzustellen. Hochgradig vernetzte Demonstratoren zeigen verschiedene Forschungsarbeiten, beispielsweise zu Photovoltaik oder der Energiespeicherung. Außerdem wird in zwei Projekten versucht, durch die Integration innovativer Technologien und Ansätze den Energieverbrauch zu minimieren. Zentraler Schlüssel ist dabei die Erfassung und Analyse von Gebäudedaten. Darauf aufbauend werden modulare Lösungen entworfen, die nach erfolgreicher Testung auch auf andere Gebäude übertragen werden können. Ein Schwerpunkt der Optimierung ist diesbezüglich die Entwicklung intelligenter Regelung zur Steuerung von Energieverbrauchsanlagen in einigen Gebäuden und der Energiedemonstratoren des Campus. Um der hohen Heterogenität der Gebäude bzw. Gebäudeteile zu begegnen, muss dabei eine Vielzahl an Einflussgrößen betrachtet werden. Parallel dazu wird in einem anderen Gebäude das Nutzerverhalten als aktives Mittel zur Verbrauchsminimierung erforscht und genutzt. Das LLEC ermöglicht die Entwicklung und Anwendung solcher Lösungen in einem repräsentativen und realistischen Umfeld, das Validierung von Forschungsergebnissen ermöglicht. Insbesondere im Verwaltungsbau kann die Einwirkung auf die intrinsische Motivation von Personen essentiell sein, da sie sich nachgewiesenermaßen nicht für ihren Einfluss auf Energieverbrauch verantwortlich fühlen, solange sie die Kosten nicht tragen. 
+Ein weiteres Ziel des Projekts ist die Förderung des Wissenstransfers und die Sensibilisierung für das Thema Energieeffizienz in Gebäuden. Das LLEC bietet dazu Schulungen, Workshops und Informationsveranstaltungen für Fachleute, Studierende und die interessierte Öffentlichkeit an, um das Bewusstsein für energieeffizientes Bauen zu stärken und Fachwissen zu verbreiten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Fokus des Projekts liegt insbesondere auf der Energieeffizienzsteigerung von Heizungs-, Kühlungs- und Klimasysteme in Bürogebäuden unter Berücksichtigung der Zufriedenheit der Nutzenden. Zum Einsatz kommt dabei eine Modell-prädikative Regelung (engl. Model Predicitve Control (MPC)), die es ermöglicht, nicht-lineares Systemverhalten vorauszusagen und automatisiert zu steuern. Verschiedene Studien beziffern die Energieeinsparungen zwischen 15 % und 50 % (Mork et al. 2023). Im Projekt berücksichtigt die praktisch umgesetzte MPC den Energieverbrauch für Heizung und Beleuchtung, thermisches Unbehagen, sowie potenzielle Nutzer-Störungen durch hochfrequentes Fahren der Verschattung. Die Steuerung erfolgt unter Rücksichtnahme auf Abstimmungsparameter und Komfortgrenzen. Es ist zu erwähnen, dass für die Nutzung der MPC derzeit eine maßgeschneiderte Modellierung für jedes individuelle Gebäude notwendig ist, aber auch in diesem Projekt an Vereinfachungen gearbeitet wird (z.B. einfach zu erstellende und übertragbare Modelica-Module).  Bezüglich des Einflusses des Wetters wurden unterschiedliche Effekte wie Außentemperaturen / Heizbedarfe, Windstärken und solare Gewinne mit in die Steueralgorithmen einbezogen. 
+Unabhängig von den Ansätzen zur MPC, beschäftigen sich die Forschenden mit der Integration von Softwareanwendungen, die es ermöglichen, Energieverbrauchsdaten einzusehen und den Nutzenden Echtzeitempfehlungen für Verhaltensänderungen zu geben (Ubachukwu et al. 2023). Das „Energy Dashboard“ bietet Mitarbeitenden und Besucher*innen des LLEC u.a. auf Raumlevel einen Überblick über Heiz- und Stromverbrauch in Echtzeit. „JuControl“ geht eine Ebene weiter und ermöglicht es den Nutzenden, ihre persönlichen Präferenzen für das Raumklima abzubilden und in die Steuerung einzugreifen. In die Anwendung ist dabei ein Gamification Ansatz eingebettet, der den Vergleich mit anderen Personen/Teams ermöglicht. Das Feedback an die Nutzenden erfolgt über ein Ampelsystem, das den Energieverbrauch angibt. Die Bewertung der Ampel erfolgt anhand festgelegter Grenzen, gemessen in Kilowattstunden. Außerdem spiegelte die Anwendung einen “Energiestrafwert” wider, der simuliert wie hoch der Energieverbrauch des gesamten LLEC Campus gewesen wäre, wenn alle Personen ein entsprechendes Nutzungsprofil gehabt hätten (Idealwert). In diesem Sinne grenzt sich das Projekt von herkömmlichen Ansätzen zur Bewertung der positiven Umweltwirkungen ab. Während normalerweise die Einsparung in Referenz zum Status-Quo-Verbrauch gesetzt wird, fragt die Referenz am LLEC nach dem Idealzustand, der erreicht werden könnte. Denn je nach Lage, Nutzungsart und persönlichen Erfahrungen der Nutzenden, können die Möglichkeiten zu Energieeinsparungen in Einzelräumen stark variieren. Durch die Definition eines Ideals wird diesen Einflüssen Rechnung getragen. Ergänzt wird das System zur Nutzendeneinbindung durch ein Leaderboard (in der Anwendung „JuPower“), das Teams mit dem niedrigsten Energieverbrauch auszeichnet. Anreize für energieeffizientes Verhalten der Nutzenden wird zudem durch soziale Interaktion und „game rewards“ geschaffen.
+Um die korrekte Messung der Daten zu gewährleisten wurden in allen teilnehmenden Gebäuden Sensoren des Typs EnOcean zur Messung der Luftqualität, der CO2 Konzentration, Temperatur und Feuchtigkeit verbaut. Die Verarbeitung der Daten erfolgte mit M-Bus. Zur automatischen Steuerung von Beleuchtung, Heizung und Sonnenschutz kamen KNX Steuerelemente und BACnet-Systeme zum Einsatz. Über den gesamten Campus des LLEC wurden Untersuchungen zur Integration von über 1800 Geräten in 18 Gebäuden mittels einer Informations- und Kommunikationsplattform durchgeführt (EnOcean: 1676 Sensoren und 108 Aktuatoren, KNX: 48 Sensoren und 36 Aktuatoren) (Althaus et al. 2022). </t>
   </si>
   <si>
     <t xml:space="preserve">FeBOp_Jahresvgl_groß</t>
@@ -346,7 +603,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -382,6 +639,64 @@
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val=""/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -441,7 +756,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -474,7 +789,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -730,13 +1057,16 @@
   </sheetPr>
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R4" activeCellId="0" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="58.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="51.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="44.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="26.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="26.35"/>
@@ -863,119 +1193,125 @@
       <c r="S2" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="T2" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="X3" s="8"/>
+        <v>42</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="X3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -990,7 +1326,9 @@
     <hyperlink ref="I2" r:id="rId3" display="https://www.iosb.fraunhofer.de/de/projekte-produkte/rlt-opt-lueftungsanlagen-klimaanlagen-optimieren/konsortium.html"/>
     <hyperlink ref="J2" r:id="rId4" display="https://effizienzboard.de"/>
     <hyperlink ref="H3" r:id="rId5" display="https://www.fz-juelich.de/de/llec"/>
-    <hyperlink ref="H4" r:id="rId6" display="https://www.klimaschutz-niedersachsen.de/themen/waerme/FeBop.php "/>
+    <hyperlink ref="T3" r:id="rId6" display="http://www.proceedings.com/069564-0291.html"/>
+    <hyperlink ref="H4" r:id="rId7" display="https://www.klimaschutz-niedersachsen.de/themen/waerme/FeBop.php "/>
+    <hyperlink ref="T4" r:id="rId8" display="https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -999,7 +1337,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId7"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -1011,14 +1349,14 @@
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="26.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="24" style="2" width="8.72"/>
   </cols>
   <sheetData>
@@ -1086,10 +1424,10 @@
     </row>
     <row r="2" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>23</v>
@@ -1125,127 +1463,133 @@
         <v>33</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>35</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>37</v>
+        <v>75</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>53</v>
+        <v>80</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="X3" s="8"/>
+        <v>42</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="X3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1260,7 +1604,9 @@
     <hyperlink ref="I2" r:id="rId3" display="https://www.iosb.fraunhofer.de/de/projekte-produkte/rlt-opt-lueftungsanlagen-klimaanlagen-optimieren/konsortium.html"/>
     <hyperlink ref="J2" r:id="rId4" display="https://effizienzboard.de"/>
     <hyperlink ref="H3" r:id="rId5" display="https://www.fz-juelich.de/de/llec"/>
-    <hyperlink ref="H4" r:id="rId6" display="https://www.klimaschutz-niedersachsen.de/themen/waerme/FeBop.php "/>
+    <hyperlink ref="T3" r:id="rId6" display="http://www.proceedings.com/069564-0291.html"/>
+    <hyperlink ref="H4" r:id="rId7" display="https://www.klimaschutz-niedersachsen.de/themen/waerme/FeBop.php "/>
+    <hyperlink ref="T4" r:id="rId8" display="https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1269,6 +1615,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId7"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implemented suggestions from jan and felix
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/16_positive_environmental_impact/Vorlage_Datenmodel_environmentalImpact_08204.xlsx
+++ b/02_work_doc/01_daten/16_positive_environmental_impact/Vorlage_Datenmodel_environmentalImpact_08204.xlsx
@@ -192,37 +192,9 @@
 Die Implementierung des stationären Monitorings erforderte wiederum zusätzliche Hardware und einen höheren Datenaufwand. Dabei gilt grundsätzlich, dass Art und Anzahl der zusätzlich notwendigen Komponenten stark von der Größe und Grundausstattung der Liegenschaft sowie von den dortigen Anlagen abhängt. Mit der Aufnahme detaillierter Betriebszustände sind dann jedoch tiefergehende Analysen möglich, mit denen weitere Einsparpotenziale erst erschlossen werden können. </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Als positive Umweltwirkungen wurden im Projekt vor allem Energie- und CO2-Einsparungen angestrebt. Die Quantifizierung dieser Wirkungen wurde mittels eines Vorher-Nachher-Vergleichs tatsächlicher Energiemengen versucht, der sich auf unterschiedliche Zeiträume erstrecken kann (in Abh. des jeweiligen Monitoringkonzepts – mobil und/oder stationär). Im Allgemeinen wurden Kennwerte zur Anlagenbewertung in Anlehnung an DIN SPEC 15240 und DIN 18599 gebildet. Einsparungen wurden teilweise messtechnisch nachgewiesen und teilweise über Hochrechnungen nach allgemeinen physikalischen Regeln bewertet, wobei um Wettereinflüsse gewichtete Bereinigungen vorgenommen wurden. Darauf aufbauend wurden die CO2-Einsparungen ausgehend von den, vom Bundesamt für Wirtschaft und Ausfuhrkontrolle veröffentlichten, Emissionsfaktoren für Energieaudits berechnet.&lt;sup id=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"ref1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&gt;&lt;a href="#footnote1"&gt;1&lt;/a&gt;&lt;/sup&gt;    &lt;br&gt;&lt;br&gt;
+    <t xml:space="preserve">Als positive Umweltwirkungen wurden im Projekt vor allem Energie- und CO2-Einsparungen angestrebt. Die Quantifizierung dieser Wirkungen wurde mittels eines Vorher-Nachher-Vergleichs tatsächlicher Energiemengen versucht, der sich auf unterschiedliche Zeiträume erstrecken kann (in Abh. des jeweiligen Monitoringkonzepts – mobil und/oder stationär). Im Allgemeinen wurden Kennwerte zur Anlagenbewertung in Anlehnung an DIN SPEC 15240 und DIN 18599 gebildet. Einsparungen wurden teilweise messtechnisch nachgewiesen und teilweise über Hochrechnungen nach allgemeinen physikalischen Regeln bewertet, wobei um Wettereinflüsse gewichtete Bereinigungen vorgenommen wurden. Darauf aufbauend wurden die CO2-Einsparungen ausgehend von den, vom Bundesamt für Wirtschaft und Ausfuhrkontrolle veröffentlichten, Emissionsfaktoren für Energieaudits berechnet.&lt;sup id="ref1"&gt;&lt;a href="#footnote1"&gt;1&lt;/a&gt;&lt;/sup&gt;    &lt;br&gt;&lt;br&gt;
 Die erzielten Ergebnisse der Optimierung nach den Normen DIN EN 15232 und ISO 52120 waren bemerkenswert mit durchschnittlichen Stromeinsparungen von durchgängig &gt; 30 %. Gerade das grundsätzliche Einstellen des Volumenstroms (Soll-Ist Abgleich, Anpassen der Betriebszeiten etc.) stellt dabei eine einfach umzusetzende Maßnahme dar, welche sich bereits unter Einsatz des mobilen Monitorings – also unter minimalen Einsatz von Messtechnik und Ressourcen – durchführen lässt. Bei einigen Anlagen können die somit erzielten Einsparungen auch noch deutlich höher als die mittleren 30 % ausfallen. Denn bereits bei einer Verringerung des Volumenstroms um 20 % halbiert sich die Leistungsaufnahme. So konnte der Volumenstrom für die Belüftung des Kellerbereichs einer Beispielliegenschaft um 39 % gesenkt werden, was eine Reduktion des Strombedarfs um 78 % bewirkte. Jährlich können somit ca. 270 MWh bzw. 198 tCO2eqeingespart werden. Mit der Feinjustierung der Anlagen in Abhängigkeit der Raumbelegung/Raumnutzung lassen sich dann weitere Effizienzpotenziale erschließen. Dafür wird jedoch das stationäre Monitoring notwendig, da längere Zeiträume betrachtet werden müssen. Eine weitere positive Umweltwirkung die mit der Optimierung des Betriebs einhergeht: durch die geringe Nutzung, verschleißen die Anlagen auch weniger. Dadurch kann die Lebensdauer deutlich gesteigert werden. Der Projektverbund geht hier von möglichen Lebensdauersteigerungen von bis zu 10 Jahren aus. Ressourcen werden somit länger genutzt und Emissionen vermieden. Ebenso wird die Fehlererkennung vereinfacht bzw. verfrüht, was dazu führen kann, die Anlagen schneller und effektiver zu warten bzw. instand zu halten.  
 Negative Umweltauswirkungen der digitalen Anwendungen wurden nicht mit in die Bilanz einbezogen. Je nach vorhandener Anlagentechnik und Gebäudeleittechnik fallen die Emissionen, hervorgerufen durch das Monitoring sowie die Datenverarbeitung, in den einzelnen Liegenschaften unterschiedlich hoch aus. Am Beispiel des großen Bürogebäudekomplexes (größte untersuchte Liegenschaft): hier wurden über hundert zusätzliche Sensoren (Lufttemperatur, Bestrahlungsstärke, Luftfeuchte, Präsenzmelder, CO2, Druck) ca. 50 Zähler (Strom, Volumenstrom, Wärmemengen), mehrere Kommunikationssysteme (BUS-Systeme, Router, Repeater, Laptops) und mehrere hundert Meter Kabel (Strom, Luft, LAN) für das stationäre Monitoring zusätzlich installiert. Insgesamt entsteht bei dieser Liegenschaft ein Datenaufwand von 10 GB/Jahr. Bei solchen, vergleichsweise komplexen, Liegenschaften kann es zudem zu weiteren Hürden kommen, die die Effektivität der Maßnahmen verringern können. Hier ist vor allem die Gebäudeleittechnik bzw. deren Zugänglichkeit (geschlossene Schnittstellen, Fehlen der Expert*innenebene) zu nennen, welche die Umsetzbarkeit der Handlungsempfehlungen zur Betriebsoptimierung erschweren kann. Prädiktive Regelstrategien, die ggf. noch höhere Einsparpotenziale mit sich bringen würden, sind somit oftmals nur kostspielig umsetzbar. Gleichzeitig ist es sinnvoll, die Anlagenbetreiber*innen bei der Umsetzung der möglichen Betriebsoptimierungsstrategien (z.B. manuelles Einstellen des Volumenstroms oder der Betriebszeiten) zu unterstützen, da sich im Projekt zeigte, dass diesbezüglich z.T. wenig Expertise und vorherige Berührungspunkte existieren. Trotz der materiellen Aufwände und technisch-organisatorischen Hürden, konnten auch bei großen Liegenschaften Stromeinsparungen von durchgängig &gt; 30 % realisiert werden. </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">RLT-Opt– Lüftungs- und Klimaanlagen ganzheitlich optimieren</t>
@@ -236,25 +208,15 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">&lt;sup id=”sup1”&gt;&lt;a href="#ref1"&gt;1&lt;/a&gt;&lt;/sup&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Basis für Berechnung: Emissionsfaktor Strom (Effizienzmaßnahmen) = 0,732 tCO</t>
+      <t xml:space="preserve">&lt;sup id=”sup1”&gt;&lt;a href="#ref1"&gt;1&lt;/a&gt;&lt;/sup&gt; Basis für Berechnung: Emissionsfaktor Strom (Effizienzmaßnahmen) = 0,732 tCO</t>
     </r>
     <r>
       <rPr>
         <vertAlign val="subscript"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
@@ -263,8 +225,8 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/MWh, aus </t>
@@ -274,8 +236,8 @@
         <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Informationsblatt CO</t>
@@ -286,8 +248,8 @@
         <vertAlign val="subscript"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
@@ -297,8 +259,8 @@
         <i val="true"/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-Faktoren</t>
@@ -307,8 +269,8 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">; Bundesamt für Wirtschaft und Ausfuhrkontrolle, 2021.</t>
@@ -354,109 +316,117 @@
     <t xml:space="preserve">assets/images/llec_logo_large_transparent.png</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Die Heterogenität von Gebäuden, die beispielsweise durch unterschiedliche Anlagenparks und/oder Nutzungsprofile entsteht, sowie das Verhalten der Nutzenden von Gebäuden stellen komplexe Herausforderungen zur Minimierung des Energieverbrauchs dar. Oftmals fehlen verlässliche Daten und entsprechende digitale Anwendungen, um den Energieverbrauch und die Effizienz von Gebäuden angemessen zu bewerten und zu optimieren. Durch ihren erheblichen Anteil am Gesamtenergieverbrauch (30 %) steht die Verbesserung der Energieeffizienz und Reduzierung von CO2-Emissionen von Gebäuden zunehmend im Fokus derzeitiger Forschung &lt;a href="#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">United_Nations_Environment_2021"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(United Nations Environment Programme 2021)&lt;/a&gt;.
+    <t xml:space="preserve">Die Heterogenität von Gebäuden, die beispielsweise durch unterschiedliche Anlagenparks und/oder Nutzungsprofile entsteht, sowie das Verhalten der Nutzenden von Gebäuden stellen komplexe Herausforderungen zur Minimierung des Energieverbrauchs dar. Oftmals fehlen verlässliche Daten und entsprechende digitale Anwendungen, um den Energieverbrauch und die Effizienz von Gebäuden angemessen zu bewerten und zu optimieren. Durch ihren erheblichen Anteil am Gesamtenergieverbrauch (30 %) steht die Verbesserung der Energieeffizienz und Reduzierung von CO2-Emissionen von Gebäuden zunehmend im Fokus derzeitiger Forschung &lt;a href="#United_Nations_Environment_2021"&gt;(United Nations Environment Programme 2021)&lt;/a&gt;.
 &lt;br&gt;&lt;br&gt;
 Das Living Lab Energy Campus (LLEC) am Forschungszentrum Jülich verfolgt das Ziel, Lösungen für die Energieeffizienz in Gebäuden zu erforschen und der Öffentlichkeit  vorzustellen. Hochgradig vernetzte Demonstratoren zeigen verschiedene Forschungsarbeiten, beispielsweise zu Photovoltaik oder der Energiespeicherung. Außerdem wird in zwei Projekten versucht, durch die Integration innovativer Technologien und Ansätze den Energieverbrauch zu minimieren. Zentraler Schlüssel ist dabei die Erfassung und Analyse von Gebäudedaten. Darauf aufbauend werden modulare Lösungen entworfen, die nach erfolgreicher Testung auch auf andere Gebäude übertragen werden können. Ein Schwerpunkt der Optimierung ist diesbezüglich die Entwicklung intelligenter Regelung zur Steuerung von Energieverbrauchsanlagen in einigen Gebäuden und der Energiedemonstratoren des Campus. Um der hohen Heterogenität der Gebäude bzw. Gebäudeteile zu begegnen, muss dabei eine Vielzahl an Einflussgrößen betrachtet werden. Parallel dazu wird in einem anderen Gebäude das Nutzerverhalten als aktives Mittel zur Verbrauchsminimierung erforscht und genutzt. Das LLEC ermöglicht die Entwicklung und Anwendung solcher Lösungen in einem repräsentativen und realistischen Umfeld, das Validierung von Forschungsergebnissen ermöglicht. Insbesondere im Verwaltungsbau kann die Einwirkung auf die intrinsische Motivation von Personen essentiell sein, da sie sich nachgewiesenermaßen nicht für ihren Einfluss auf Energieverbrauch verantwortlich fühlen, solange sie die Kosten nicht tragen. 
 Ein weiteres Ziel des Projekts ist die Förderung des Wissenstransfers und die Sensibilisierung für das Thema Energieeffizienz in Gebäuden. Das LLEC bietet dazu Schulungen, Workshops und Informationsveranstaltungen für Fachleute, Studierende und die interessierte Öffentlichkeit an, um das Bewusstsein für energieeffizientes Bauen zu stärken und Fachwissen zu verbreiten.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Der Fokus des Projekts liegt insbesondere auf der Energieeffizienzsteigerung von Heizungs-, Kühlungs- und Klimasysteme in Bürogebäuden unter Berücksichtigung der Zufriedenheit der Nutzenden. Zum Einsatz kommt dabei eine Modell-prädikative Regelung (engl. Model Predicitve Control (MPC)), die es ermöglicht, nicht-lineares Systemverhalten vorauszusagen und automatisiert zu steuern. Verschiedene Studien beziffern die Energieeinsparungen zwischen 15 % und 50 % &lt;a href=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"#Mork,_Maximilian,_Florian_2023"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(Mork et al. 2023)&lt;/a&gt;. Im Projekt berücksichtigt die praktisch umgesetzte MPC den Energieverbrauch für Heizung und Beleuchtung, thermisches Unbehagen, sowie potenzielle Nutzer-Störungen durch hochfrequentes Fahren der Verschattung. Die Steuerung erfolgt unter Rücksichtnahme auf Abstimmungsparameter und Komfortgrenzen. Es ist zu erwähnen, dass für die Nutzung der MPC derzeit eine maßgeschneiderte Modellierung für jedes individuelle Gebäude notwendig ist, aber auch in diesem Projekt an Vereinfachungen gearbeitet wird (z.B. einfach zu erstellende und übertragbare Modelica-Module).  Bezüglich des Einflusses des Wetters wurden unterschiedliche Effekte wie Außentemperaturen / Heizbedarfe, Windstärken und solare Gewinne mit in die Steueralgorithmen einbezogen. &lt;br&gt;&lt;br&gt; 
-Unabhängig von den Ansätzen zur MPC, beschäftigen sich die Forschenden mit der Integration von Softwareanwendungen, die es ermöglichen, Energieverbrauchsdaten einzusehen und den Nutzenden Echtzeitempfehlungen für Verhaltensänderungen zu geben &lt;a href=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"#Ubachukwu,_Eziama,_Jana_2023"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(Ubachukwu et al. 2023)&lt;/a&gt;. Das „Energy Dashboard“ bietet Mitarbeitenden und Besucher*innen des LLEC u.a. auf Raumlevel einen Überblick über Heiz- und Stromverbrauch in Echtzeit. „JuControl“ geht eine Ebene weiter und ermöglicht es den Nutzenden, ihre persönlichen Präferenzen für das Raumklima abzubilden und in die Steuerung einzugreifen. In die Anwendung ist dabei ein Gamification Ansatz eingebettet, der den Vergleich mit anderen Personen/Teams ermöglicht. Das Feedback an die Nutzenden erfolgt über ein Ampelsystem, das den Energieverbrauch angibt. Die Bewertung der Ampel erfolgt anhand festgelegter Grenzen, gemessen in Kilowattstunden. Außerdem spiegelte die Anwendung einen “Energiestrafwert” wider, der simuliert wie hoch der Energieverbrauch des gesamten LLEC Campus gewesen wäre, wenn alle Personen ein entsprechendes Nutzungsprofil gehabt hätten (Idealwert). In diesem Sinne grenzt sich das Projekt von herkömmlichen Ansätzen zur Bewertung der positiven Umweltwirkungen ab. Während normalerweise die Einsparung in Referenz zum Status-Quo-Verbrauch gesetzt wird, fragt die Referenz am LLEC nach dem Idealzustand, der erreicht werden könnte. Denn je nach Lage, Nutzungsart und persönlichen Erfahrungen der Nutzenden, können die Möglichkeiten zu Energieeinsparungen in Einzelräumen stark variieren. Durch die Definition eines Ideals wird diesen Einflüssen Rechnung getragen. Ergänzt wird das System zur Nutzendeneinbindung durch ein Leaderboard (in der Anwendung „JuPower“), das Teams mit dem niedrigsten Energieverbrauch auszeichnet. Anreize für energieeffizientes Verhalten der Nutzenden wird zudem durch soziale Interaktion und „game rewards“ geschaffen.
-&lt;br&gt;&lt;br&gt;Um die korrekte Messung der Daten zu gewährleisten wurden in allen teilnehmenden Gebäuden Sensoren des Typs EnOcean zur Messung der Luftqualität, der CO2 Konzentration, Temperatur und Feuchtigkeit verbaut. Die Verarbeitung der Daten erfolgte mit M-Bus. Zur automatischen Steuerung von Beleuchtung, Heizung und Sonnenschutz kamen KNX Steuerelemente und BACnet-Systeme zum Einsatz. Über den gesamten Campus des LLEC wurden Untersuchungen zur Integration von über 1800 Geräten in 18 Gebäuden mittels einer Informations- und Kommunikationsplattform durchgeführt (EnOcean: 1676 Sensoren und 108 Aktuatoren, KNX: 48 Sensoren und 36 Aktuatoren) &lt;a href="#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Althaus,_Philipp,_Florian</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_2022"&gt;(Althaus et al. 2022)&lt;/a&gt;. </t>
-    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Fokus des Projekts liegt insbesondere auf der Energieeffizienzsteigerung von Heizungs-, Kühlungs- und Klimasysteme in Bürogebäuden unter Berücksichtigung der Zufriedenheit der Nutzenden. Zum Einsatz kommt dabei eine Modell-prädikative Regelung (engl. Model Predicitve Control (MPC)), die es ermöglicht, nicht-lineares Systemverhalten vorauszusagen und automatisiert zu steuern. Verschiedene Studien beziffern die Energieeinsparungen zwischen 15 % und 50 % &lt;a href="#Mork,_Maximilian,_Florian_2023"&gt;(Mork et al. 2023)&lt;/a&gt;. Im Projekt berücksichtigt die praktisch umgesetzte MPC den Energieverbrauch für Heizung und Beleuchtung, thermisches Unbehagen, sowie potenzielle Nutzer-Störungen durch hochfrequentes Fahren der Verschattung. Die Steuerung erfolgt unter Rücksichtnahme auf Abstimmungsparameter und Komfortgrenzen. Es ist zu erwähnen, dass für die Nutzung der MPC derzeit eine maßgeschneiderte Modellierung für jedes individuelle Gebäude notwendig ist, aber auch in diesem Projekt an Vereinfachungen gearbeitet wird (z.B. einfach zu erstellende und übertragbare Modelica-Module).  Bezüglich des Einflusses des Wetters wurden unterschiedliche Effekte wie Außentemperaturen / Heizbedarfe, Windstärken und solare Gewinne mit in die Steueralgorithmen einbezogen. &lt;br&gt;&lt;br&gt; 
+Unabhängig von den Ansätzen zur MPC, beschäftigen sich die Forschenden mit der Integration von Softwareanwendungen, die es ermöglichen, Energieverbrauchsdaten einzusehen und den Nutzenden Echtzeitempfehlungen für Verhaltensänderungen zu geben &lt;a href="#Ubachukwu,_Eziama,_Jana_2023"&gt;(Ubachukwu et al. 2023)&lt;/a&gt;. Das „Energy Dashboard“ bietet Mitarbeitenden und Besucher*innen des LLEC u.a. auf Raumlevel einen Überblick über Heiz- und Stromverbrauch in Echtzeit. „JuControl“ geht eine Ebene weiter und ermöglicht es den Nutzenden, ihre persönlichen Präferenzen für das Raumklima abzubilden und in die Steuerung einzugreifen. In die Anwendung ist dabei ein Gamification Ansatz eingebettet, der den Vergleich mit anderen Personen/Teams ermöglicht. Das Feedback an die Nutzenden erfolgt über ein Ampelsystem, das den Energieverbrauch angibt. Die Bewertung der Ampel erfolgt anhand festgelegter Grenzen, gemessen in Kilowattstunden. Außerdem spiegelte die Anwendung einen “Energiestrafwert” wider, der simuliert wie hoch der Energieverbrauch des gesamten LLEC Campus gewesen wäre, wenn alle Personen ein entsprechendes Nutzungsprofil gehabt hätten (Idealwert). In diesem Sinne grenzt sich das Projekt von herkömmlichen Ansätzen zur Bewertung der positiven Umweltwirkungen ab. Während normalerweise die Einsparung in Referenz zum Status-Quo-Verbrauch gesetzt wird, fragt die Referenz am LLEC nach dem Idealzustand, der erreicht werden könnte. Denn je nach Lage, Nutzungsart und persönlichen Erfahrungen der Nutzenden, können die Möglichkeiten zu Energieeinsparungen in Einzelräumen stark variieren. Durch die Definition eines Ideals wird diesen Einflüssen Rechnung getragen. Ergänzt wird das System zur Nutzendeneinbindung durch ein Leaderboard (in der Anwendung „JuPower“), das Teams mit dem niedrigsten Energieverbrauch auszeichnet. Anreize für energieeffizientes Verhalten der Nutzenden wird zudem durch soziale Interaktion und „game rewards“ geschaffen.
+&lt;br&gt;&lt;br&gt;Um die korrekte Messung der Daten zu gewährleisten wurden in allen teilnehmenden Gebäuden Sensoren des Typs EnOcean zur Messung der Luftqualität, der CO2 Konzentration, Temperatur und Feuchtigkeit verbaut. Die Verarbeitung der Daten erfolgte mit M-Bus. Zur automatischen Steuerung von Beleuchtung, Heizung und Sonnenschutz kamen KNX Steuerelemente und BACnet-Systeme zum Einsatz. Über den gesamten Campus des LLEC wurden Untersuchungen zur Integration von über 1800 Geräten in 18 Gebäuden mittels einer Informations- und Kommunikationsplattform durchgeführt (EnOcean: 1676 Sensoren und 108 Aktuatoren, KNX: 48 Sensoren und 36 Aktuatoren) &lt;a href="#Althaus,_Philipp,_Florian_2022"&gt;(Althaus et al. 2022)&lt;/a&gt;. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Forschenden schätzen die Energieeinsparungen, die mittels MPC erreicht werden können, über sämtliche getestete Gebäude auf ca. 10 – 15 %. Dazu wurde ein digitaler Zwilling der Gebäude mittels unterschiedlicher Regelstrategien vergleichend betrieben. Den größten Einfluss auf die Energieeinsparungen haben dabei das intelligente Steuern der Raumtemperatur, der automatisierten Fensteröffnung sowie das Anpassen des Sonnenschutzes (Fokus Wärme/Klimatisierung; Auswirkungen auf Strombedarf für Beleuchtung nicht inkludiert).  Der Sonnenschutz ist so ausgelegt, dass ein Maximum an solaren Wärmegewinnen und Tageslicht nutzbar gemacht werden kann, um den Energieverbrauch für Heizung und Beleuchtung zu minimieren. Die messtechnische Überprüfung konnte die Simulationen qualitativ bestätigen. So wurden energieeffizientere Raumtemperaturprofile gemessen. Ein genauer Vergleich des Energieverbrauchs konnte jedoch auf Grund mangelnder Zähler in den einzelnen Räumen / Gebäudeteilen nicht zielführend durchgeführt werden. Quantitativ kann das LLEC die hohe Genauigkeit des white-box MPC-Modells bestätigen. Der Root Mean Square Error (RSME) zwischen gemessener und geschätzter Raumtemperatur lag bei 0,49 °C. Zudem konnte die effiziente Arbeitsweise der Regelung belegt werden. Im Vergleich mit einem konventionellen Regelungsansatz (0,47 kh/d) blieb die thermische Unbehaglichkeit mit einem Wert von 0,53 kh/d weitestgehend stabil. 
+&lt;br&gt;&lt;br&gt;
+Für die Nutzendeneinbindung ist zu erwähnen, dass unterschiedlichen Maßnahmen (Dashboards, JuControl, JuPower) seit 2020 durch mehr als 1300 Mitarbeitende genutzt wurden. Zur Evaluierung der Effektivität der Nutzendeneinbindung wurde basierend auf den historischen Daten vor Implementierung der Maßnahmen ein Regressionsmodell aufgesetzt, was den entstandenen Heizenergiebedarf maßgeblich als Funktion der Außentemperatur beschreibt (Fitgüte: R2 = 0,91). Dieses Modell wurde dann ebenso auf die Periode mit implementierten Maßnahmen zur Nutzendeneinbindung angewandt und mit dem tatsächlichen Energieverbrauch des Gebäudes verglichen. Es konnte gezeigt werden, dass, verglichen mit der Referenzperiode, der Heizbedarf in Abhängigkeit der Außentemperatur weniger stark anstieg und die durchschnittliche Temperatur des Pilotgebäudes durchschnittlich um 1 °C gesenkt werden konnte. Diese Effekte trugen maßgeblich zu der gemessenen Verbrauchsreduktion von 11.1 MWh pro Jahr (- 16,7 %) bei, welche die Verantwortlichen auf Grund der gleichen Systemparameter (Energetischer Zustand des Gebäudes und des Heizsystems) auf die effizientere Nutzung des Heizsystems und ein effizienteres Nutzendenverhalten zurückführen. Bei einem Gaskraftwerk zur Heizwärmebereitstellung (angenommener Emissionsfaktor von 200 g CO2e/kWhprimär; Primärenergiefaktor Erdgas = 1,1) entspricht dies einer Einsparung von ca. 2,44 t CO2e pro Jahr. Für Unterschiede in der Außentemperatur der beiden Perioden wurde dabei korrigiert, andere Einflussgrößen wurden jedoch nicht betrachtet (z.B. Wind, Solare Gewinne). Das Komfortlevel der Menschen wurde dabei nicht negativ beeinflusst. Dabei weisen die Projektverantwortlichen auf das zusätzliche Potential hin, da nur ein Fünftel der Büros in dem Gebäude für die Maßnahmen zur Nutzendeneinbindung aktiviert waren. 
+&lt;br&gt;&lt;br&gt;
+Die negativen Umweltwirkungen der verbauten Komponenten wurden weder für die MPC noch die Nutzendeneinbindung bilanziert. Bei der am LLEC vorzufindenden (Komponenten-)Infrastruktur besteht die Schwierigkeit zur Bewertung der negativen Wirkungen vor allem in der Allokation der Komponenten, da neben den hier beschriebenen digitalen Anwendungen noch viele weitere Prozesse und Anwendungen die gleichen Komponenten nutzen. Daher ist eine genaue Zuordnung zu einzelnen digitalen Anwendungen schwierig. Jedoch mussten für die Einzelraummessungen eine Vielzahl an batteriebetriebenen Komponenten verbaut werden (&gt; 1800 Komponenten auf dem Campus insgesamt). Da all diese Komponenten fortwährend mit den digitalen Anwendungen Daten austauschen bzw. diese auf diese zurückgreifen, fällt ein entsprechend hoher Datenaufwand an. Alleine für die Maßnahmen zur Nutzendeneinbindung wurden in ca. 3 Jahren 364 Mio. Datensätzen erfasst und aufgearbeitet (ca. 74 GB insgesamt bzw. ca. 25 GB/a). Dabei gehen die Forschenden davon aus, dass sich der Datenaufwand bei einer noch praxisnäheren Implementierung um ca. 25% reduzieren lassen könnte. Zum einen, da die Anzahl an Datenpunkten in etwa um diese Größe reduziert werden könnte. Zum anderen, weil nach erfolgreicher Erprobung im Forschungskontext weniger Redundanzen bei den Messstellen und eine geringerer Datengranularität nötig wären.  Für die MPC werden täglich ca. 300 MB an Daten auf einem OpenStack Server verarbeitet. Nur ein Bruchteil entfällt dabei auf die Erfassung der Messdaten aus den Räumen (ca. 5 MB pro Tag; 15 minütige Daten zu Raum-Temperatur, Zustände von Fenster- und Tür-Kontakten und Anzahl an Personen im Raum). Zusammengenommen fragen die Nutzendeneinbindung und die MPC jährlich virtuelle Ressourcen für ca. 124 GB nach, was überschlägig CO2-Emissionen von ca. 339 kg CO2e bedeuten würde (vergleiche Abschätzung der negativen Wirkungen durch die Datenübertragung und -verarbeitung &lt;a href="{% url  'dataProcessing' %}"&gt;hier&lt;/a&gt; ).  
+&lt;br&gt;&lt;br&gt;
+Schließlich sieht das Projekt verschiedene Anknüpfungsmöglichkeiten für künftige Forschungsvorhaben. Da MPC-Modelle zwar hohe Einsparpotenziale versprechen, jedoch gleichzeitig einen hohen Aufwand für individuelle Kalibrierung benötigen, besteht ein hoher Bedarf für die Entwicklung von einfach übertragbaren MPC-Ansätzen für kommerzielle Zwecke. Auf die vereinfachte Übertragung auf andere Gebäude zielt auch die angestrebte Verknüpfung beider Anwendungen des Projekts ab (MPC &amp; Nutzendeneinbindung). So sind noch effizienzsteigernde Anpassungsmöglichkeiten innerhalb der Kostenfunktion des MPC möglich. Da beide Aspekte modular entwickelt wurden, ist eine zukünftige Verschränkung denkbar und sinnvoll um bspw. die Effektivität der MPC unter Einfluss von benutzerdefinierte Komforteinstellungen oder angepassten Handlungsempfehlungen an die Nutzenden zu testen. Zudem nennen die Forschenden den Bedarf für umfassendere Versuche in größeren Gebäuden unter Einbeziehung ganzzahliger Entscheidungsvariablen, sowie der Vorlauftemperaturen von Heizwasservolumenströmen (zentrale Heizungssysteme) als weitere Entwicklungsfelder. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Althaus, Philipp, Florian Redder, Eziama Ubachukwu, Maximilian Mork, André Xhonneux und Dirk Müller (2022): Enhancing Building Monitoring and Control for District Energy Systems: Technology Selection and Installation within the Living Lab Energy Campus. Applied Sciences 12, Nr. 7 (Januar): 3305.;;
+Mork, Maximilian, Florian Redder, André Xhonneux und Dirk Müller (2023): Real-world implementation and evaluation of a Model Predictive Control framework in an office space. Journal of Building Engineering 78 (1. November): 107619.;;
+Ubachukwu, Eziama, Jana Pick, Lea Riebesel, Paul Lieberenz, Philipp Althaus, Dirk Müller und André Xhonneux (2023): LLEC Energy Dashboard Suite: User Engagement for Energy-Efficient Behavior Using Dashboards and Gamification. In: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), S. 3241–3252. Veranstaltung: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), Las Palmas De Gran Canaria, Spain. &lt;a href="http://www.proceedings.com/069564-0291.html"&gt;http://www.proceedings.com/069564-0291.html&lt;/a&gt;.;;
+United Nations Environment Programme (2021): 2021 Global Status Report for Buildings and Construction: Towards a Zero-Emission, Efficient and Resilient Buildings and Construction Sector. Nairobi, Kenya: United Nations Environment Programme.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wohnungsunternehmen betreiben meist unterschiedliche Gebäude mit einer Vielfalt von Technologien für die Heiz- und Warmwasserversorgung. Das Potenzial zur Betriebsoptimierung dieser Heizzentralen in Mehrfamilienhäusern ist enorm. Dies sollte möglichst bedienerfreundlich und idealerweise automatisiert erfolgen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FeBOp-MFH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FeBOp-MFH – Feldanalyse zur Betriebsoptimierung von Mehrfamilienhäusern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03ET1573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/2018 – 07/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institut für Solarenergieforschung Hameln, Klimaschutz- und Energieagentur Niedersachsen GmbH, proKlima – der enercity-Fonds, Corona SOLAR GmbH; acht niedersächsische Kooperationspartner aus der Wohnungswirtschaft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.klimaschutz-niedersachsen.de/themen/waerme/FeBop.php </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betriebsoptimierung, Dashboard/Plattform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verbrauchsminimierung, Steigerung der Materialeffizienz, Effizienzsteigerung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informations- und Wissensvermittlung, Nudging, Austausch von Komponenten/Geräten, Umsetzung Messkonzepte/Monitoring, Automatisierung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geringe Umweltlasen bei gleichzeitig hoher Verbreitungschance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assets/images/FeBOp_year_comparison.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wohnungsunternehmen betreiben meist unterschiedliche Gebäude mit einer Vielfalt von Technologien für die Heiz- und Warmwasserversorgung. Das Potenzial zur Betriebsoptimierung dieser Heizzentralen in Mehrfamilienhäusern ist enorm. Dies sollte möglichst bedienerfreundlich und idealerweise automatisiert erfolgen. 
+Das Forschungsprojekt FeBOp-MFH zielt darauf ab, mit minimalem zusätzlichem Messaufwand, Daten der Heizzentralen mithilfe eines intelligenten Mess- und Analysesystems zu erfassen und zu analysieren. Dadurch sollen automatisierte Effizienzanalysen ermöglicht und der Betrieb jeder Heizzentrale optimiert werden. Der primäre Fokus des Projekts liegt auf der Erzielung von Energie- und CO2-Einsparungen sowie auf der Komfortsteigerung aus Sicht des Anlagenbetreibers (vereinfachte Betriebsführung). Sekundäre Ziele sind Kosteneinsparungen sowie die Verlängerung der Lebensdauer der Heiztechnik. Die erwarteten Energieeinsparungen liegen bei mindestens 10 %.
+Der Anwendungsbereich des Projekts erstreckt sich auf die Wärmeoptimierung im Betrieb von Mehrfamilienhäusern, die von Wohnungsunternehmen betrieben werden. Strategisch setzt das Projekt auf Monitoring, Informations- und Wissensvermittlung sowie Handlungsempfehlungen. Diese Maßnahmen richten sich hauptsächlich an die Anlagenbetreiber und nicht an die Mietenden. Es kommen zum einen die Betriebsoptimierung sowie die dafür notwendige Aufbereitung mittels Dashboards bzw. einer digitalen Plattform zum Einsatz. Hierzu werden Kennwerte wie der Nutzungsgrad unter anderem mit „adaptiven“ Benchmarks verglichen. Diese adaptiven Benchmarks nach VDI 3807-1 beziehen sich nicht nur auf das individuelle Gebäude, sondern sind besonders für das gesamte Gebäudeportfolio von Interesse. Hierbei wird der Mittelwert der besten 25 % der Gebäude mit vergleichbarer Technik und Nutzung als Benchmark verwendet. Wohnungsbauunternehmen können so die Gebäude bzw. Anlagen mit dem Benchmark vergleichen und größte Bedarfe und Potenziale für ihr eigenes Portfolio identifizieren. Diese adaptive Herangehensweise mit praktisch erreichten und somit realistischen Kennwerten ermöglicht eine kontinuierliche Anpassung der Benchmarks je nach Zeitraum und durchgeführten Modernisierungsmaßnahmen. Dadurch entsteht nicht nur eine interne Vergleichbarkeit, sondern auch die mit anderen Unternehmen und Objekten, was zu gezielten Handlungen anregen kann.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In dem Projekt FeBOp-MFH wurden gezielt die Potenziale zur Effizienzsteigerung von Heizzentralen angegangen. Die zentrale Stellschraube lag in der Effizienzanalyse des bestehenden Systems, um darauf basierend Verbesserungsmöglichkeiten zu identifizieren. Frühzeitiges Erkennen eines ineffizienten oder fehlerhaften Betriebs ermöglichte die Identifikation von geringinvestiv nutzbaren Einsparpotenzialen und den einfachen Nachweis erzielter Energie- und CO2-Einsparungen. Neben den Echtzeitdaten der Anlagen, können die Betreiber aus Monats- und Jahresberichten Ansatzpunkte für Optimierungsoptionen ableiten. Dazu werden wichtige Kennzahlen wie die Auslastung, Betriebszeiten, Temperaturverläufe, Verluste und der Nutzungsgrad der Heizzentrale dargestellt. Die im Projekt identifizierten Stellschrauben zum Heben der Effizienzpotenziale umfassten die Anpassung von Betriebszeiten und Temperaturen, das Minimieren von Zirkulationszeiten und – für einen möglichen Kessel/Heizungstausch – Hilfestellungen für eine bedarfsgerechte Dimensionierung der Heizung, was den zukünftigen Materialeinsatz minimiert und Überdimensionierungen vermeidet. In den bisherigen Untersuchungen wurde zudem die zentrale Trinkwarmwassererzeugung als häufig ineffizient identifiziert, was den Einsatz dezentraler Systeme zur Warmwasserbereitung (z.B. Wohnungsstationen) zu einer weiteren relevanten Stellschraube macht (ebenfalls im Falle möglicher Modernisierungsmaßnahmen durch die Wohnungsunternehmen). 
+Um diese Stellschrauben zu identifizieren, werden zusätzliche Messwerte benötigt. Dazu müssen jedoch nur sehr wenige Zähler, sowie Temperatur- und Volumenstromsensoren verbaut und mit einem extra Datenlogger kommunikativ über Funk oder Kabel verbunden werden. Die minütlichen Daten werden dann auf dem Datenlogger zwischengespeichert, verschlüsselt und an einen Server versendet. Dort findet wiederum die eigentliche, automatisierte Messwertaufbereitung und -auswertung statt. Die Anlagenbetreiber*innen können die Daten sodann in Echtzeit oder aggregiert vom Server abrufen.  
+Methodisch erfolgte die Messwertaufbereitung anhand einer Vergleichsbildung durch adaptive Benchmarks. Dadurch wird die Performance der Anlage schnell mit vergleichbaren Objekten bewertbar. Die detaillierte Aufarbeitung der eigentlichen Betriebsparameter der Heizzentrale erfolgt dann entweder individuell in Echtzeit oder in automatisierter Form der Monats- oder Jahresberichte. Die Berichte sind dabei unter anderem für den monatlichen/jährlichen Vergleich der Performance der Heizzentrale ausgelegt. Für einige Optimierungsstellschrauben werden auch automatisierte Handlungsempfehlungen gegeben. So werden die Anlagenbetreiber*innen beispielsweise darauf hingewiesen, wenn mögliche Ruhezeiten der Trinkwarmwasserzirkulation nicht ausgeschöpft werden oder die Betriebstemperaturen zu hoch sind.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das Analysesystem des Projekts ermöglicht die Evaluierung der ermittelten Kennwerte anhand von drei Referenzszenarien (Benchmarks). Im ersten Szenario wird ein fester Referenzwert als Benchmark gesetzt, der beispielsweise für den Heizkessel nach VDI 3807-5 bestimmt werden kann. Im zweiten Szenario erfolgt der Vergleich anhand von Kennwerten aus den Vorjahren (historische Daten). Dies ist allerdings erst dann sinnvoll, wenn Betriebsdaten aus mindestens zwei Jahren vorliegen und zeitliche Trends identifiziert werden sollen. Im letzten Szenario werden Kennwerte mit den entsprechenden Kennwerten aller anderen Anlagen verglichen. Diese Werte müssen alle auf der gleichen Basis berechnet worden sein. Die Benchmark ist erst dann aussagekräftig, wenn eine größere Anzahl von Anlagen über mindestens ein Jahr untersucht wurden. 
+Im Projekt werden folgende vier Kennwerte genutzt, um einen Überblick über relevanten Qualitäten der Wärmezentralen zu geben. Die Effizienz des Wärmeerzeugers ist von zentraler Bedeutung, da diese Komponente die zugeführte Endenergie in nutzbare Wärme wandelt. Die Wärmeerzeuger werden nach den verschiedenen Endenergieträgern Gas, Öl Holz und Strom unterschieden, nicht jedoch nach Baujahr oder Bauart. Die Effizienz der Komponente wird durch den Jahresnutzungsgrad (Jahresarbeitszahl bei Wärmepumpen) charakterisiert. Er ist definiert als Verhältnis der im Jahr zur Nutzung erzeugten Wärme zu der dem Wärmeerzeuger zugefügten Endenergie ohne erneuerbare Energien. Der nächste untersuchte Kennwert ist die Effizienz der zentralen Trinkwarmwasserversorgung. Sie gibt Aufschluss über Zirkulationsverluste und Verluste der Speicherung und Beladeleitung und ist häufig der Nutzungspfad mit der geringsten Effizienz. Die Effizienz wird über den Nutzungsgrad dargestellt und berechnet sich aus der Wärmeenergie, die im verbrauchten Trinkwarmwasser enthalten ist, dividiert durch die dem Trinkwarmwasserbereiter zugeführte Wärmemenge. Auch der Anteil lokaler erneuerbarer Energien wird betrachtet. Dieser Kennwert stellt dar, wie weit das Gebäude und die Wärmezentrale durch autarke erneuerbare Energie betrieben wird. Er wird aus dem Verhältnis der am und um das Gebäude lokal bereitgestellten erneuerbaren Energien zur Summe aller zugeführten Energien berechnet. Zuletzt werden die spezifischen CO2-Emissionen untersucht. Dieser Kennwert gibt an, welche Gesamtmenge an CO2-Emissionen durch den Wärmeverbrauch des Gebäudes erzeugt werden. Die Kennwerte „Wärmeerzeuger“ und „Trinkwarmwasserversorgung“ reflektieren die Effizienz der Anlagenteile, während die Kennwerte „lokal erzeugte erneuerbare Energien“ und „CO2-Emissionen“ die Zukunftsfähigkeit der Anlage beurteilen. 
+Im einem Beispielobjekt des Projektes ist ein Optimierungspotential für die Effizienz des Kesselnutzungsgrades von 8 % zu erkennen, für Trinkwarmwasserversorgung wird ein Optimierungspotential von 9 % berechnet, allerdings liegt der Zielwert auf einem geringeren Niveau. Ein Anzeichen dafür, dass eine zentrale Trinkwarmwasserbereitung im Allgemeinen keine gute Effizienz aufweist, da signifikante Verteilverluste nicht vermieden werden können. Der Deutsche Verein des Gas- und Wasserfaches gibt an, dass die höchsten Effizienzen und Endenergieeinsparungen hygienisch sicher nur durch eine dezentrale Trinkwarmwasserversorgung erreicht werden können. Für den Anteil erneuerbarer Energie liegt der Zielwert dreimal so hoch wie der Messwert, was einem Potential von 300 % entspricht. Auch hier liegt der Zielwert auf einem niedrigen Niveau, da die lokale Nutzung regenerativer Energien im MFH-Bereich (Umweltwärme, Solarenergie) noch nicht stark verbreitet ist. Im Gegensatz zum gegrenzten Nutzungsgrad der zentralen Trinkwarmwasserversorgung wird der Zielwert bzw. das Potential beim Anteil der regenerativen Energien durch entsprechende Modernisierungen immer weiter Richtung 100% bewegen. Der Kennwert für die CO2-Emissionen liegt am Objekt recht nah am Zielwert, was unter Berücksichtigung des geringen Anteils lokal erzeugter regenerativer Energien auf eine Ausführung der Gebäudedämmung nach mindestens aktuellem Stand der Technik hinweist. 
+Für die Gaskessel im Gesamtbestand mit einem Mittelwert aller Anlagen von 80 % Jahresnutzungsgrad und von den besten Anlagen mit 90 % Jahresnutzungsgrad ergibt sich eine Abweichung von 10 %. Dies stellt auch das mittlere Optimierungspotential dar. Für die zentrale Trinkwarmwasserversorgung werden ebenso Einsparpotentiale berechnet. So zeigte sich an einem Beispielgebäude, dass höhere Trinkwarmwassertemperaturen und eine deutlich geringere Auslastung im Sommer zur Senkung des Nutzungsgrades der Heizzentrale um 10 %-Punkte führen können. Damit einher geht ein gesteigerter Endenergiebedarf von mindestens 10 %.
+Diesen, mit wenigen Mitteln erreichten, Einsparungen bzw. den ggf. durch die Erschließung der aufgezeigten Potenziale noch darüber hinaus möglichen Verbesserungen, stehen nur geringe ökologische Wirkungen gegenüber. Den CO2-Fußabdruck für die Komponenten eines Wärmepumpensystems (1 Wassserzähler, 2 Wärmezähler, 8 kabellose Temperatursensoren, 1 Datenlogger, 1 Smart-Meter) schätzt das Projekt mittels der &lt;a href="{% url 'components' %}"&gt;Hilfestellung&lt;/a&gt;  zu den Umweltwirkungen häufig verwendeter Komponenten auf ca. 103,3 kg CO2eq/Jahr. Auch der Datenaufwand ist mit ca. 0,3 GB/Jahr gering. Über die &lt;a href="{% url 'dataProcessing' %}"&gt;Kennwerte&lt;/a&gt;  zu den Umweltlasten der Datenübertragung- und verarbeitung können die CO2-Emissionen auf ca. 0,8 kg CO2eq/Jahr geschätzt werden (Datenübertragung mit VDSL; Serverstandort Deutschland; Use-Case virtuelle Maschine). Bei einem Emissionsfaktor von ca. 0,5 kg CO2eq/kWh&lt;sup&gt;&lt;a href="#sup1"&gt;1&lt;/a&gt;&lt;/sup&gt;  müssten also nur ca. 208 kWh/a Strom eingespart werden, um die Umweltlasten ausgleichen zu können.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup id=”sup1”&gt;&lt;a href="#ref1"&gt;1&lt;/a&gt;&lt;/sup&gt; Vergleiche: &lt;a href='https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf'&gt;https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive impact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name Digitale Anwendung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bild1_RLT-Opt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Im Rahmen des Projekts wurden verschiedene Ansätze verfolgt, um Potenziale zu heben und die Effizienz der raumlufttechnischen Anlagen zu steigern. Eine zentrale Stellschraube war die einfache Regelungsoptimierung nach den Normen DIN EN 15232 und ISO 52120. Hierbei erfolgte eine Gesamtsystembetrachtung, um den Volumenstrom des Ventilators aus Basis eines Soll-Ist-Vergleichs zu minimieren. Bedarfsgerechte Anpassungen der Betriebszeiten und Volumenströme im fortlaufenden Betrieb wurden ebenfalls umgesetzt. Zusätzlich wurden umfangreichere Optimierungsmaßnahmen auf Grundlage von Monitoring-Daten durchgeführt, um beispielsweise gleichzeitiges Heizen und Kühlen zu verhindern.
+Für die technische Umsetzung kamen zwei Varianten des Monitorings zum Einsatz. Ein mobiles Monitoring wurde zur Erfassung und Bewertung des Status-Quo genutzt, während ein stationäres Monitoring mit festverbauten Komponenten zusätzliche Einblicke in den Betrieb und eine kontinuierliche Betriebsoptimierung ermöglichte. Das mobile Monitoring erfordert weniger Komponenten. Der Ressourcen-Energiebedarf der Technik für das mobile Monitoring wird im Projekt als sehr gering eingeschätzt. Er beläuft sich auf wenige zusätzliche Sensoren und Zähler. Nichtsdestotrotz lassen sich bereits mit dem mobilen Monitoring enorme Einspareffekte erzielen, insbesondere in Bezug auf die Funktionalität und Dimensionierung der Anlagen bzw. deren Betriebsparameter. 
+Die Implementierung des stationären Monitorings erforderte wiederum zusätzliche Hardware und einen höheren Datenaufwand. Dabei gilt grundsätzlich, dass Art und Anzahl der zusätzlich notwendigen Komponenten stark von der Größe und Grundausstattung der Liegenschaft sowie von den dortigen Anlagen abhängt. Mit der Aufnahme detaillierter Betriebszustände sind dann jedoch tiefergehende Analysen möglich, mit denen weitere Einsparpotenziale erst erschlossen werden können. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/2018 – 06/2025
+01/2018 – 03/2025 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">llec_logo_large_transparent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Heterogenität von Gebäuden, die beispielsweise durch unterschiedliche Anlagenparks und/oder Nutzungsprofile entsteht, sowie das Verhalten der Nutzenden von Gebäuden stellen komplexe Herausforderungen zur Minimierung des Energieverbrauchs dar. Oftmals fehlen verlässliche Daten und entsprechende digitale Anwendungen, um den Energieverbrauch und die Effizienz von Gebäuden angemessen zu bewerten und zu optimieren. Durch ihren erheblichen Anteil am Gesamtenergieverbrauch (30 %) steht die Verbesserung der Energieeffizienz und Reduzierung von CO2-Emissionen von Gebäuden zunehmend im Fokus derzeitiger Forschung (United Nations Environment Programme 2021).
+Das Living Lab Energy Campus (LLEC) am Forschungszentrum Jülich verfolgt das Ziel, Lösungen für die Energieeffizienz in Gebäuden zu erforschen und der Öffentlichkeit  vorzustellen. Hochgradig vernetzte Demonstratoren zeigen verschiedene Forschungsarbeiten, beispielsweise zu Photovoltaik oder der Energiespeicherung. Außerdem wird in zwei Projekten versucht, durch die Integration innovativer Technologien und Ansätze den Energieverbrauch zu minimieren. Zentraler Schlüssel ist dabei die Erfassung und Analyse von Gebäudedaten. Darauf aufbauend werden modulare Lösungen entworfen, die nach erfolgreicher Testung auch auf andere Gebäude übertragen werden können. Ein Schwerpunkt der Optimierung ist diesbezüglich die Entwicklung intelligenter Regelung zur Steuerung von Energieverbrauchsanlagen in einigen Gebäuden und der Energiedemonstratoren des Campus. Um der hohen Heterogenität der Gebäude bzw. Gebäudeteile zu begegnen, muss dabei eine Vielzahl an Einflussgrößen betrachtet werden. Parallel dazu wird in einem anderen Gebäude das Nutzerverhalten als aktives Mittel zur Verbrauchsminimierung erforscht und genutzt. Das LLEC ermöglicht die Entwicklung und Anwendung solcher Lösungen in einem repräsentativen und realistischen Umfeld, das Validierung von Forschungsergebnissen ermöglicht. Insbesondere im Verwaltungsbau kann die Einwirkung auf die intrinsische Motivation von Personen essentiell sein, da sie sich nachgewiesenermaßen nicht für ihren Einfluss auf Energieverbrauch verantwortlich fühlen, solange sie die Kosten nicht tragen. 
+Ein weiteres Ziel des Projekts ist die Förderung des Wissenstransfers und die Sensibilisierung für das Thema Energieeffizienz in Gebäuden. Das LLEC bietet dazu Schulungen, Workshops und Informationsveranstaltungen für Fachleute, Studierende und die interessierte Öffentlichkeit an, um das Bewusstsein für energieeffizientes Bauen zu stärken und Fachwissen zu verbreiten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Fokus des Projekts liegt insbesondere auf der Energieeffizienzsteigerung von Heizungs-, Kühlungs- und Klimasysteme in Bürogebäuden unter Berücksichtigung der Zufriedenheit der Nutzenden. Zum Einsatz kommt dabei eine Modell-prädikative Regelung (engl. Model Predicitve Control (MPC)), die es ermöglicht, nicht-lineares Systemverhalten vorauszusagen und automatisiert zu steuern. Verschiedene Studien beziffern die Energieeinsparungen zwischen 15 % und 50 % (Mork et al. 2023). Im Projekt berücksichtigt die praktisch umgesetzte MPC den Energieverbrauch für Heizung und Beleuchtung, thermisches Unbehagen, sowie potenzielle Nutzer-Störungen durch hochfrequentes Fahren der Verschattung. Die Steuerung erfolgt unter Rücksichtnahme auf Abstimmungsparameter und Komfortgrenzen. Es ist zu erwähnen, dass für die Nutzung der MPC derzeit eine maßgeschneiderte Modellierung für jedes individuelle Gebäude notwendig ist, aber auch in diesem Projekt an Vereinfachungen gearbeitet wird (z.B. einfach zu erstellende und übertragbare Modelica-Module).  Bezüglich des Einflusses des Wetters wurden unterschiedliche Effekte wie Außentemperaturen / Heizbedarfe, Windstärken und solare Gewinne mit in die Steueralgorithmen einbezogen. 
+Unabhängig von den Ansätzen zur MPC, beschäftigen sich die Forschenden mit der Integration von Softwareanwendungen, die es ermöglichen, Energieverbrauchsdaten einzusehen und den Nutzenden Echtzeitempfehlungen für Verhaltensänderungen zu geben (Ubachukwu et al. 2023). Das „Energy Dashboard“ bietet Mitarbeitenden und Besucher*innen des LLEC u.a. auf Raumlevel einen Überblick über Heiz- und Stromverbrauch in Echtzeit. „JuControl“ geht eine Ebene weiter und ermöglicht es den Nutzenden, ihre persönlichen Präferenzen für das Raumklima abzubilden und in die Steuerung einzugreifen. In die Anwendung ist dabei ein Gamification Ansatz eingebettet, der den Vergleich mit anderen Personen/Teams ermöglicht. Das Feedback an die Nutzenden erfolgt über ein Ampelsystem, das den Energieverbrauch angibt. Die Bewertung der Ampel erfolgt anhand festgelegter Grenzen, gemessen in Kilowattstunden. Außerdem spiegelte die Anwendung einen “Energiestrafwert” wider, der simuliert wie hoch der Energieverbrauch des gesamten LLEC Campus gewesen wäre, wenn alle Personen ein entsprechendes Nutzungsprofil gehabt hätten (Idealwert). In diesem Sinne grenzt sich das Projekt von herkömmlichen Ansätzen zur Bewertung der positiven Umweltwirkungen ab. Während normalerweise die Einsparung in Referenz zum Status-Quo-Verbrauch gesetzt wird, fragt die Referenz am LLEC nach dem Idealzustand, der erreicht werden könnte. Denn je nach Lage, Nutzungsart und persönlichen Erfahrungen der Nutzenden, können die Möglichkeiten zu Energieeinsparungen in Einzelräumen stark variieren. Durch die Definition eines Ideals wird diesen Einflüssen Rechnung getragen. Ergänzt wird das System zur Nutzendeneinbindung durch ein Leaderboard (in der Anwendung „JuPower“), das Teams mit dem niedrigsten Energieverbrauch auszeichnet. Anreize für energieeffizientes Verhalten der Nutzenden wird zudem durch soziale Interaktion und „game rewards“ geschaffen.
+Um die korrekte Messung der Daten zu gewährleisten wurden in allen teilnehmenden Gebäuden Sensoren des Typs EnOcean zur Messung der Luftqualität, der CO2 Konzentration, Temperatur und Feuchtigkeit verbaut. Die Verarbeitung der Daten erfolgte mit M-Bus. Zur automatischen Steuerung von Beleuchtung, Heizung und Sonnenschutz kamen KNX Steuerelemente und BACnet-Systeme zum Einsatz. Über den gesamten Campus des LLEC wurden Untersuchungen zur Integration von über 1800 Geräten in 18 Gebäuden mittels einer Informations- und Kommunikationsplattform durchgeführt (EnOcean: 1676 Sensoren und 108 Aktuatoren, KNX: 48 Sensoren und 36 Aktuatoren) (Althaus et al. 2022). </t>
   </si>
   <si>
     <t xml:space="preserve">Die Forschenden schätzen die Energieeinsparungen, die mittels MPC erreicht werden können, über sämtliche getestete Gebäude auf ca. 10 – 15 %. Dazu wurde ein digitaler Zwilling der Gebäude mittels unterschiedlicher Regelstrategien vergleichend betrieben. Den größten Einfluss auf die Energieeinsparungen haben dabei das intelligente Steuern der Raumtemperatur, der automatisierten Fensteröffnung sowie das Anpassen des Sonnenschutzes (Fokus Wärme/Klimatisierung; Auswirkungen auf Strombedarf für Beleuchtung nicht inkludiert).  Der Sonnenschutz ist so ausgelegt, dass ein Maximum an solaren Wärmegewinnen und Tageslicht nutzbar gemacht werden kann, um den Energieverbrauch für Heizung und Beleuchtung zu minimieren. Die messtechnische Überprüfung konnte die Simulationen qualitativ bestätigen. So wurden energieeffizientere Raumtemperaturprofile gemessen. Ein genauer Vergleich des Energieverbrauchs konnte jedoch auf Grund mangelnder Zähler in den einzelnen Räumen / Gebäudeteilen nicht zielführend durchgeführt werden. Quantitativ kann das LLEC die hohe Genauigkeit des white-box MPC-Modells bestätigen. Der Root Mean Square Error (RSME) zwischen gemessener und geschätzter Raumtemperatur lag bei 0,49 °C. Zudem konnte die effiziente Arbeitsweise der Regelung belegt werden. Im Vergleich mit einem konventionellen Regelungsansatz (0,47 kh/d) blieb die thermische Unbehaglichkeit mit einem Wert von 0,53 kh/d weitestgehend stabil. 
@@ -466,131 +436,6 @@
 Die negativen Umweltwirkungen der verbauten Komponenten wurden weder für die MPC noch die Nutzendeneinbindung bilanziert. Bei der am LLEC vorzufindenden (Komponenten-)Infrastruktur besteht die Schwierigkeit zur Bewertung der negativen Wirkungen vor allem in der Allokation der Komponenten, da neben den hier beschriebenen digitalen Anwendungen noch viele weitere Prozesse und Anwendungen die gleichen Komponenten nutzen. Daher ist eine genaue Zuordnung zu einzelnen digitalen Anwendungen schwierig. Jedoch mussten für die Einzelraummessungen eine Vielzahl an batteriebetriebenen Komponenten verbaut werden (&gt; 1800 Komponenten auf dem Campus insgesamt). Da all diese Komponenten fortwährend mit den digitalen Anwendungen Daten austauschen bzw. diese auf diese zurückgreifen, fällt ein entsprechend hoher Datenaufwand an. Alleine für die Maßnahmen zur Nutzendeneinbindung wurden in ca. 3 Jahren 364 Mio. Datensätzen erfasst und aufgearbeitet (ca. 74 GB insgesamt bzw. ca. 25 GB/a). Dabei gehen die Forschenden davon aus, dass sich der Datenaufwand bei einer noch praxisnäheren Implementierung um ca. 25% reduzieren lassen könnte. Zum einen, da die Anzahl an Datenpunkten in etwa um diese Größe reduziert werden könnte. Zum anderen, weil nach erfolgreicher Erprobung im Forschungskontext weniger Redundanzen bei den Messstellen und eine geringerer Datengranularität nötig wären.  Für die MPC werden täglich ca. 300 MB an Daten auf einem OpenStack Server verarbeitet. Nur ein Bruchteil entfällt dabei auf die Erfassung der Messdaten aus den Räumen (ca. 5 MB pro Tag; 15 minütige Daten zu Raum-Temperatur, Zustände von Fenster- und Tür-Kontakten und Anzahl an Personen im Raum). Zusammengenommen fragen die Nutzendeneinbindung und die MPC jährlich virtuelle Ressourcen für ca. 124 GB nach, was überschlägig CO2-Emissionen von ca. 339 kg CO2e bedeuten würde (vergleiche Abschätzung der negativen Wirkungen durch die Datenübertragung und -verarbeitung &lt;a href=“{% url  'dataProcessing' %}“&gt;hier&lt;/a&gt; ).  
 &lt;br&gt;&lt;br&gt;
 Schließlich sieht das Projekt verschiedene Anknüpfungsmöglichkeiten für künftige Forschungsvorhaben. Da MPC-Modelle zwar hohe Einsparpotenziale versprechen, jedoch gleichzeitig einen hohen Aufwand für individuelle Kalibrierung benötigen, besteht ein hoher Bedarf für die Entwicklung von einfach übertragbaren MPC-Ansätzen für kommerzielle Zwecke. Auf die vereinfachte Übertragung auf andere Gebäude zielt auch die angestrebte Verknüpfung beider Anwendungen des Projekts ab (MPC &amp; Nutzendeneinbindung). So sind noch effizienzsteigernde Anpassungsmöglichkeiten innerhalb der Kostenfunktion des MPC möglich. Da beide Aspekte modular entwickelt wurden, ist eine zukünftige Verschränkung denkbar und sinnvoll um bspw. die Effektivität der MPC unter Einfluss von benutzerdefinierte Komforteinstellungen oder angepassten Handlungsempfehlungen an die Nutzenden zu testen. Zudem nennen die Forschenden den Bedarf für umfassendere Versuche in größeren Gebäuden unter Einbeziehung ganzzahliger Entscheidungsvariablen, sowie der Vorlauftemperaturen von Heizwasservolumenströmen (zentrale Heizungssysteme) als weitere Entwicklungsfelder. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Althaus, Philipp, Florian Redder, Eziama Ubachukwu, Maximilian Mork, André Xhonneux und Dirk Müller (2022): Enhancing Building Monitoring and Control for District Energy Systems: Technology Selection and Installation within the Living Lab Energy Campus. Applied Sciences 12, Nr. 7 (Januar): 3305.;;
-Mork, Maximilian, Florian Redder, André Xhonneux und Dirk Müller (2023): Real-world implementation and evaluation of a Model Predictive Control framework in an office space. Journal of Building Engineering 78 (1. November): 107619.;;
-Ubachukwu, Eziama, Jana Pick, Lea Riebesel, Paul Lieberenz, Philipp Althaus, Dirk Müller und André Xhonneux (2023): LLEC Energy Dashboard Suite: User Engagement for Energy-Efficient Behavior Using Dashboards and Gamification. In: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), S. 3241–3252. Veranstaltung: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), Las Palmas De Gran Canaria, Spain. &lt;a href="http://www.proceedings.com/069564-0291.html"&gt;http://www.proceedings.com/069564-0291.html&lt;/a&gt;.;;
-United Nations Environment Programme (2021): 2021 Global Status Report for Buildings and Construction: Towards a Zero-Emission, Efficient and Resilient Buildings and Construction Sector. Nairobi, Kenya: United Nations Environment Programme.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wohnungsunternehmen betreiben meist unterschiedliche Gebäude mit einer Vielfalt von Technologien für die Heiz- und Warmwasserversorgung. Das Potenzial zur Betriebsoptimierung dieser Heizzentralen in Mehrfamilienhäusern ist enorm. Dies sollte möglichst bedienerfreundlich und idealerweise automatisiert erfolgen. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FeBOp-MFH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FeBOp-MFH – Feldanalyse zur Betriebsoptimierung von Mehrfamilienhäusern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03ET1573</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/2018 – 07/2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Institut für Solarenergieforschung Hameln, Klimaschutz- und Energieagentur Niedersachsen GmbH, proKlima – der enercity-Fonds, Corona SOLAR GmbH; acht niedersächsische Kooperationspartner aus der Wohnungswirtschaft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.klimaschutz-niedersachsen.de/themen/waerme/FeBop.php </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Betriebsoptimierung, Dashboard/Plattform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verbrauchsminimierung, Steigerung der Materialeffizienz, Effizienzsteigerung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Informations- und Wissensvermittlung, Nudging, Austausch von Komponenten/Geräten, Umsetzung Messkonzepte/Monitoring, Automatisierung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geringe Umweltlasen bei gleichzeitig hoher Verbreitungschance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assets/images/FeBOp_year_comparison.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wohnungsunternehmen betreiben meist unterschiedliche Gebäude mit einer Vielfalt von Technologien für die Heiz- und Warmwasserversorgung. Das Potenzial zur Betriebsoptimierung dieser Heizzentralen in Mehrfamilienhäusern ist enorm. Dies sollte möglichst bedienerfreundlich und idealerweise automatisiert erfolgen. 
-Das Forschungsprojekt FeBOp-MFH zielt darauf ab, mit minimalem zusätzlichem Messaufwand, Daten der Heizzentralen mithilfe eines intelligenten Mess- und Analysesystems zu erfassen und zu analysieren. Dadurch sollen automatisierte Effizienzanalysen ermöglicht und der Betrieb jeder Heizzentrale optimiert werden. Der primäre Fokus des Projekts liegt auf der Erzielung von Energie- und CO2-Einsparungen sowie auf der Komfortsteigerung aus Sicht des Anlagenbetreibers (vereinfachte Betriebsführung). Sekundäre Ziele sind Kosteneinsparungen sowie die Verlängerung der Lebensdauer der Heiztechnik. Die erwarteten Energieeinsparungen liegen bei mindestens 10 %.
-Der Anwendungsbereich des Projekts erstreckt sich auf die Wärmeoptimierung im Betrieb von Mehrfamilienhäusern, die von Wohnungsunternehmen betrieben werden. Strategisch setzt das Projekt auf Monitoring, Informations- und Wissensvermittlung sowie Handlungsempfehlungen. Diese Maßnahmen richten sich hauptsächlich an die Anlagenbetreiber und nicht an die Mietenden. Es kommen zum einen die Betriebsoptimierung sowie die dafür notwendige Aufbereitung mittels Dashboards bzw. einer digitalen Plattform zum Einsatz. Hierzu werden Kennwerte wie der Nutzungsgrad unter anderem mit „adaptiven“ Benchmarks verglichen. Diese adaptiven Benchmarks nach VDI 3807-1 beziehen sich nicht nur auf das individuelle Gebäude, sondern sind besonders für das gesamte Gebäudeportfolio von Interesse. Hierbei wird der Mittelwert der besten 25 % der Gebäude mit vergleichbarer Technik und Nutzung als Benchmark verwendet. Wohnungsbauunternehmen können so die Gebäude bzw. Anlagen mit dem Benchmark vergleichen und größte Bedarfe und Potenziale für ihr eigenes Portfolio identifizieren. Diese adaptive Herangehensweise mit praktisch erreichten und somit realistischen Kennwerten ermöglicht eine kontinuierliche Anpassung der Benchmarks je nach Zeitraum und durchgeführten Modernisierungsmaßnahmen. Dadurch entsteht nicht nur eine interne Vergleichbarkeit, sondern auch die mit anderen Unternehmen und Objekten, was zu gezielten Handlungen anregen kann.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In dem Projekt FeBOp-MFH wurden gezielt die Potenziale zur Effizienzsteigerung von Heizzentralen angegangen. Die zentrale Stellschraube lag in der Effizienzanalyse des bestehenden Systems, um darauf basierend Verbesserungsmöglichkeiten zu identifizieren. Frühzeitiges Erkennen eines ineffizienten oder fehlerhaften Betriebs ermöglichte die Identifikation von geringinvestiv nutzbaren Einsparpotenzialen und den einfachen Nachweis erzielter Energie- und CO2-Einsparungen. Neben den Echtzeitdaten der Anlagen, können die Betreiber aus Monats- und Jahresberichten Ansatzpunkte für Optimierungsoptionen ableiten. Dazu werden wichtige Kennzahlen wie die Auslastung, Betriebszeiten, Temperaturverläufe, Verluste und der Nutzungsgrad der Heizzentrale dargestellt. Die im Projekt identifizierten Stellschrauben zum Heben der Effizienzpotenziale umfassten die Anpassung von Betriebszeiten und Temperaturen, das Minimieren von Zirkulationszeiten und – für einen möglichen Kessel/Heizungstausch – Hilfestellungen für eine bedarfsgerechte Dimensionierung der Heizung, was den zukünftigen Materialeinsatz minimiert und Überdimensionierungen vermeidet. In den bisherigen Untersuchungen wurde zudem die zentrale Trinkwarmwassererzeugung als häufig ineffizient identifiziert, was den Einsatz dezentraler Systeme zur Warmwasserbereitung (z.B. Wohnungsstationen) zu einer weiteren relevanten Stellschraube macht (ebenfalls im Falle möglicher Modernisierungsmaßnahmen durch die Wohnungsunternehmen). 
-Um diese Stellschrauben zu identifizieren, werden zusätzliche Messwerte benötigt. Dazu müssen jedoch nur sehr wenige Zähler, sowie Temperatur- und Volumenstromsensoren verbaut und mit einem extra Datenlogger kommunikativ über Funk oder Kabel verbunden werden. Die minütlichen Daten werden dann auf dem Datenlogger zwischengespeichert, verschlüsselt und an einen Server versendet. Dort findet wiederum die eigentliche, automatisierte Messwertaufbereitung und -auswertung statt. Die Anlagenbetreiber*innen können die Daten sodann in Echtzeit oder aggregiert vom Server abrufen.  
-Methodisch erfolgte die Messwertaufbereitung anhand einer Vergleichsbildung durch adaptive Benchmarks. Dadurch wird die Performance der Anlage schnell mit vergleichbaren Objekten bewertbar. Die detaillierte Aufarbeitung der eigentlichen Betriebsparameter der Heizzentrale erfolgt dann entweder individuell in Echtzeit oder in automatisierter Form der Monats- oder Jahresberichte. Die Berichte sind dabei unter anderem für den monatlichen/jährlichen Vergleich der Performance der Heizzentrale ausgelegt. Für einige Optimierungsstellschrauben werden auch automatisierte Handlungsempfehlungen gegeben. So werden die Anlagenbetreiber*innen beispielsweise darauf hingewiesen, wenn mögliche Ruhezeiten der Trinkwarmwasserzirkulation nicht ausgeschöpft werden oder die Betriebstemperaturen zu hoch sind.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Das Analysesystem des Projekts ermöglicht die Evaluierung der ermittelten Kennwerte anhand von drei Referenzszenarien (Benchmarks). Im ersten Szenario wird ein fester Referenzwert als Benchmark gesetzt, der beispielsweise für den Heizkessel nach VDI 3807-5 bestimmt werden kann. Im zweiten Szenario erfolgt der Vergleich anhand von Kennwerten aus den Vorjahren (historische Daten). Dies ist allerdings erst dann sinnvoll, wenn Betriebsdaten aus mindestens zwei Jahren vorliegen und zeitliche Trends identifiziert werden sollen. Im letzten Szenario werden Kennwerte mit den entsprechenden Kennwerten aller anderen Anlagen verglichen. Diese Werte müssen alle auf der gleichen Basis berechnet worden sein. Die Benchmark ist erst dann aussagekräftig, wenn eine größere Anzahl von Anlagen über mindestens ein Jahr untersucht wurden. 
-Im Projekt werden folgende vier Kennwerte genutzt, um einen Überblick über relevanten Qualitäten der Wärmezentralen zu geben. Die Effizienz des Wärmeerzeugers ist von zentraler Bedeutung, da diese Komponente die zugeführte Endenergie in nutzbare Wärme wandelt. Die Wärmeerzeuger werden nach den verschiedenen Endenergieträgern Gas, Öl Holz und Strom unterschieden, nicht jedoch nach Baujahr oder Bauart. Die Effizienz der Komponente wird durch den Jahresnutzungsgrad (Jahresarbeitszahl bei Wärmepumpen) charakterisiert. Er ist definiert als Verhältnis der im Jahr zur Nutzung erzeugten Wärme zu der dem Wärmeerzeuger zugefügten Endenergie ohne erneuerbare Energien. Der nächste untersuchte Kennwert ist die Effizienz der zentralen Trinkwarmwasserversorgung. Sie gibt Aufschluss über Zirkulationsverluste und Verluste der Speicherung und Beladeleitung und ist häufig der Nutzungspfad mit der geringsten Effizienz. Die Effizienz wird über den Nutzungsgrad dargestellt und berechnet sich aus der Wärmeenergie, die im verbrauchten Trinkwarmwasser enthalten ist, dividiert durch die dem Trinkwarmwasserbereiter zugeführte Wärmemenge. Auch der Anteil lokaler erneuerbarer Energien wird betrachtet. Dieser Kennwert stellt dar, wie weit das Gebäude und die Wärmezentrale durch autarke erneuerbare Energie betrieben wird. Er wird aus dem Verhältnis der am und um das Gebäude lokal bereitgestellten erneuerbaren Energien zur Summe aller zugeführten Energien berechnet. Zuletzt werden die spezifischen CO2-Emissionen untersucht. Dieser Kennwert gibt an, welche Gesamtmenge an CO2-Emissionen durch den Wärmeverbrauch des Gebäudes erzeugt werden. Die Kennwerte „Wärmeerzeuger“ und „Trinkwarmwasserversorgung“ reflektieren die Effizienz der Anlagenteile, während die Kennwerte „lokal erzeugte erneuerbare Energien“ und „CO2-Emissionen“ die Zukunftsfähigkeit der Anlage beurteilen. 
-Im einem Beispielobjekt des Projektes ist ein Optimierungspotential für die Effizienz des Kesselnutzungsgrades von 8 % zu erkennen, für Trinkwarmwasserversorgung wird ein Optimierungspotential von 9 % berechnet, allerdings liegt der Zielwert auf einem geringeren Niveau. Ein Anzeichen dafür, dass eine zentrale Trinkwarmwasserbereitung im Allgemeinen keine gute Effizienz aufweist, da signifikante Verteilverluste nicht vermieden werden können. Der Deutsche Verein des Gas- und Wasserfaches gibt an, dass die höchsten Effizienzen und Endenergieeinsparungen hygienisch sicher nur durch eine dezentrale Trinkwarmwasserversorgung erreicht werden können. Für den Anteil erneuerbarer Energie liegt der Zielwert dreimal so hoch wie der Messwert, was einem Potential von 300 % entspricht. Auch hier liegt der Zielwert auf einem niedrigen Niveau, da die lokale Nutzung regenerativer Energien im MFH-Bereich (Umweltwärme, Solarenergie) noch nicht stark verbreitet ist. Im Gegensatz zum gegrenzten Nutzungsgrad der zentralen Trinkwarmwasserversorgung wird der Zielwert bzw. das Potential beim Anteil der regenerativen Energien durch entsprechende Modernisierungen immer weiter Richtung 100% bewegen. Der Kennwert für die CO2-Emissionen liegt am Objekt recht nah am Zielwert, was unter Berücksichtigung des geringen Anteils lokal erzeugter regenerativer Energien auf eine Ausführung der Gebäudedämmung nach mindestens aktuellem Stand der Technik hinweist. 
-Für die Gaskessel im Gesamtbestand mit einem Mittelwert aller Anlagen von 80 % Jahresnutzungsgrad und von den besten Anlagen mit 90 % Jahresnutzungsgrad ergibt sich eine Abweichung von 10 %. Dies stellt auch das mittlere Optimierungspotential dar. Für die zentrale Trinkwarmwasserversorgung werden ebenso Einsparpotentiale berechnet. So zeigte sich an einem Beispielgebäude, dass höhere Trinkwarmwassertemperaturen und eine deutlich geringere Auslastung im Sommer zur Senkung des Nutzungsgrades der Heizzentrale um 10 %-Punkte führen können. Damit einher geht ein gesteigerter Endenergiebedarf von mindestens 10 %.
-Diesen, mit wenigen Mitteln erreichten, Einsparungen bzw. den ggf. durch die Erschließung der aufgezeigten Potenziale noch darüber hinaus möglichen Verbesserungen, stehen nur geringe ökologische Wirkungen gegenüber. Den CO2-Fußabdruck für die Komponenten eines Wärmepumpensystems (1 Wassserzähler, 2 Wärmezähler, 8 kabellose Temperatursensoren, 1 Datenlogger, 1 Smart-Meter) schätzt das Projekt mittels der &lt;a href="{% url 'components' %}"&gt;Hilfestellung&lt;/a&gt;  zu den Umweltwirkungen häufig verwendeter Komponenten auf ca. 103,3 kg CO2eq/Jahr. Auch der Datenaufwand ist mit ca. 0,3 GB/Jahr gering. Über die &lt;a href="{% url 'dataProcessing' %}"&gt;Kennwerte&lt;/a&gt;  zu den Umweltlasten der Datenübertragung- und verarbeitung können die CO2-Emissionen auf ca. 0,8 kg CO2eq/Jahr geschätzt werden (Datenübertragung mit VDSL; Serverstandort Deutschland; Use-Case virtuelle Maschine). Bei einem Emissionsfaktor von ca. 0,5 kg CO2eq/kWh&lt;sup&gt;&lt;a href="#sup1"&gt;1&lt;/a&gt;&lt;/sup&gt;  müssten also nur ca. 208 kWh/a Strom eingespart werden, um die Umweltlasten ausgleichen zu können.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;sup id=”sup1”&gt;&lt;a href="#ref1"&gt;1&lt;/a&gt;&lt;/sup&gt; Vergleiche: &lt;a href='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'&gt;https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf&lt;/a&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Positive impact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name Digitale Anwendung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bild1_RLT-Opt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Im Rahmen des Projekts wurden verschiedene Ansätze verfolgt, um Potenziale zu heben und die Effizienz der raumlufttechnischen Anlagen zu steigern. Eine zentrale Stellschraube war die einfache Regelungsoptimierung nach den Normen DIN EN 15232 und ISO 52120. Hierbei erfolgte eine Gesamtsystembetrachtung, um den Volumenstrom des Ventilators aus Basis eines Soll-Ist-Vergleichs zu minimieren. Bedarfsgerechte Anpassungen der Betriebszeiten und Volumenströme im fortlaufenden Betrieb wurden ebenfalls umgesetzt. Zusätzlich wurden umfangreichere Optimierungsmaßnahmen auf Grundlage von Monitoring-Daten durchgeführt, um beispielsweise gleichzeitiges Heizen und Kühlen zu verhindern.
-Für die technische Umsetzung kamen zwei Varianten des Monitorings zum Einsatz. Ein mobiles Monitoring wurde zur Erfassung und Bewertung des Status-Quo genutzt, während ein stationäres Monitoring mit festverbauten Komponenten zusätzliche Einblicke in den Betrieb und eine kontinuierliche Betriebsoptimierung ermöglichte. Das mobile Monitoring erfordert weniger Komponenten. Der Ressourcen-Energiebedarf der Technik für das mobile Monitoring wird im Projekt als sehr gering eingeschätzt. Er beläuft sich auf wenige zusätzliche Sensoren und Zähler. Nichtsdestotrotz lassen sich bereits mit dem mobilen Monitoring enorme Einspareffekte erzielen, insbesondere in Bezug auf die Funktionalität und Dimensionierung der Anlagen bzw. deren Betriebsparameter. 
-Die Implementierung des stationären Monitorings erforderte wiederum zusätzliche Hardware und einen höheren Datenaufwand. Dabei gilt grundsätzlich, dass Art und Anzahl der zusätzlich notwendigen Komponenten stark von der Größe und Grundausstattung der Liegenschaft sowie von den dortigen Anlagen abhängt. Mit der Aufnahme detaillierter Betriebszustände sind dann jedoch tiefergehende Analysen möglich, mit denen weitere Einsparpotenziale erst erschlossen werden können. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Als positive Umweltwirkungen wurden im Projekt vor allem Energie- und CO2-Einsparungen angestrebt. Die Quantifizierung dieser Wirkungen wurde mittels eines Vorher-Nachher-Vergleichs tatsächlicher Energiemengen versucht, der sich auf unterschiedliche Zeiträume erstrecken kann (in Abh. des jeweiligen Monitoringkonzepts – mobil und/oder stationär). Im Allgemeinen wurden Kennwerte zur Anlagenbewertung in Anlehnung an DIN SPEC 15240 und DIN 18599 gebildet. Einsparungen wurden teilweise messtechnisch nachgewiesen und teilweise über Hochrechnungen nach allgemeinen physikalischen Regeln bewertet, wobei um Wettereinflüsse gewichtete Bereinigungen vorgenommen wurden. Darauf aufbauend wurden die CO2-Einsparungen ausgehend von den, vom Bundesamt für Wirtschaft und Ausfuhrkontrolle veröffentlichten, Emissionsfaktoren für Energieaudits berechnet.&lt;sup id="ref1"&gt;&lt;a href="#footnote1"&gt;1&lt;/a&gt;&lt;/sup&gt;    &lt;br&gt;&lt;br&gt;
-Die erzielten Ergebnisse der Optimierung nach den Normen DIN EN 15232 und ISO 52120 waren bemerkenswert mit durchschnittlichen Stromeinsparungen von durchgängig &gt; 30 %. Gerade das grundsätzliche Einstellen des Volumenstroms (Soll-Ist Abgleich, Anpassen der Betriebszeiten etc.) stellt dabei eine einfach umzusetzende Maßnahme dar, welche sich bereits unter Einsatz des mobilen Monitorings – also unter minimalen Einsatz von Messtechnik und Ressourcen – durchführen lässt. Bei einigen Anlagen können die somit erzielten Einsparungen auch noch deutlich höher als die mittleren 30 % ausfallen. Denn bereits bei einer Verringerung des Volumenstroms um 20 % halbiert sich die Leistungsaufnahme. So konnte der Volumenstrom für die Belüftung des Kellerbereichs einer Beispielliegenschaft um 39 % gesenkt werden, was eine Reduktion des Strombedarfs um 78 % bewirkte. Jährlich können somit ca. 270 MWh bzw. 198 tCO2eqeingespart werden. Mit der Feinjustierung der Anlagen in Abhängigkeit der Raumbelegung/Raumnutzung lassen sich dann weitere Effizienzpotenziale erschließen. Dafür wird jedoch das stationäre Monitoring notwendig, da längere Zeiträume betrachtet werden müssen. Eine weitere positive Umweltwirkung die mit der Optimierung des Betriebs einhergeht: durch die geringe Nutzung, verschleißen die Anlagen auch weniger. Dadurch kann die Lebensdauer deutlich gesteigert werden. Der Projektverbund geht hier von möglichen Lebensdauersteigerungen von bis zu 10 Jahren aus. Ressourcen werden somit länger genutzt und Emissionen vermieden. Ebenso wird die Fehlererkennung vereinfacht bzw. verfrüht, was dazu führen kann, die Anlagen schneller und effektiver zu warten bzw. instand zu halten.  
-Negative Umweltauswirkungen der digitalen Anwendungen wurden nicht mit in die Bilanz einbezogen. Je nach vorhandener Anlagentechnik und Gebäudeleittechnik fallen die Emissionen, hervorgerufen durch das Monitoring sowie die Datenverarbeitung, in den einzelnen Liegenschaften unterschiedlich hoch aus. Am Beispiel des großen Bürogebäudekomplexes (größte untersuchte Liegenschaft): hier wurden über hundert zusätzliche Sensoren (Lufttemperatur, Bestrahlungsstärke, Luftfeuchte, Präsenzmelder, CO2, Druck) ca. 50 Zähler (Strom, Volumenstrom, Wärmemengen), mehrere Kommunikationssysteme (BUS-Systeme, Router, Repeater, Laptops) und mehrere hundert Meter Kabel (Strom, Luft, LAN) für das stationäre Monitoring zusätzlich installiert. Insgesamt entsteht bei dieser Liegenschaft ein Datenaufwand von 10 GB/Jahr. Bei solchen, vergleichsweise komplexen, Liegenschaften kann es zudem zu weiteren Hürden kommen, die die Effektivität der Maßnahmen verringern können. Hier ist vor allem die Gebäudeleittechnik bzw. deren Zugänglichkeit (geschlossene Schnittstellen, Fehlen der Expert*innenebene) zu nennen, welche die Umsetzbarkeit der Handlungsempfehlungen zur Betriebsoptimierung erschweren kann. Prädiktive Regelstrategien, die ggf. noch höhere Einsparpotenziale mit sich bringen würden, sind somit oftmals nur kostspielig umsetzbar. Gleichzeitig ist es sinnvoll, die Anlagenbetreiber*innen bei der Umsetzung der möglichen Betriebsoptimierungsstrategien (z.B. manuelles Einstellen des Volumenstroms oder der Betriebszeiten) zu unterstützen, da sich im Projekt zeigte, dass diesbezüglich z.T. wenig Expertise und vorherige Berührungspunkte existieren. Trotz der materiellen Aufwände und technisch-organisatorischen Hürden, konnten auch bei großen Liegenschaften Stromeinsparungen von durchgängig &gt; 30 % realisiert werden. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">01/2018 – 06/2025
-01/2018 – 03/2025 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">llec_logo_large_transparent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Heterogenität von Gebäuden, die beispielsweise durch unterschiedliche Anlagenparks und/oder Nutzungsprofile entsteht, sowie das Verhalten der Nutzenden von Gebäuden stellen komplexe Herausforderungen zur Minimierung des Energieverbrauchs dar. Oftmals fehlen verlässliche Daten und entsprechende digitale Anwendungen, um den Energieverbrauch und die Effizienz von Gebäuden angemessen zu bewerten und zu optimieren. Durch ihren erheblichen Anteil am Gesamtenergieverbrauch (30 %) steht die Verbesserung der Energieeffizienz und Reduzierung von CO2-Emissionen von Gebäuden zunehmend im Fokus derzeitiger Forschung (United Nations Environment Programme 2021).
-Das Living Lab Energy Campus (LLEC) am Forschungszentrum Jülich verfolgt das Ziel, Lösungen für die Energieeffizienz in Gebäuden zu erforschen und der Öffentlichkeit  vorzustellen. Hochgradig vernetzte Demonstratoren zeigen verschiedene Forschungsarbeiten, beispielsweise zu Photovoltaik oder der Energiespeicherung. Außerdem wird in zwei Projekten versucht, durch die Integration innovativer Technologien und Ansätze den Energieverbrauch zu minimieren. Zentraler Schlüssel ist dabei die Erfassung und Analyse von Gebäudedaten. Darauf aufbauend werden modulare Lösungen entworfen, die nach erfolgreicher Testung auch auf andere Gebäude übertragen werden können. Ein Schwerpunkt der Optimierung ist diesbezüglich die Entwicklung intelligenter Regelung zur Steuerung von Energieverbrauchsanlagen in einigen Gebäuden und der Energiedemonstratoren des Campus. Um der hohen Heterogenität der Gebäude bzw. Gebäudeteile zu begegnen, muss dabei eine Vielzahl an Einflussgrößen betrachtet werden. Parallel dazu wird in einem anderen Gebäude das Nutzerverhalten als aktives Mittel zur Verbrauchsminimierung erforscht und genutzt. Das LLEC ermöglicht die Entwicklung und Anwendung solcher Lösungen in einem repräsentativen und realistischen Umfeld, das Validierung von Forschungsergebnissen ermöglicht. Insbesondere im Verwaltungsbau kann die Einwirkung auf die intrinsische Motivation von Personen essentiell sein, da sie sich nachgewiesenermaßen nicht für ihren Einfluss auf Energieverbrauch verantwortlich fühlen, solange sie die Kosten nicht tragen. 
-Ein weiteres Ziel des Projekts ist die Förderung des Wissenstransfers und die Sensibilisierung für das Thema Energieeffizienz in Gebäuden. Das LLEC bietet dazu Schulungen, Workshops und Informationsveranstaltungen für Fachleute, Studierende und die interessierte Öffentlichkeit an, um das Bewusstsein für energieeffizientes Bauen zu stärken und Fachwissen zu verbreiten.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Der Fokus des Projekts liegt insbesondere auf der Energieeffizienzsteigerung von Heizungs-, Kühlungs- und Klimasysteme in Bürogebäuden unter Berücksichtigung der Zufriedenheit der Nutzenden. Zum Einsatz kommt dabei eine Modell-prädikative Regelung (engl. Model Predicitve Control (MPC)), die es ermöglicht, nicht-lineares Systemverhalten vorauszusagen und automatisiert zu steuern. Verschiedene Studien beziffern die Energieeinsparungen zwischen 15 % und 50 % (Mork et al. 2023). Im Projekt berücksichtigt die praktisch umgesetzte MPC den Energieverbrauch für Heizung und Beleuchtung, thermisches Unbehagen, sowie potenzielle Nutzer-Störungen durch hochfrequentes Fahren der Verschattung. Die Steuerung erfolgt unter Rücksichtnahme auf Abstimmungsparameter und Komfortgrenzen. Es ist zu erwähnen, dass für die Nutzung der MPC derzeit eine maßgeschneiderte Modellierung für jedes individuelle Gebäude notwendig ist, aber auch in diesem Projekt an Vereinfachungen gearbeitet wird (z.B. einfach zu erstellende und übertragbare Modelica-Module).  Bezüglich des Einflusses des Wetters wurden unterschiedliche Effekte wie Außentemperaturen / Heizbedarfe, Windstärken und solare Gewinne mit in die Steueralgorithmen einbezogen. 
-Unabhängig von den Ansätzen zur MPC, beschäftigen sich die Forschenden mit der Integration von Softwareanwendungen, die es ermöglichen, Energieverbrauchsdaten einzusehen und den Nutzenden Echtzeitempfehlungen für Verhaltensänderungen zu geben (Ubachukwu et al. 2023). Das „Energy Dashboard“ bietet Mitarbeitenden und Besucher*innen des LLEC u.a. auf Raumlevel einen Überblick über Heiz- und Stromverbrauch in Echtzeit. „JuControl“ geht eine Ebene weiter und ermöglicht es den Nutzenden, ihre persönlichen Präferenzen für das Raumklima abzubilden und in die Steuerung einzugreifen. In die Anwendung ist dabei ein Gamification Ansatz eingebettet, der den Vergleich mit anderen Personen/Teams ermöglicht. Das Feedback an die Nutzenden erfolgt über ein Ampelsystem, das den Energieverbrauch angibt. Die Bewertung der Ampel erfolgt anhand festgelegter Grenzen, gemessen in Kilowattstunden. Außerdem spiegelte die Anwendung einen “Energiestrafwert” wider, der simuliert wie hoch der Energieverbrauch des gesamten LLEC Campus gewesen wäre, wenn alle Personen ein entsprechendes Nutzungsprofil gehabt hätten (Idealwert). In diesem Sinne grenzt sich das Projekt von herkömmlichen Ansätzen zur Bewertung der positiven Umweltwirkungen ab. Während normalerweise die Einsparung in Referenz zum Status-Quo-Verbrauch gesetzt wird, fragt die Referenz am LLEC nach dem Idealzustand, der erreicht werden könnte. Denn je nach Lage, Nutzungsart und persönlichen Erfahrungen der Nutzenden, können die Möglichkeiten zu Energieeinsparungen in Einzelräumen stark variieren. Durch die Definition eines Ideals wird diesen Einflüssen Rechnung getragen. Ergänzt wird das System zur Nutzendeneinbindung durch ein Leaderboard (in der Anwendung „JuPower“), das Teams mit dem niedrigsten Energieverbrauch auszeichnet. Anreize für energieeffizientes Verhalten der Nutzenden wird zudem durch soziale Interaktion und „game rewards“ geschaffen.
-Um die korrekte Messung der Daten zu gewährleisten wurden in allen teilnehmenden Gebäuden Sensoren des Typs EnOcean zur Messung der Luftqualität, der CO2 Konzentration, Temperatur und Feuchtigkeit verbaut. Die Verarbeitung der Daten erfolgte mit M-Bus. Zur automatischen Steuerung von Beleuchtung, Heizung und Sonnenschutz kamen KNX Steuerelemente und BACnet-Systeme zum Einsatz. Über den gesamten Campus des LLEC wurden Untersuchungen zur Integration von über 1800 Geräten in 18 Gebäuden mittels einer Informations- und Kommunikationsplattform durchgeführt (EnOcean: 1676 Sensoren und 108 Aktuatoren, KNX: 48 Sensoren und 36 Aktuatoren) (Althaus et al. 2022). </t>
   </si>
   <si>
     <t xml:space="preserve">FeBOp_Jahresvgl_groß</t>
@@ -603,7 +448,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -642,12 +487,31 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <vertAlign val="subscript"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -656,47 +520,9 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <vertAlign val="subscript"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF0000FF"/>
-      <name val=""/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -756,7 +582,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -789,7 +615,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -797,12 +623,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1064,9 +886,9 @@
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="58.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="51.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="44.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="58.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="51.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="44.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="26.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="26.35"/>
@@ -1326,9 +1148,9 @@
     <hyperlink ref="I2" r:id="rId3" display="https://www.iosb.fraunhofer.de/de/projekte-produkte/rlt-opt-lueftungsanlagen-klimaanlagen-optimieren/konsortium.html"/>
     <hyperlink ref="J2" r:id="rId4" display="https://effizienzboard.de"/>
     <hyperlink ref="H3" r:id="rId5" display="https://www.fz-juelich.de/de/llec"/>
-    <hyperlink ref="T3" r:id="rId6" display="http://www.proceedings.com/069564-0291.html"/>
+    <hyperlink ref="T3" r:id="rId6" display="Althaus, Philipp, Florian Redder, Eziama Ubachukwu, Maximilian Mork, André Xhonneux und Dirk Müller (2022): Enhancing Building Monitoring and Control for District Energy Systems: Technology Selection and Installation within the Living Lab Energy Campus. Applied Sciences 12, Nr. 7 (Januar): 3305.;;&#10;Mork, Maximilian, Florian Redder, André Xhonneux und Dirk Müller (2023): Real-world implementation and evaluation of a Model Predictive Control framework in an office space. Journal of Building Engineering 78 (1. November): 107619.;;&#10;Ubachukwu, Eziama, Jana Pick, Lea Riebesel, Paul Lieberenz, Philipp Althaus, Dirk Müller und André Xhonneux (2023): LLEC Energy Dashboard Suite: User Engagement for Energy-Efficient Behavior Using Dashboards and Gamification. In: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), S. 3241–3252. Veranstaltung: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), Las Palmas De Gran Canaria, Spain. &lt;a href=&quot;http://www.proceedings.com/069564-0291.html&quot;&gt;http://www.proceedings.com/069564-0291.html&lt;/a&gt;.;;&#10;United Nations Environment Programme (2021): 2021 Global Status Report for Buildings and Construction: Towards a Zero-Emission, Efficient and Resilient Buildings and Construction Sector. Nairobi, Kenya: United Nations Environment Programme."/>
     <hyperlink ref="H4" r:id="rId7" display="https://www.klimaschutz-niedersachsen.de/themen/waerme/FeBop.php "/>
-    <hyperlink ref="T4" r:id="rId8" display="https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf"/>
+    <hyperlink ref="T4" r:id="rId8" display="&lt;sup id=”sup1”&gt;&lt;a href=&quot;#ref1&quot;&gt;1&lt;/a&gt;&lt;/sup&gt; Vergleiche: &lt;a href='https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf'&gt;https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf&lt;/a&gt;"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1471,8 +1293,8 @@
       <c r="Q2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="R2" s="11" t="s">
-        <v>76</v>
+      <c r="R2" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>38</v>
@@ -1495,7 +1317,7 @@
         <v>43</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>45</v>
@@ -1518,16 +1340,16 @@
         <v>50</v>
       </c>
       <c r="O3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="R3" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="S3" s="7" t="s">
         <v>42</v>
@@ -1604,9 +1426,9 @@
     <hyperlink ref="I2" r:id="rId3" display="https://www.iosb.fraunhofer.de/de/projekte-produkte/rlt-opt-lueftungsanlagen-klimaanlagen-optimieren/konsortium.html"/>
     <hyperlink ref="J2" r:id="rId4" display="https://effizienzboard.de"/>
     <hyperlink ref="H3" r:id="rId5" display="https://www.fz-juelich.de/de/llec"/>
-    <hyperlink ref="T3" r:id="rId6" display="http://www.proceedings.com/069564-0291.html"/>
+    <hyperlink ref="T3" r:id="rId6" display="Althaus, Philipp, Florian Redder, Eziama Ubachukwu, Maximilian Mork, André Xhonneux und Dirk Müller (2022): Enhancing Building Monitoring and Control for District Energy Systems: Technology Selection and Installation within the Living Lab Energy Campus. Applied Sciences 12, Nr. 7 (Januar): 3305.;;&#10;Mork, Maximilian, Florian Redder, André Xhonneux und Dirk Müller (2023): Real-world implementation and evaluation of a Model Predictive Control framework in an office space. Journal of Building Engineering 78 (1. November): 107619.;;&#10;Ubachukwu, Eziama, Jana Pick, Lea Riebesel, Paul Lieberenz, Philipp Althaus, Dirk Müller und André Xhonneux (2023): LLEC Energy Dashboard Suite: User Engagement for Energy-Efficient Behavior Using Dashboards and Gamification. In: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), S. 3241–3252. Veranstaltung: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), Las Palmas De Gran Canaria, Spain. &lt;a href=&quot;http://www.proceedings.com/069564-0291.html&quot;&gt;http://www.proceedings.com/069564-0291.html&lt;/a&gt;.;;&#10;United Nations Environment Programme (2021): 2021 Global Status Report for Buildings and Construction: Towards a Zero-Emission, Efficient and Resilient Buildings and Construction Sector. Nairobi, Kenya: United Nations Environment Programme."/>
     <hyperlink ref="H4" r:id="rId7" display="https://www.klimaschutz-niedersachsen.de/themen/waerme/FeBop.php "/>
-    <hyperlink ref="T4" r:id="rId8" display="https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf"/>
+    <hyperlink ref="T4" r:id="rId8" display="&lt;sup id=”sup1”&gt;&lt;a href=&quot;#ref1&quot;&gt;1&lt;/a&gt;&lt;/sup&gt; Vergleiche: &lt;a href='https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf'&gt;https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf&lt;/a&gt;"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
added collapseInfoContainer class to div parent of a-tag with the showMore text
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/16_positive_environmental_impact/Vorlage_Datenmodel_environmentalImpact_08204.xlsx
+++ b/02_work_doc/01_daten/16_positive_environmental_impact/Vorlage_Datenmodel_environmentalImpact_08204.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="83">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -395,7 +395,7 @@
 Diesen, mit wenigen Mitteln erreichten, Einsparungen bzw. den ggf. durch die Erschließung der aufgezeigten Potenziale noch darüber hinaus möglichen Verbesserungen, stehen nur geringe ökologische Wirkungen gegenüber. Den CO2-Fußabdruck für die Komponenten eines Wärmepumpensystems (1 Wassserzähler, 2 Wärmezähler, 8 kabellose Temperatursensoren, 1 Datenlogger, 1 Smart-Meter) schätzt das Projekt mittels der &lt;a href="{% url 'components' %}"&gt;Hilfestellung&lt;/a&gt;  zu den Umweltwirkungen häufig verwendeter Komponenten auf ca. 103,3 kg CO2eq/Jahr. Auch der Datenaufwand ist mit ca. 0,3 GB/Jahr gering. Über die &lt;a href="{% url 'dataProcessing' %}"&gt;Kennwerte&lt;/a&gt;  zu den Umweltlasten der Datenübertragung- und verarbeitung können die CO2-Emissionen auf ca. 0,8 kg CO2eq/Jahr geschätzt werden (Datenübertragung mit VDSL; Serverstandort Deutschland; Use-Case virtuelle Maschine). Bei einem Emissionsfaktor von ca. 0,5 kg CO2eq/kWh&lt;sup&gt;&lt;a href="#sup1"&gt;1&lt;/a&gt;&lt;/sup&gt;  müssten also nur ca. 208 kWh/a Strom eingespart werden, um die Umweltlasten ausgleichen zu können.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;sup id=”sup1”&gt;&lt;a href="#ref1"&gt;1&lt;/a&gt;&lt;/sup&gt; Vergleiche: &lt;a href='https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf'&gt;https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf&lt;/a&gt;</t>
+    <t xml:space="preserve">&lt;sup id=”sup1”&gt;&lt;a href="#ref1"&gt;1&lt;/a&gt;&lt;/sup&gt; Vergleiche: &lt;a href='https://www.umweltbundesamt.de/publikationen/entwicklung-der-spezifischen-treibhausgas-10'&gt;https://www.umweltbundesamt.de/publikationen/entwicklung-der-spezifischen-treibhausgas-10&lt;/a&gt; abgerufen am 07.06.2024</t>
   </si>
   <si>
     <t xml:space="preserve">Positive impact</t>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t xml:space="preserve">FeBOp_Jahresvgl_groß</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;sup id=”sup1”&gt;&lt;a href="#ref1"&gt;1&lt;/a&gt;&lt;/sup&gt; Vergleiche: &lt;a href='https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf'&gt;https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -879,8 +882,8 @@
   </sheetPr>
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R4" activeCellId="0" sqref="R4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U5" activeCellId="0" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1150,7 +1153,6 @@
     <hyperlink ref="H3" r:id="rId5" display="https://www.fz-juelich.de/de/llec"/>
     <hyperlink ref="T3" r:id="rId6" display="Althaus, Philipp, Florian Redder, Eziama Ubachukwu, Maximilian Mork, André Xhonneux und Dirk Müller (2022): Enhancing Building Monitoring and Control for District Energy Systems: Technology Selection and Installation within the Living Lab Energy Campus. Applied Sciences 12, Nr. 7 (Januar): 3305.;;&#10;Mork, Maximilian, Florian Redder, André Xhonneux und Dirk Müller (2023): Real-world implementation and evaluation of a Model Predictive Control framework in an office space. Journal of Building Engineering 78 (1. November): 107619.;;&#10;Ubachukwu, Eziama, Jana Pick, Lea Riebesel, Paul Lieberenz, Philipp Althaus, Dirk Müller und André Xhonneux (2023): LLEC Energy Dashboard Suite: User Engagement for Energy-Efficient Behavior Using Dashboards and Gamification. In: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), S. 3241–3252. Veranstaltung: 36th International Conference on Efficiency, Cost, Optimization, Simulation and Environmental Impact of Energy Systems (ECOS 2023), Las Palmas De Gran Canaria, Spain. &lt;a href=&quot;http://www.proceedings.com/069564-0291.html&quot;&gt;http://www.proceedings.com/069564-0291.html&lt;/a&gt;.;;&#10;United Nations Environment Programme (2021): 2021 Global Status Report for Buildings and Construction: Towards a Zero-Emission, Efficient and Resilient Buildings and Construction Sector. Nairobi, Kenya: United Nations Environment Programme."/>
     <hyperlink ref="H4" r:id="rId7" display="https://www.klimaschutz-niedersachsen.de/themen/waerme/FeBop.php "/>
-    <hyperlink ref="T4" r:id="rId8" display="&lt;sup id=”sup1”&gt;&lt;a href=&quot;#ref1&quot;&gt;1&lt;/a&gt;&lt;/sup&gt; Vergleiche: &lt;a href='https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf'&gt;https://www.umweltbundesamt.de/sites/default/files/medien/11850/publikationen/23_2024_cc_strommix.pdf&lt;/a&gt;"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1159,7 +1161,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId9"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1411,7 +1413,7 @@
         <v>58</v>
       </c>
       <c r="T4" s="10" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>